<commit_message>
cleanup and plotting (still working on mpld3 for bubble plots)
</commit_message>
<xml_diff>
--- a/Flat_Plate_Vibration_Template.xlsx
+++ b/Flat_Plate_Vibration_Template.xlsx
@@ -8,112 +8,113 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mwachter\workspaces\vibraslab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E300EA9-C822-4CF4-86BA-1AC23ABD819E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D3492F-BD9D-4D3B-841E-548169A3D806}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="6480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="6480" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Slab_Properties" sheetId="1" r:id="rId1"/>
-    <sheet name="Sample_Slabs" sheetId="2" r:id="rId2"/>
-    <sheet name="AISC_Design_Guide_11_Criteria" sheetId="3" r:id="rId3"/>
-    <sheet name="SSM_Example" sheetId="4" r:id="rId4"/>
+    <sheet name="AISC_DG_11_Sensitive_Equipment" sheetId="3" r:id="rId2"/>
+    <sheet name="Batch calculations -&gt;" sheetId="5" r:id="rId3"/>
+    <sheet name="Sample_Slabs" sheetId="2" r:id="rId4"/>
+    <sheet name="SSM_Example" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="c_1" localSheetId="0">Slab_Properties!$B$6</definedName>
-    <definedName name="c_1" localSheetId="3">SSM_Example!$B$6</definedName>
+    <definedName name="c_1" localSheetId="4">SSM_Example!$B$6</definedName>
     <definedName name="c_1">#REF!</definedName>
     <definedName name="c_2" localSheetId="0">Slab_Properties!$B$7</definedName>
-    <definedName name="c_2" localSheetId="3">SSM_Example!$B$7</definedName>
+    <definedName name="c_2" localSheetId="4">SSM_Example!$B$7</definedName>
     <definedName name="c_2">#REF!</definedName>
     <definedName name="d" localSheetId="0">Slab_Properties!$B$13</definedName>
-    <definedName name="d" localSheetId="3">SSM_Example!$B$13</definedName>
+    <definedName name="d" localSheetId="4">SSM_Example!$B$13</definedName>
     <definedName name="d">#REF!</definedName>
     <definedName name="E_c" localSheetId="0">Slab_Properties!$B$11</definedName>
-    <definedName name="E_c" localSheetId="3">SSM_Example!$B$11</definedName>
+    <definedName name="E_c" localSheetId="4">SSM_Example!$B$11</definedName>
     <definedName name="E_c">#REF!</definedName>
     <definedName name="f_c" localSheetId="0">Slab_Properties!$B$9</definedName>
-    <definedName name="f_c" localSheetId="3">SSM_Example!$B$9</definedName>
+    <definedName name="f_c" localSheetId="4">SSM_Example!$B$9</definedName>
     <definedName name="f_c">#REF!</definedName>
-    <definedName name="f_n" localSheetId="3">SSM_Example!$B$124</definedName>
+    <definedName name="f_n" localSheetId="4">SSM_Example!$B$124</definedName>
     <definedName name="f_n">Slab_Properties!$B$124</definedName>
     <definedName name="f_r" localSheetId="0">Slab_Properties!$B$18</definedName>
-    <definedName name="f_r" localSheetId="3">SSM_Example!$B$18</definedName>
+    <definedName name="f_r" localSheetId="4">SSM_Example!$B$18</definedName>
     <definedName name="f_r">#REF!</definedName>
     <definedName name="f_y" localSheetId="0">Slab_Properties!$B$10</definedName>
-    <definedName name="f_y" localSheetId="3">SSM_Example!$B$10</definedName>
+    <definedName name="f_y" localSheetId="4">SSM_Example!$B$10</definedName>
     <definedName name="f_y">#REF!</definedName>
     <definedName name="gamma" localSheetId="0">Slab_Properties!$B$123</definedName>
-    <definedName name="gamma" localSheetId="3">SSM_Example!$B$123</definedName>
+    <definedName name="gamma" localSheetId="4">SSM_Example!$B$123</definedName>
     <definedName name="gamma">#REF!</definedName>
     <definedName name="h" localSheetId="0">Slab_Properties!$B$12</definedName>
-    <definedName name="h" localSheetId="3">SSM_Example!$B$12</definedName>
+    <definedName name="h" localSheetId="4">SSM_Example!$B$12</definedName>
     <definedName name="h">#REF!</definedName>
     <definedName name="k_1" localSheetId="0">Slab_Properties!$B$118</definedName>
-    <definedName name="k_1" localSheetId="3">SSM_Example!$B$118</definedName>
+    <definedName name="k_1" localSheetId="4">SSM_Example!$B$118</definedName>
     <definedName name="k_1">#REF!</definedName>
     <definedName name="k_2" localSheetId="0">Slab_Properties!$B$121</definedName>
-    <definedName name="k_2" localSheetId="3">SSM_Example!$B$121</definedName>
+    <definedName name="k_2" localSheetId="4">SSM_Example!$B$121</definedName>
     <definedName name="k_2">#REF!</definedName>
     <definedName name="l_1" localSheetId="0">Slab_Properties!$B$3</definedName>
-    <definedName name="l_1" localSheetId="3">SSM_Example!$B$3</definedName>
+    <definedName name="l_1" localSheetId="4">SSM_Example!$B$3</definedName>
     <definedName name="l_1">#REF!</definedName>
     <definedName name="l_1c" localSheetId="0">Slab_Properties!$B$22</definedName>
-    <definedName name="l_1c" localSheetId="3">SSM_Example!$B$22</definedName>
+    <definedName name="l_1c" localSheetId="4">SSM_Example!$B$22</definedName>
     <definedName name="l_1c">#REF!</definedName>
     <definedName name="l_1m" localSheetId="0">Slab_Properties!$C$22</definedName>
-    <definedName name="l_1m" localSheetId="3">SSM_Example!$C$22</definedName>
+    <definedName name="l_1m" localSheetId="4">SSM_Example!$C$22</definedName>
     <definedName name="l_1m">#REF!</definedName>
     <definedName name="l_2" localSheetId="0">Slab_Properties!$B$4</definedName>
-    <definedName name="l_2" localSheetId="3">SSM_Example!$B$4</definedName>
+    <definedName name="l_2" localSheetId="4">SSM_Example!$B$4</definedName>
     <definedName name="l_2">#REF!</definedName>
     <definedName name="l_2c" localSheetId="0">Slab_Properties!$B$23</definedName>
-    <definedName name="l_2c" localSheetId="3">SSM_Example!$B$23</definedName>
+    <definedName name="l_2c" localSheetId="4">SSM_Example!$B$23</definedName>
     <definedName name="l_2c">#REF!</definedName>
     <definedName name="l_2m" localSheetId="0">Slab_Properties!$C$23</definedName>
-    <definedName name="l_2m" localSheetId="3">SSM_Example!$C$23</definedName>
+    <definedName name="l_2m" localSheetId="4">SSM_Example!$C$23</definedName>
     <definedName name="l_2m">#REF!</definedName>
     <definedName name="lambda_cw" localSheetId="0">Slab_Properties!$B$17</definedName>
-    <definedName name="lambda_cw" localSheetId="3">SSM_Example!$B$17</definedName>
+    <definedName name="lambda_cw" localSheetId="4">SSM_Example!$B$17</definedName>
     <definedName name="lambda_cw">#REF!</definedName>
     <definedName name="lambda_i_sq" localSheetId="0">Slab_Properties!$B$122</definedName>
-    <definedName name="lambda_i_sq" localSheetId="3">SSM_Example!$B$122</definedName>
+    <definedName name="lambda_i_sq" localSheetId="4">SSM_Example!$B$122</definedName>
     <definedName name="lambda_i_sq">#REF!</definedName>
     <definedName name="lambda_w" localSheetId="0">Slab_Properties!$B$17</definedName>
-    <definedName name="lambda_w" localSheetId="3">SSM_Example!$B$17</definedName>
+    <definedName name="lambda_w" localSheetId="4">SSM_Example!$B$17</definedName>
     <definedName name="lambda_w">#REF!</definedName>
     <definedName name="LL" localSheetId="0">Slab_Properties!$B$27</definedName>
-    <definedName name="LL" localSheetId="3">SSM_Example!$B$27</definedName>
+    <definedName name="LL" localSheetId="4">SSM_Example!$B$27</definedName>
     <definedName name="LL">#REF!</definedName>
     <definedName name="LLvib" localSheetId="0">Slab_Properties!$B$28</definedName>
-    <definedName name="LLvib" localSheetId="3">SSM_Example!$B$28</definedName>
+    <definedName name="LLvib" localSheetId="4">SSM_Example!$B$28</definedName>
     <definedName name="LLvib">#REF!</definedName>
     <definedName name="mass" localSheetId="0">Slab_Properties!$B$30</definedName>
-    <definedName name="mass" localSheetId="3">SSM_Example!$B$30</definedName>
+    <definedName name="mass" localSheetId="4">SSM_Example!$B$30</definedName>
     <definedName name="mass">#REF!</definedName>
     <definedName name="n" localSheetId="0">Slab_Properties!$B$16</definedName>
-    <definedName name="n" localSheetId="3">SSM_Example!$B$16</definedName>
+    <definedName name="n" localSheetId="4">SSM_Example!$B$16</definedName>
     <definedName name="n">#REF!</definedName>
     <definedName name="nu" localSheetId="0">Slab_Properties!$B$8</definedName>
-    <definedName name="nu" localSheetId="3">SSM_Example!$B$8</definedName>
+    <definedName name="nu" localSheetId="4">SSM_Example!$B$8</definedName>
     <definedName name="nu">#REF!</definedName>
-    <definedName name="q_u" localSheetId="3">SSM_Example!$B$36</definedName>
+    <definedName name="q_u" localSheetId="4">SSM_Example!$B$36</definedName>
     <definedName name="q_u">Slab_Properties!$B$36</definedName>
-    <definedName name="qu" localSheetId="3">SSM_Example!$B$36</definedName>
+    <definedName name="qu" localSheetId="4">SSM_Example!$B$36</definedName>
     <definedName name="qu">Slab_Properties!$B$36</definedName>
     <definedName name="SDL" localSheetId="0">Slab_Properties!$B$26</definedName>
-    <definedName name="SDL" localSheetId="3">SSM_Example!$B$26</definedName>
+    <definedName name="SDL" localSheetId="4">SSM_Example!$B$26</definedName>
     <definedName name="SDL">#REF!</definedName>
     <definedName name="SW" localSheetId="0">Slab_Properties!$B$29</definedName>
-    <definedName name="SW" localSheetId="3">SSM_Example!$B$29</definedName>
+    <definedName name="SW" localSheetId="4">SSM_Example!$B$29</definedName>
     <definedName name="SW">#REF!</definedName>
     <definedName name="v" localSheetId="0">Slab_Properties!$B$8</definedName>
-    <definedName name="v" localSheetId="3">SSM_Example!$B$8</definedName>
+    <definedName name="v" localSheetId="4">SSM_Example!$B$8</definedName>
     <definedName name="v">#REF!</definedName>
     <definedName name="w_c" localSheetId="0">Slab_Properties!$B$14</definedName>
-    <definedName name="w_c" localSheetId="3">SSM_Example!$B$14</definedName>
+    <definedName name="w_c" localSheetId="4">SSM_Example!$B$14</definedName>
     <definedName name="w_c">#REF!</definedName>
     <definedName name="y_t" localSheetId="0">Slab_Properties!$B$15</definedName>
-    <definedName name="y_t" localSheetId="3">SSM_Example!$B$15</definedName>
+    <definedName name="y_t" localSheetId="4">SSM_Example!$B$15</definedName>
     <definedName name="y_t">#REF!</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -121,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="163">
   <si>
     <t>Slab properties:</t>
   </si>
@@ -601,6 +602,15 @@
   </si>
   <si>
     <t>fL &lt; fn &lt; fU</t>
+  </si>
+  <si>
+    <t>fn = fU</t>
+  </si>
+  <si>
+    <t>fn = fL</t>
+  </si>
+  <si>
+    <t>* does not consider mode scaling</t>
   </si>
 </sst>
 </file>
@@ -1387,8 +1397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:Q128"/>
   <sheetViews>
-    <sheetView topLeftCell="A112" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView topLeftCell="A103" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1415,13 +1425,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
@@ -1432,7 +1442,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -1447,7 +1457,7 @@
       </c>
       <c r="B5" s="4">
         <f>l_1/l_2</f>
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="D5" s="56" t="s">
         <v>8</v>
@@ -1458,7 +1468,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="2">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -1469,7 +1479,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="2">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -1488,7 +1498,7 @@
         <v>13</v>
       </c>
       <c r="B9" s="2">
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
@@ -1511,7 +1521,7 @@
       </c>
       <c r="B11">
         <f>IF(AND(B14&gt;90,B14&lt;=160),B14^1.5*33*SQRT(B9))*1.2</f>
-        <v>4601104.2152944095</v>
+        <v>5144190.8984795641</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
@@ -1525,7 +1535,7 @@
         <v>18</v>
       </c>
       <c r="B12" s="2">
-        <v>9.5</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
@@ -1536,7 +1546,8 @@
         <v>19</v>
       </c>
       <c r="B13" s="2">
-        <v>8.25</v>
+        <f>h-1.25</f>
+        <v>16.75</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
@@ -1559,7 +1570,7 @@
       </c>
       <c r="B15">
         <f>h/2</f>
-        <v>4.75</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
@@ -1571,7 +1582,7 @@
       </c>
       <c r="B16" s="5">
         <f>29000000/E_c</f>
-        <v>6.3028348507303669</v>
+        <v>5.6374268708751352</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="18" customHeight="1">
@@ -1589,7 +1600,7 @@
       </c>
       <c r="B18" s="5">
         <f>4.5*lambda_w*SQRT(f_c)</f>
-        <v>284.60498941515414</v>
+        <v>318.1980515339464</v>
       </c>
       <c r="C18" t="s">
         <v>14</v>
@@ -1620,11 +1631,11 @@
       </c>
       <c r="B22" s="56">
         <f>MIN(0.25*l_1, 0.25*l_2)*2</f>
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C22" s="56">
         <f>l_2-B22</f>
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D22" t="s">
         <v>3</v>
@@ -1639,11 +1650,11 @@
       </c>
       <c r="B23" s="56">
         <f>MIN(0.25*l_1, 0.25*l_2)*2</f>
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C23" s="56">
         <f>l_1-B23</f>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D23" t="s">
         <v>3</v>
@@ -1659,7 +1670,7 @@
         <v>34</v>
       </c>
       <c r="B26" s="2">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C26" t="s">
         <v>35</v>
@@ -1670,7 +1681,7 @@
         <v>36</v>
       </c>
       <c r="B27" s="2">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="C27" t="s">
         <v>35</v>
@@ -1693,7 +1704,7 @@
       </c>
       <c r="B29" s="6">
         <f>(h/12*w_c)</f>
-        <v>118.75</v>
+        <v>225</v>
       </c>
       <c r="C29" t="s">
         <v>35</v>
@@ -1705,7 +1716,7 @@
       </c>
       <c r="B30" s="6">
         <f>(h / 12 * w_c +SDL+LLvib)*l_1*l_2/32.2</f>
-        <v>2325.310559006211</v>
+        <v>8472.5465838509317</v>
       </c>
       <c r="C30" t="s">
         <v>40</v>
@@ -1717,7 +1728,7 @@
       </c>
       <c r="B31" s="6">
         <f>mass * 32.2/1000</f>
-        <v>74.875</v>
+        <v>272.81599999999997</v>
       </c>
       <c r="C31" t="s">
         <v>42</v>
@@ -1800,7 +1811,7 @@
       </c>
       <c r="B36" s="6">
         <f>1.2*(SDL+SW) +1.6*LL</f>
-        <v>270.5</v>
+        <v>398</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>49</v>
@@ -1836,7 +1847,7 @@
       </c>
       <c r="B37" s="6">
         <f>(q_u*l_2*(l_1-c_1 / 12)^2 / 8) / 1000</f>
-        <v>362.93961805555557</v>
+        <v>1660.6771111111111</v>
       </c>
       <c r="C37" t="s">
         <v>53</v>
@@ -1875,7 +1886,7 @@
       </c>
       <c r="B38" s="6">
         <f>(q_u*l_1*(l_2 - c_2 / 12) ^2 / 8) / 1000</f>
-        <v>278.97660590277781</v>
+        <v>1660.6771111111111</v>
       </c>
       <c r="C38" t="s">
         <v>53</v>
@@ -1946,7 +1957,7 @@
       </c>
       <c r="B40" s="6">
         <f>IF($D$3="interior", F37*B37,  IF($D$3="exterior", J37*B37, "ERROR"))</f>
-        <v>127.02886631944445</v>
+        <v>863.55209777777782</v>
       </c>
       <c r="C40" t="s">
         <v>53</v>
@@ -1967,7 +1978,7 @@
       </c>
       <c r="B41" s="6">
         <f>IF($D$3="interior", F38*B37,  IF($D$3="exterior", J38*B37, "ERROR"))</f>
-        <v>235.91075173611114</v>
+        <v>431.77604888888891</v>
       </c>
       <c r="C41" t="s">
         <v>53</v>
@@ -1988,7 +1999,7 @@
       </c>
       <c r="B42" s="6">
         <f>IF($D$3="interior", F39*B37,  IF($D$3="exterior", J39*B37, "ERROR"))</f>
-        <v>235.91075173611114</v>
+        <v>1162.4739777777777</v>
       </c>
       <c r="C42" t="s">
         <v>53</v>
@@ -2009,7 +2020,7 @@
       </c>
       <c r="B43" s="6">
         <f>IF($D$4="interior", F37*B38,  IF($D$4="exterior", J37*B38, "ERROR"))</f>
-        <v>97.641812065972232</v>
+        <v>581.23698888888885</v>
       </c>
       <c r="C43" t="s">
         <v>53</v>
@@ -2030,7 +2041,7 @@
       </c>
       <c r="B44" s="6">
         <f>IF($D$4="interior", F38*B38,  IF($D$4="exterior", J38*B38, "ERROR"))</f>
-        <v>181.33479383680557</v>
+        <v>1079.4401222222223</v>
       </c>
       <c r="C44" t="s">
         <v>53</v>
@@ -2051,7 +2062,7 @@
       </c>
       <c r="B45" s="6">
         <f>IF($D$4="interior", F39*B38,  IF($D$4="exterior", J39*B38, "ERROR"))</f>
-        <v>181.33479383680557</v>
+        <v>1079.4401222222223</v>
       </c>
       <c r="C45" t="s">
         <v>53</v>
@@ -2097,7 +2108,7 @@
       </c>
       <c r="B48" s="7">
         <f>((SW+SDL)*l_2*(l_1-c_1 / 12) ^ 2 / 8) / 1000</f>
-        <v>186.16588541666667</v>
+        <v>938.82499999999993</v>
       </c>
       <c r="C48" t="s">
         <v>53</v>
@@ -2121,7 +2132,7 @@
       </c>
       <c r="B49" s="7">
         <f>((LL)*l_2*(l_1-c_1 / 12) ^ 2 / 8) / 1000</f>
-        <v>87.212847222222223</v>
+        <v>333.80444444444441</v>
       </c>
       <c r="C49" t="s">
         <v>53</v>
@@ -2142,7 +2153,7 @@
       </c>
       <c r="B50" s="7">
         <f>((SW+SDL)*l_1*(l_2-c_2 / 12) ^ 2 / 8) / 1000</f>
-        <v>143.09798177083334</v>
+        <v>938.82499999999993</v>
       </c>
       <c r="C50" t="s">
         <v>53</v>
@@ -2163,7 +2174,7 @@
       </c>
       <c r="B51" s="7">
         <f>((LL)*l_1*(l_2-c_2 / 12) ^ 2 / 8) / 1000</f>
-        <v>67.036892361111128</v>
+        <v>333.80444444444441</v>
       </c>
       <c r="C51" t="s">
         <v>53</v>
@@ -2225,11 +2236,11 @@
       </c>
       <c r="D55" s="7">
         <f>IF($D$3="interior", F37*G37*B48,  IF($D$3="exterior", J37*K37*B48, "ERROR"))</f>
-        <v>39.094835937500001</v>
+        <v>292.91339999999997</v>
       </c>
       <c r="E55" s="7">
         <f>IF($D$3="interior", H37*I37*B48,  IF($D$3="exterior", L37*M37*B48, "ERROR"))</f>
-        <v>26.063223958333332</v>
+        <v>195.2756</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>53</v>
@@ -2247,11 +2258,11 @@
       </c>
       <c r="D56" s="7">
         <f>IF($D$3="interior", F38*G38*B48,  IF($D$3="exterior", J38*K38*B48, "ERROR"))</f>
-        <v>90.755869140625009</v>
+        <v>244.09449999999998</v>
       </c>
       <c r="E56" s="7">
         <f>IF($D$3="interior", H38*I38*B48,  IF($D$3="exterior", L38*M38*B48, "ERROR"))</f>
-        <v>30.251956380208334</v>
+        <v>0</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>53</v>
@@ -2269,11 +2280,11 @@
       </c>
       <c r="D57" s="7">
         <f>IF($D$3="interior", F39*G39*B48,  IF($D$3="exterior", J39*K39*B48, "ERROR"))</f>
-        <v>90.755869140625009</v>
+        <v>492.88312499999989</v>
       </c>
       <c r="E57" s="7">
         <f>IF($D$4="interior", H39*I39*B48,  IF($D$4="exterior", L39*M39*B48, "ERROR"))</f>
-        <v>30.251956380208334</v>
+        <v>152.55906249999998</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>53</v>
@@ -2291,11 +2302,11 @@
       </c>
       <c r="D58" s="7">
         <f>IF($D$3="interior", F37*G37*B49,  IF($D$3="exterior", J37*K37*B49, "ERROR"))</f>
-        <v>18.314697916666667</v>
+        <v>104.14698666666666</v>
       </c>
       <c r="E58" s="7">
         <f>IF($D$3="interior", H37*I37*B49,  IF($D$3="exterior", L37*M37*B49, "ERROR"))</f>
-        <v>12.209798611111109</v>
+        <v>69.431324444444442</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>53</v>
@@ -2313,11 +2324,11 @@
       </c>
       <c r="D59" s="7">
         <f>IF($D$3="interior", F38*G38*B49,  IF($D$3="exterior", J38*K38*B49, "ERROR"))</f>
-        <v>42.516263020833335</v>
+        <v>86.789155555555553</v>
       </c>
       <c r="E59" s="7">
         <f>IF($D$3="interior", H38*I38*B49,  IF($D$3="exterior", L38*M38*B49, "ERROR"))</f>
-        <v>14.172087673611111</v>
+        <v>0</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>53</v>
@@ -2335,11 +2346,11 @@
       </c>
       <c r="D60" s="7">
         <f>IF($D$3="interior", F39*G39*B49,  IF($D$3="exterior", J39*K39*B49, "ERROR"))</f>
-        <v>42.516263020833335</v>
+        <v>175.2473333333333</v>
       </c>
       <c r="E60" s="7">
         <f>IF($D$3="interior", H39*I39*B49,  IF($D$3="exterior", L39*M39*B49, "ERROR"))</f>
-        <v>14.172087673611111</v>
+        <v>58.41577777777777</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>53</v>
@@ -2357,11 +2368,11 @@
       </c>
       <c r="D61" s="7">
         <f>IF($D$4="interior", F37*G37*B50,  IF($D$4="exterior", J37*K37*B50, "ERROR"))</f>
-        <v>30.050576171875001</v>
+        <v>197.15324999999999</v>
       </c>
       <c r="E61" s="7">
         <f>IF($D$4="interior", H37*I37*B50,  IF($D$4="exterior", L37*M37*B50, "ERROR"))</f>
-        <v>20.033717447916665</v>
+        <v>131.43549999999999</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>53</v>
@@ -2379,11 +2390,11 @@
       </c>
       <c r="D62" s="7">
         <f>IF($D$4="interior", F38*G38*B50,  IF($D$4="exterior", J38*K38*B50, "ERROR"))</f>
-        <v>69.760266113281261</v>
+        <v>457.6771875</v>
       </c>
       <c r="E62" s="7">
         <f>IF($D$4="interior", H38*I38*B50,  IF($D$4="exterior", L38*M38*B50, "ERROR"))</f>
-        <v>23.253422037760419</v>
+        <v>152.55906249999998</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>53</v>
@@ -2401,11 +2412,11 @@
       </c>
       <c r="D63" s="7">
         <f>IF($D$4="interior", F39*G39*B50,  IF($D$4="exterior", J39*K39*B50, "ERROR"))</f>
-        <v>69.760266113281261</v>
+        <v>457.6771875</v>
       </c>
       <c r="E63" s="7">
         <f>IF($D$4="interior", H39*I39*B50,  IF($D$4="exterior", L39*M39*B50, "ERROR"))</f>
-        <v>23.253422037760419</v>
+        <v>152.55906249999998</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>53</v>
@@ -2423,11 +2434,11 @@
       </c>
       <c r="D64" s="7">
         <f>IF($D$4="interior", F37*G37*B51,  IF($D$4="exterior", J37*K37*B51, "ERROR"))</f>
-        <v>14.077747395833336</v>
+        <v>70.098933333333321</v>
       </c>
       <c r="E64" s="7">
         <f>IF($D$4="interior", H37*I37*B51,  IF($D$4="exterior", L37*M37*B51, "ERROR"))</f>
-        <v>9.3851649305555576</v>
+        <v>46.732622222222211</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>53</v>
@@ -2445,11 +2456,11 @@
       </c>
       <c r="D65" s="7">
         <f>IF($D$4="interior", F38*G38*B51,  IF($D$4="exterior", J38*K38*B51, "ERROR"))</f>
-        <v>32.68048502604168</v>
+        <v>162.72966666666667</v>
       </c>
       <c r="E65" s="7">
         <f>IF($D$4="interior", H38*I38*B51,  IF($D$4="exterior", L38*M38*B51, "ERROR"))</f>
-        <v>10.893495008680558</v>
+        <v>54.243222222222222</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>53</v>
@@ -2467,11 +2478,11 @@
       </c>
       <c r="D66" s="7">
         <f>IF($D$4="interior", F39*G39*B51,  IF($D$4="exterior", J39*K39*B51, "ERROR"))</f>
-        <v>32.68048502604168</v>
+        <v>162.72966666666667</v>
       </c>
       <c r="E66" s="7">
         <f>IF($D$4="interior", H39*I39*B51,  IF($D$4="exterior", L39*M39*B51, "ERROR"))</f>
-        <v>10.893495008680558</v>
+        <v>54.243222222222222</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>53</v>
@@ -2505,11 +2516,11 @@
       </c>
       <c r="C71" s="7">
         <f t="shared" ref="C71:D73" si="0">1.2*D55+1.6*D58</f>
-        <v>76.217319791666668</v>
+        <v>518.13125866666655</v>
       </c>
       <c r="D71" s="7">
         <f t="shared" si="0"/>
-        <v>50.811546527777779</v>
+        <v>345.42083911111109</v>
       </c>
       <c r="E71" t="s">
         <v>53</v>
@@ -2524,11 +2535,11 @@
       </c>
       <c r="C72" s="7">
         <f t="shared" si="0"/>
-        <v>176.93306380208332</v>
+        <v>431.77604888888885</v>
       </c>
       <c r="D72" s="7">
         <f t="shared" si="0"/>
-        <v>58.977687934027777</v>
+        <v>0</v>
       </c>
       <c r="E72" t="s">
         <v>53</v>
@@ -2543,11 +2554,11 @@
       </c>
       <c r="C73" s="7">
         <f t="shared" si="0"/>
-        <v>176.93306380208332</v>
+        <v>871.85548333333315</v>
       </c>
       <c r="D73" s="7">
         <f t="shared" si="0"/>
-        <v>58.977687934027777</v>
+        <v>276.53611944444441</v>
       </c>
       <c r="E73" t="s">
         <v>53</v>
@@ -2562,11 +2573,11 @@
       </c>
       <c r="C74" s="7">
         <f t="shared" ref="C74:D76" si="1">1.2*D61+1.6*D64</f>
-        <v>58.585087239583345</v>
+        <v>348.74219333333326</v>
       </c>
       <c r="D74" s="7">
         <f t="shared" si="1"/>
-        <v>39.056724826388887</v>
+        <v>232.49479555555553</v>
       </c>
       <c r="E74" t="s">
         <v>53</v>
@@ -2581,11 +2592,11 @@
       </c>
       <c r="C75" s="7">
         <f t="shared" si="1"/>
-        <v>136.0010953776042</v>
+        <v>809.5800916666667</v>
       </c>
       <c r="D75" s="7">
         <f t="shared" si="1"/>
-        <v>45.333698459201401</v>
+        <v>269.86003055555557</v>
       </c>
       <c r="E75" t="s">
         <v>53</v>
@@ -2600,11 +2611,11 @@
       </c>
       <c r="C76" s="7">
         <f t="shared" si="1"/>
-        <v>136.0010953776042</v>
+        <v>809.5800916666667</v>
       </c>
       <c r="D76" s="7">
         <f t="shared" si="1"/>
-        <v>45.333698459201401</v>
+        <v>269.86003055555557</v>
       </c>
       <c r="E76" t="s">
         <v>53</v>
@@ -2662,11 +2673,11 @@
       </c>
       <c r="C80" s="10">
         <f t="shared" ref="C80:D85" si="2">IF(ISBLANK(K80),H80,K80)</f>
-        <v>2.4750000000000005</v>
+        <v>8.5425000000000004</v>
       </c>
       <c r="D80" s="10">
         <f t="shared" si="2"/>
-        <v>2.4750000000000005</v>
+        <v>8.5425000000000004</v>
       </c>
       <c r="E80" t="s">
         <v>83</v>
@@ -2679,11 +2690,11 @@
       </c>
       <c r="H80" s="10">
         <f>MAX(C71*12000/d*0.85/54000, 0.0025*l_1c*12*d)</f>
-        <v>2.4750000000000005</v>
+        <v>8.5425000000000004</v>
       </c>
       <c r="I80" s="10">
         <f>MAX(D71*12000/d*0.85/54000, 0.0025*l_1m*12*d)</f>
-        <v>2.4750000000000005</v>
+        <v>8.5425000000000004</v>
       </c>
       <c r="J80" t="s">
         <v>83</v>
@@ -2700,11 +2711,11 @@
       </c>
       <c r="C81" s="10">
         <f t="shared" si="2"/>
-        <v>4.0509927065796854</v>
+        <v>8.5425000000000004</v>
       </c>
       <c r="D81" s="10">
         <f t="shared" si="2"/>
-        <v>2.4750000000000005</v>
+        <v>8.5425000000000004</v>
       </c>
       <c r="E81" t="s">
         <v>83</v>
@@ -2717,11 +2728,11 @@
       </c>
       <c r="H81" s="10">
         <f>MAX(C72*12000/d*0.85/54000, 0.0025*l_1c*12*d)</f>
-        <v>4.0509927065796854</v>
+        <v>8.5425000000000004</v>
       </c>
       <c r="I81" s="10">
         <f>MAX(D72*12000/d*0.85/54000, 0.0025*l_1m*12*d)</f>
-        <v>2.4750000000000005</v>
+        <v>8.5425000000000004</v>
       </c>
       <c r="J81" t="s">
         <v>83</v>
@@ -2738,11 +2749,11 @@
       </c>
       <c r="C82" s="10">
         <f t="shared" si="2"/>
-        <v>4.0509927065796854</v>
+        <v>9.8318694637921453</v>
       </c>
       <c r="D82" s="10">
         <f t="shared" si="2"/>
-        <v>2.4750000000000005</v>
+        <v>8.5425000000000004</v>
       </c>
       <c r="E82" t="s">
         <v>83</v>
@@ -2755,11 +2766,11 @@
       </c>
       <c r="H82" s="10">
         <f>MAX(C73*12000/d*0.85/54000, 0.0025*l_1c*12*d)</f>
-        <v>4.0509927065796854</v>
+        <v>9.8318694637921453</v>
       </c>
       <c r="I82" s="10">
         <f>MAX(D73*12000/d*0.85/54000, 0.0025*l_1m*12*d)</f>
-        <v>2.4750000000000005</v>
+        <v>8.5425000000000004</v>
       </c>
       <c r="J82" t="s">
         <v>83</v>
@@ -2776,11 +2787,11 @@
       </c>
       <c r="C83" s="10">
         <f t="shared" si="2"/>
-        <v>2.4750000000000005</v>
+        <v>8.5425000000000004</v>
       </c>
       <c r="D83" s="10">
         <f t="shared" si="2"/>
-        <v>3.7124999999999995</v>
+        <v>8.5425000000000004</v>
       </c>
       <c r="E83" t="s">
         <v>83</v>
@@ -2793,11 +2804,11 @@
       </c>
       <c r="H83" s="10">
         <f>MAX(C74*12000/d*0.85/54000, 0.0025*l_2c*12*d)</f>
-        <v>2.4750000000000005</v>
+        <v>8.5425000000000004</v>
       </c>
       <c r="I83" s="10">
         <f>MAX(D74*12000/d*0.85/54000, 0.0025*l_2m*12*d)</f>
-        <v>3.7124999999999995</v>
+        <v>8.5425000000000004</v>
       </c>
       <c r="J83" t="s">
         <v>83</v>
@@ -2814,11 +2825,11 @@
       </c>
       <c r="C84" s="10">
         <f t="shared" si="2"/>
-        <v>3.1138297931572678</v>
+        <v>9.1295930735212831</v>
       </c>
       <c r="D84" s="10">
         <f t="shared" si="2"/>
-        <v>3.7124999999999995</v>
+        <v>8.5425000000000004</v>
       </c>
       <c r="E84" t="s">
         <v>83</v>
@@ -2831,11 +2842,11 @@
       </c>
       <c r="H84" s="10">
         <f>MAX(C75*12000/d*0.85/54000, 0.0025*l_2c*12*d)</f>
-        <v>3.1138297931572678</v>
+        <v>9.1295930735212831</v>
       </c>
       <c r="I84" s="10">
         <f>MAX(D75*12000/d*0.85/54000, 0.0025*l_2m*12*d)</f>
-        <v>3.7124999999999995</v>
+        <v>8.5425000000000004</v>
       </c>
       <c r="J84" t="s">
         <v>83</v>
@@ -2852,11 +2863,11 @@
       </c>
       <c r="C85" s="10">
         <f t="shared" si="2"/>
-        <v>3.1138297931572678</v>
+        <v>9.1295930735212831</v>
       </c>
       <c r="D85" s="10">
         <f t="shared" si="2"/>
-        <v>3.7124999999999995</v>
+        <v>8.5425000000000004</v>
       </c>
       <c r="E85" t="s">
         <v>83</v>
@@ -2869,11 +2880,11 @@
       </c>
       <c r="H85" s="10">
         <f>MAX(C76*12000/d*0.85/54000, 0.0025*l_2c*12*d)</f>
-        <v>3.1138297931572678</v>
+        <v>9.1295930735212831</v>
       </c>
       <c r="I85" s="10">
         <f>MAX(D76*12000/d*0.85/54000, 0.0025*l_2m*12*d)</f>
-        <v>3.7124999999999995</v>
+        <v>8.5425000000000004</v>
       </c>
       <c r="J85" t="s">
         <v>83</v>
@@ -2909,11 +2920,11 @@
       </c>
       <c r="C89" s="7">
         <f>1/12*l_1c*12*h^3</f>
-        <v>8573.75</v>
+        <v>99144</v>
       </c>
       <c r="D89" s="7">
         <f>1/12*l_1m*12*h^3</f>
-        <v>8573.75</v>
+        <v>99144</v>
       </c>
       <c r="E89" t="s">
         <v>85</v>
@@ -2928,11 +2939,11 @@
       </c>
       <c r="C90" s="7">
         <f>1/12*l_1c*12*h^3</f>
-        <v>8573.75</v>
+        <v>99144</v>
       </c>
       <c r="D90" s="7">
         <f>1/12*l_1m*12*h^3</f>
-        <v>8573.75</v>
+        <v>99144</v>
       </c>
       <c r="E90" t="s">
         <v>85</v>
@@ -2947,11 +2958,11 @@
       </c>
       <c r="C91" s="7">
         <f>1/12*l_1c*12*h^3</f>
-        <v>8573.75</v>
+        <v>99144</v>
       </c>
       <c r="D91" s="7">
         <f>1/12*l_1m*12*h^3</f>
-        <v>8573.75</v>
+        <v>99144</v>
       </c>
       <c r="E91" t="s">
         <v>85</v>
@@ -2966,11 +2977,11 @@
       </c>
       <c r="C92" s="7">
         <f>1/12*l_2c*12*h^3</f>
-        <v>8573.75</v>
+        <v>99144</v>
       </c>
       <c r="D92" s="7">
         <f>1/12*l_2m*12*h^3</f>
-        <v>12860.625</v>
+        <v>99144</v>
       </c>
       <c r="E92" t="s">
         <v>85</v>
@@ -2985,11 +2996,11 @@
       </c>
       <c r="C93" s="7">
         <f>1/12*l_2c*12*h^3</f>
-        <v>8573.75</v>
+        <v>99144</v>
       </c>
       <c r="D93" s="7">
         <f>1/12*l_2m*12*h^3</f>
-        <v>12860.625</v>
+        <v>99144</v>
       </c>
       <c r="E93" t="s">
         <v>85</v>
@@ -3004,11 +3015,11 @@
       </c>
       <c r="C94" s="7">
         <f>1/12*l_2c*12*h^3</f>
-        <v>8573.75</v>
+        <v>99144</v>
       </c>
       <c r="D94" s="7">
         <f>1/12*l_2m*12*h^3</f>
-        <v>12860.625</v>
+        <v>99144</v>
       </c>
       <c r="E94" t="s">
         <v>85</v>
@@ -3145,62 +3156,62 @@
       </c>
       <c r="C99" s="7">
         <f t="shared" ref="C99:D104" si="3">IF(N99&lt;1, J99/(1-N99^2*(1-J99/C89)), C89)</f>
-        <v>1687.2288339349891</v>
+        <v>20923.579313621052</v>
       </c>
       <c r="D99" s="7">
         <f t="shared" si="3"/>
-        <v>8573.75</v>
+        <v>99144</v>
       </c>
       <c r="E99" t="s">
         <v>85</v>
       </c>
       <c r="F99" s="30">
         <f>l_1c*12/(n*C80)</f>
-        <v>7.6925462324671399</v>
+        <v>4.2360810280840466</v>
       </c>
       <c r="G99" s="24">
         <f>l_1m*12/(n*D80)</f>
-        <v>7.6925462324671399</v>
+        <v>4.2360810280840466</v>
       </c>
       <c r="H99" s="24">
         <f t="shared" ref="H99:I104" si="4">(SQRT(2*d*F99+1) - 1)/F99</f>
-        <v>1.3403211524542247</v>
+        <v>2.5859853057996141</v>
       </c>
       <c r="I99" s="24">
         <f t="shared" si="4"/>
-        <v>1.3403211524542247</v>
+        <v>2.5859853057996141</v>
       </c>
       <c r="J99" s="25">
         <f>MIN(l_1c * 12*H99^3/3+n*C80*(d-H99)^2,C89)</f>
-        <v>841.09140392569111</v>
+        <v>10837.313640259599</v>
       </c>
       <c r="K99" s="25">
         <f>MIN(l_1m * 12*I99^3/3+n*D80*(d-I99)^2,D89)</f>
-        <v>841.09140392569111</v>
+        <v>10837.313640259599</v>
       </c>
       <c r="L99" s="25">
         <f t="shared" ref="L99:M104" si="5">f_r*C89/y_t * 1 / 12000</f>
-        <v>42.809333824529432</v>
+        <v>292.1058113081628</v>
       </c>
       <c r="M99" s="25">
         <f t="shared" si="5"/>
-        <v>42.809333824529432</v>
+        <v>292.1058113081628</v>
       </c>
       <c r="N99" s="24">
         <f t="shared" ref="N99:O101" si="6">IF((D55+D58)=0, 1.1, L99/(D55+D58))</f>
-        <v>0.74568335519453821</v>
+        <v>0.73567099896416122</v>
       </c>
       <c r="O99" s="24">
         <f t="shared" si="6"/>
-        <v>1.1185250327918075</v>
+        <v>1.1035064984462419</v>
       </c>
       <c r="P99" s="24">
         <f>C80/(l_1c*d)</f>
-        <v>3.0000000000000006E-2</v>
+        <v>3.0000000000000002E-2</v>
       </c>
       <c r="Q99" s="31">
         <f>D80/(l_1m*d)</f>
-        <v>3.0000000000000006E-2</v>
+        <v>3.0000000000000002E-2</v>
       </c>
     </row>
     <row r="100" spans="1:17" ht="18.75" customHeight="1">
@@ -3212,62 +3223,62 @@
       </c>
       <c r="C100" s="7">
         <f t="shared" si="3"/>
-        <v>1415.8499431215773</v>
+        <v>35434.091357987243</v>
       </c>
       <c r="D100" s="7">
         <f t="shared" si="3"/>
-        <v>5176.8048268949115</v>
+        <v>99144</v>
       </c>
       <c r="E100" t="s">
         <v>85</v>
       </c>
       <c r="F100" s="32">
         <f>l_1c*12/(n*C81)</f>
-        <v>4.6998484826775053</v>
+        <v>4.2360810280840466</v>
       </c>
       <c r="G100" s="22">
         <f>l_1m*12/(n*D81)</f>
-        <v>7.6925462324671399</v>
+        <v>4.2360810280840466</v>
       </c>
       <c r="H100" s="22">
         <f t="shared" si="4"/>
-        <v>1.6729694106081459</v>
+        <v>2.5859853057996141</v>
       </c>
       <c r="I100" s="22">
         <f t="shared" si="4"/>
-        <v>1.3403211524542247</v>
+        <v>2.5859853057996141</v>
       </c>
       <c r="J100" s="23">
         <f>MIN(l_1c * 12*H100^3/3+n*C81*(d-H100)^2,C90)</f>
-        <v>1291.7721637893619</v>
+        <v>10837.313640259599</v>
       </c>
       <c r="K100" s="23">
         <f>MIN(l_1m * 12*I100^3/3+n*D81*(d-I100)^2,D90)</f>
-        <v>841.09140392569111</v>
+        <v>10837.313640259599</v>
       </c>
       <c r="L100" s="23">
         <f t="shared" si="5"/>
-        <v>42.809333824529432</v>
+        <v>292.1058113081628</v>
       </c>
       <c r="M100" s="23">
         <f t="shared" si="5"/>
-        <v>42.809333824529432</v>
+        <v>292.1058113081628</v>
       </c>
       <c r="N100" s="22">
         <f t="shared" si="6"/>
-        <v>0.32121744531457036</v>
+        <v>0.88280519875699348</v>
       </c>
       <c r="O100" s="22">
         <f t="shared" si="6"/>
-        <v>0.96365233594371102</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="P100" s="22">
         <f>C81/(l_1c*d)</f>
-        <v>4.9102941897935577E-2</v>
+        <v>3.0000000000000002E-2</v>
       </c>
       <c r="Q100" s="33">
         <f>D81/(l_1m*d)</f>
-        <v>3.0000000000000006E-2</v>
+        <v>3.0000000000000002E-2</v>
       </c>
     </row>
     <row r="101" spans="1:17" ht="18.75" customHeight="1">
@@ -3279,62 +3290,62 @@
       </c>
       <c r="C101" s="7">
         <f t="shared" si="3"/>
-        <v>1415.8499431215773</v>
+        <v>14747.538229238649</v>
       </c>
       <c r="D101" s="7">
         <f t="shared" si="3"/>
-        <v>5176.8048268949115</v>
+        <v>99144</v>
       </c>
       <c r="E101" t="s">
         <v>85</v>
       </c>
       <c r="F101" s="32">
         <f>l_1c*12/(n*C82)</f>
-        <v>4.6998484826775053</v>
+        <v>3.680553562643698</v>
       </c>
       <c r="G101" s="22">
         <f>l_1m*12/(n*D82)</f>
-        <v>7.6925462324671399</v>
+        <v>4.2360810280840466</v>
       </c>
       <c r="H101" s="22">
         <f t="shared" si="4"/>
-        <v>1.6729694106081459</v>
+        <v>2.7574454578775947</v>
       </c>
       <c r="I101" s="22">
         <f t="shared" si="4"/>
-        <v>1.3403211524542247</v>
+        <v>2.5859853057996141</v>
       </c>
       <c r="J101" s="23">
         <f>MIN(l_1c * 12*H101^3/3+n*C82*(d-H101)^2,C91)</f>
-        <v>1291.7721637893619</v>
+        <v>12277.736513163687</v>
       </c>
       <c r="K101" s="23">
         <f>MIN(l_1m * 12*I101^3/3+n*D82*(d-I101)^2,D91)</f>
-        <v>841.09140392569111</v>
+        <v>10837.313640259599</v>
       </c>
       <c r="L101" s="23">
         <f t="shared" si="5"/>
-        <v>42.809333824529432</v>
+        <v>292.1058113081628</v>
       </c>
       <c r="M101" s="23">
         <f t="shared" si="5"/>
-        <v>42.809333824529432</v>
+        <v>292.1058113081628</v>
       </c>
       <c r="N101" s="22">
         <f t="shared" si="6"/>
-        <v>0.32121744531457036</v>
+        <v>0.43719876509870165</v>
       </c>
       <c r="O101" s="22">
         <f t="shared" si="6"/>
-        <v>0.96365233594371102</v>
+        <v>1.3845528259368027</v>
       </c>
       <c r="P101" s="22">
         <f>C82/(l_1c*d)</f>
-        <v>4.9102941897935577E-2</v>
+        <v>3.4528075377672149E-2</v>
       </c>
       <c r="Q101" s="33">
         <f>D82/(l_1m*d)</f>
-        <v>3.0000000000000006E-2</v>
+        <v>3.0000000000000002E-2</v>
       </c>
     </row>
     <row r="102" spans="1:17" ht="18.75" customHeight="1">
@@ -3346,62 +3357,62 @@
       </c>
       <c r="C102" s="7">
         <f t="shared" si="3"/>
-        <v>5562.3949754248479</v>
+        <v>99144</v>
       </c>
       <c r="D102" s="7">
         <f t="shared" si="3"/>
-        <v>12860.625</v>
+        <v>99144</v>
       </c>
       <c r="E102" t="s">
         <v>85</v>
       </c>
       <c r="F102" s="32">
         <f>l_2c*12/(n*C83)</f>
-        <v>7.6925462324671399</v>
+        <v>4.2360810280840466</v>
       </c>
       <c r="G102" s="22">
         <f>l_2m*12/(n*D83)</f>
-        <v>7.6925462324671434</v>
+        <v>4.2360810280840466</v>
       </c>
       <c r="H102" s="22">
         <f t="shared" si="4"/>
-        <v>1.3403211524542247</v>
+        <v>2.5859853057996141</v>
       </c>
       <c r="I102" s="22">
         <f t="shared" si="4"/>
-        <v>1.3403211524542245</v>
+        <v>2.5859853057996141</v>
       </c>
       <c r="J102" s="23">
         <f>MIN(l_2c * 12*H102^3/3+n*C83*(d-H102)^2,C92)</f>
-        <v>841.09140392569111</v>
+        <v>10837.313640259599</v>
       </c>
       <c r="K102" s="23">
         <f>MIN(l_2m * 12*I102^3/3+n*D83*(d-I102)^2,D92)</f>
-        <v>1261.6371058885361</v>
+        <v>10837.313640259599</v>
       </c>
       <c r="L102" s="23">
         <f t="shared" si="5"/>
-        <v>42.809333824529432</v>
+        <v>292.1058113081628</v>
       </c>
       <c r="M102" s="23">
         <f t="shared" si="5"/>
-        <v>64.214000736794148</v>
+        <v>292.1058113081628</v>
       </c>
       <c r="N102" s="22">
         <f t="shared" ref="N102:O104" si="7">IF((D61+D64)=0, 1.1, L102/(D61+D64))</f>
-        <v>0.97011013252848566</v>
+        <v>1.092996912746754</v>
       </c>
       <c r="O102" s="22">
         <f t="shared" si="7"/>
-        <v>2.182747798189093</v>
+        <v>1.6394953691201311</v>
       </c>
       <c r="P102" s="22">
         <f>C83/(l_2c*d)</f>
-        <v>3.0000000000000006E-2</v>
+        <v>3.0000000000000002E-2</v>
       </c>
       <c r="Q102" s="33">
         <f>D83/(l_2m*d)</f>
-        <v>2.9999999999999995E-2</v>
+        <v>3.0000000000000002E-2</v>
       </c>
     </row>
     <row r="103" spans="1:17" ht="18.75" customHeight="1">
@@ -3413,62 +3424,62 @@
       </c>
       <c r="C103" s="7">
         <f t="shared" si="3"/>
-        <v>1216.0484164407735</v>
+        <v>14299.936557503812</v>
       </c>
       <c r="D103" s="7">
         <f t="shared" si="3"/>
-        <v>12860.625</v>
+        <v>99144</v>
       </c>
       <c r="E103" t="s">
         <v>85</v>
       </c>
       <c r="F103" s="32">
         <f>l_2c*12/(n*C84)</f>
-        <v>6.1143521611858969</v>
+        <v>3.9636730674624419</v>
       </c>
       <c r="G103" s="22">
         <f>l_2m*12/(n*D84)</f>
-        <v>7.6925462324671434</v>
+        <v>4.2360810280840466</v>
       </c>
       <c r="H103" s="22">
         <f t="shared" si="4"/>
-        <v>1.4873038771390279</v>
+        <v>2.665825868427758</v>
       </c>
       <c r="I103" s="22">
         <f t="shared" si="4"/>
-        <v>1.3403211524542245</v>
+        <v>2.5859853057996141</v>
       </c>
       <c r="J103" s="23">
         <f>MIN(l_2c * 12*H103^3/3+n*C84*(d-H103)^2,C93)</f>
-        <v>1029.1755576397973</v>
+        <v>11497.542113570875</v>
       </c>
       <c r="K103" s="23">
         <f>MIN(l_2m * 12*I103^3/3+n*D84*(d-I103)^2,D93)</f>
-        <v>1261.6371058885361</v>
+        <v>10837.313640259599</v>
       </c>
       <c r="L103" s="23">
         <f t="shared" si="5"/>
-        <v>42.809333824529432</v>
+        <v>292.1058113081628</v>
       </c>
       <c r="M103" s="23">
         <f t="shared" si="5"/>
-        <v>64.214000736794148</v>
+        <v>292.1058113081628</v>
       </c>
       <c r="N103" s="22">
         <f t="shared" si="7"/>
-        <v>0.41789359555073224</v>
+        <v>0.47082943933706317</v>
       </c>
       <c r="O103" s="22">
         <f t="shared" si="7"/>
-        <v>1.8805211799782953</v>
+        <v>1.4124883180111898</v>
       </c>
       <c r="P103" s="22">
         <f>C84/(l_2c*d)</f>
-        <v>3.7743391432209304E-2</v>
+        <v>3.2061784279267015E-2</v>
       </c>
       <c r="Q103" s="33">
         <f>D84/(l_2m*d)</f>
-        <v>2.9999999999999995E-2</v>
+        <v>3.0000000000000002E-2</v>
       </c>
     </row>
     <row r="104" spans="1:17" ht="19.5" customHeight="1" thickBot="1">
@@ -3480,62 +3491,62 @@
       </c>
       <c r="C104" s="7">
         <f t="shared" si="3"/>
-        <v>1216.0484164407735</v>
+        <v>14299.936557503812</v>
       </c>
       <c r="D104" s="7">
         <f t="shared" si="3"/>
-        <v>12860.625</v>
+        <v>99144</v>
       </c>
       <c r="E104" t="s">
         <v>85</v>
       </c>
       <c r="F104" s="34">
         <f>l_2c*12/(n*C85)</f>
-        <v>6.1143521611858969</v>
+        <v>3.9636730674624419</v>
       </c>
       <c r="G104" s="35">
         <f>l_2m*12/(n*D85)</f>
-        <v>7.6925462324671434</v>
+        <v>4.2360810280840466</v>
       </c>
       <c r="H104" s="35">
         <f t="shared" si="4"/>
-        <v>1.4873038771390279</v>
+        <v>2.665825868427758</v>
       </c>
       <c r="I104" s="35">
         <f t="shared" si="4"/>
-        <v>1.3403211524542245</v>
+        <v>2.5859853057996141</v>
       </c>
       <c r="J104" s="36">
         <f>MIN(l_2c * 12*H104^3/3+n*C85*(d-H104)^2,C94)</f>
-        <v>1029.1755576397973</v>
+        <v>11497.542113570875</v>
       </c>
       <c r="K104" s="36">
         <f>MIN(l_2m * 12*I104^3/3+n*D85*(d-I104)^2,D94)</f>
-        <v>1261.6371058885361</v>
+        <v>10837.313640259599</v>
       </c>
       <c r="L104" s="36">
         <f t="shared" si="5"/>
-        <v>42.809333824529432</v>
+        <v>292.1058113081628</v>
       </c>
       <c r="M104" s="36">
         <f t="shared" si="5"/>
-        <v>64.214000736794148</v>
+        <v>292.1058113081628</v>
       </c>
       <c r="N104" s="35">
         <f t="shared" si="7"/>
-        <v>0.41789359555073224</v>
+        <v>0.47082943933706317</v>
       </c>
       <c r="O104" s="35">
         <f t="shared" si="7"/>
-        <v>1.8805211799782953</v>
+        <v>1.4124883180111898</v>
       </c>
       <c r="P104" s="35">
         <f>C85/(l_2c*d)</f>
-        <v>3.7743391432209304E-2</v>
+        <v>3.2061784279267015E-2</v>
       </c>
       <c r="Q104" s="37">
         <f>D85/(l_2m*d)</f>
-        <v>2.9999999999999995E-2</v>
+        <v>3.0000000000000002E-2</v>
       </c>
     </row>
     <row r="106" spans="1:17" ht="18" customHeight="1">
@@ -3560,11 +3571,11 @@
       </c>
       <c r="B108" s="7">
         <f>0.7*C99+ 0.15*SUM(C100:C101)</f>
-        <v>1605.8151666909655</v>
+        <v>22173.74995761862</v>
       </c>
       <c r="C108" s="7">
         <f>0.7*D99+ 0.15*SUM(D100:D101)</f>
-        <v>7554.6664480684731</v>
+        <v>99143.999999999985</v>
       </c>
       <c r="D108" t="s">
         <v>85</v>
@@ -3576,11 +3587,11 @@
       </c>
       <c r="B109" s="7">
         <f>0.7*C102+ 0.15*SUM(C103:C104)</f>
-        <v>4258.4910077296254</v>
+        <v>73690.780967251136</v>
       </c>
       <c r="C109" s="7">
         <f>0.7*D102+ 0.15*SUM(D103:D104)</f>
-        <v>12860.625</v>
+        <v>99143.999999999985</v>
       </c>
       <c r="D109" t="s">
         <v>85</v>
@@ -3602,7 +3613,7 @@
       </c>
       <c r="B112" s="7">
         <f>IF(l_1/l_2&lt;1.05, B108+C109, (B108+C108+B109+C109)/2)</f>
-        <v>13139.798811244533</v>
+        <v>121317.74995761861</v>
       </c>
       <c r="C112" t="s">
         <v>85</v>
@@ -3623,7 +3634,7 @@
       </c>
       <c r="B115" s="7">
         <f>IF(l_1/l_2&lt;1.05, C89+D92, (C89+D89+C92+D92)/2)</f>
-        <v>19290.9375</v>
+        <v>198288</v>
       </c>
       <c r="C115" t="s">
         <v>85</v>
@@ -3640,7 +3651,7 @@
       </c>
       <c r="B118" s="10">
         <f>B112/B115</f>
-        <v>0.68113842633332533</v>
+        <v>0.61182598017842027</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="19.5" customHeight="1" thickBot="1">
@@ -3657,7 +3668,7 @@
       </c>
       <c r="B121">
         <f>IF(MAX(c_1, c_2)&gt;24, 2.1, 1.9)</f>
-        <v>1.9</v>
+        <v>2.1</v>
       </c>
       <c r="D121" s="27">
         <v>1</v>
@@ -3676,7 +3687,7 @@
 IF(B5=1.5,E122,
 IF(AND(B5&gt;1.5, B5&lt;2), E122+(E123-E122)/(D123-D122)*(B5-D122), E123)
 )))</f>
-        <v>8.02</v>
+        <v>7.12</v>
       </c>
       <c r="D122" s="13">
         <v>1.5</v>
@@ -3691,7 +3702,7 @@
       </c>
       <c r="B123" s="4">
         <f>(SW+SDL+LLvib)/32.2</f>
-        <v>4.6506211180124222</v>
+        <v>7.3291925465838501</v>
       </c>
       <c r="C123" t="s">
         <v>105</v>
@@ -3709,7 +3720,7 @@
       </c>
       <c r="B124" s="4">
         <f>k_2*lambda_i_sq / (2 * PI() * l_1^2) * SQRT(k_1 * E_c*144*(h/12)^3 / (12*gamma*(1-nu^2)))</f>
-        <v>7.9328615571404866</v>
+        <v>8.7618923090782665</v>
       </c>
       <c r="C124" t="s">
         <v>107</v>
@@ -3726,7 +3737,7 @@
       </c>
       <c r="B127" s="6">
         <f>gamma*32.2*l_1*l_2</f>
-        <v>74875</v>
+        <v>272816</v>
       </c>
       <c r="C127" t="s">
         <v>110</v>
@@ -3737,7 +3748,7 @@
         <v>111</v>
       </c>
       <c r="B128">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
     </row>
   </sheetData>
@@ -3747,18 +3758,373 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:O13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" style="8" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" style="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" s="52" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="18" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" s="4">
+        <f>f_n</f>
+        <v>8.7618923090782665</v>
+      </c>
+      <c r="C3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="6">
+        <f>Slab_Properties!B127</f>
+        <v>272816</v>
+      </c>
+      <c r="C4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5">
+        <f>Slab_Properties!B128</f>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="11"/>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="52" t="s">
+        <v>147</v>
+      </c>
+      <c r="H7" s="56" t="s">
+        <v>148</v>
+      </c>
+      <c r="I7" s="56" t="s">
+        <v>149</v>
+      </c>
+      <c r="L7" s="56" t="s">
+        <v>150</v>
+      </c>
+      <c r="M7" s="8"/>
+    </row>
+    <row r="8" spans="1:15" ht="18" customHeight="1">
+      <c r="A8" s="56" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8" s="56" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" s="56" t="s">
+        <v>152</v>
+      </c>
+      <c r="D8" s="56" t="s">
+        <v>153</v>
+      </c>
+      <c r="E8" s="56" t="s">
+        <v>154</v>
+      </c>
+      <c r="F8" s="56" t="s">
+        <v>155</v>
+      </c>
+      <c r="G8" s="57" t="s">
+        <v>156</v>
+      </c>
+      <c r="H8" s="56" t="s">
+        <v>157</v>
+      </c>
+      <c r="I8" s="56" t="s">
+        <v>158</v>
+      </c>
+      <c r="J8" s="56" t="s">
+        <v>161</v>
+      </c>
+      <c r="K8" s="56" t="s">
+        <v>160</v>
+      </c>
+      <c r="L8" s="56" t="s">
+        <v>159</v>
+      </c>
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="56"/>
+      <c r="B9" s="56" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="56" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" s="56" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="56" t="s">
+        <v>107</v>
+      </c>
+      <c r="F9" s="56" t="s">
+        <v>107</v>
+      </c>
+      <c r="G9" s="57"/>
+      <c r="H9" s="56" t="s">
+        <v>143</v>
+      </c>
+      <c r="I9" s="56" t="s">
+        <v>143</v>
+      </c>
+      <c r="J9" s="56" t="s">
+        <v>143</v>
+      </c>
+      <c r="K9" s="56" t="s">
+        <v>143</v>
+      </c>
+      <c r="L9" s="56" t="s">
+        <v>143</v>
+      </c>
+      <c r="M9" s="8"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10" s="10">
+        <f>$B$3</f>
+        <v>8.7618923090782665</v>
+      </c>
+      <c r="C10" s="56">
+        <v>1.25</v>
+      </c>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7">
+        <f>250000000/($B$4*$B$5)*($C10^2.43/$B10^1.8)*(1-EXP(-2*PI()*$B$5*$B10/$C10))</f>
+        <v>656.12079321093131</v>
+      </c>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7">
+        <f>250000000/($B$4*$B$5)*($C10^2.43/$B10^1.8)*(1-EXP(-2*PI()*$B$5*$B10/$C10))</f>
+        <v>656.12079321093131</v>
+      </c>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7">
+        <f>I10</f>
+        <v>656.12079321093131</v>
+      </c>
+      <c r="N10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="56" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" s="10">
+        <f>$B$3</f>
+        <v>8.7618923090782665</v>
+      </c>
+      <c r="C11" s="56">
+        <v>1.6</v>
+      </c>
+      <c r="D11" s="56">
+        <v>6.8</v>
+      </c>
+      <c r="E11" s="56">
+        <v>6</v>
+      </c>
+      <c r="F11" s="56">
+        <v>8</v>
+      </c>
+      <c r="G11" s="56">
+        <v>0.1</v>
+      </c>
+      <c r="H11" s="7">
+        <f>175000000/($B$4*$B$5*SQRT($B11))*(EXP(-$G11*$B11))</f>
+        <v>2255.7196184024665</v>
+      </c>
+      <c r="I11" s="7">
+        <f t="shared" ref="I11:K13" si="0">250000000/($B$4*$B$5)*($C11^2.43/$B11^1.8)*(1-EXP(-2*PI()*$B$5*$B11/$C11))</f>
+        <v>1078.8284997051478</v>
+      </c>
+      <c r="J11" s="7">
+        <f>175000000/($B$4*$B$5*SQRT($E11))*(EXP(-$G11*$E11))</f>
+        <v>3592.9891519248181</v>
+      </c>
+      <c r="K11" s="7">
+        <f>250000000/($B$4*$B$5)*($C11^2.43/$F11^1.8)*(1-EXP(-2*PI()*$B$5*$F11/$C11))</f>
+        <v>1216.1941326856029</v>
+      </c>
+      <c r="L11" s="7" t="str">
+        <f>IF(AND($B11&gt;$E11,$B11&lt;$F11),$J11 + ($B11-$E11) * ($K11-$J11)/($F11-$E11), "N/A")</f>
+        <v>N/A</v>
+      </c>
+      <c r="M11" s="7">
+        <f>IF($B11&gt;=F11,I11, IF($B11&lt;=E11,H11,L11))</f>
+        <v>1078.8284997051478</v>
+      </c>
+      <c r="N11" t="s">
+        <v>143</v>
+      </c>
+      <c r="O11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="56" t="s">
+        <v>131</v>
+      </c>
+      <c r="B12" s="10">
+        <f>$B$3</f>
+        <v>8.7618923090782665</v>
+      </c>
+      <c r="C12" s="56">
+        <v>1.85</v>
+      </c>
+      <c r="D12" s="56">
+        <v>8</v>
+      </c>
+      <c r="E12" s="56">
+        <v>7</v>
+      </c>
+      <c r="F12" s="56">
+        <v>9</v>
+      </c>
+      <c r="G12" s="56">
+        <v>0.09</v>
+      </c>
+      <c r="H12" s="7">
+        <f>175000000/($B$4*$B$5*SQRT($B12))*(EXP(-$G12*$B12))</f>
+        <v>2462.2805328579611</v>
+      </c>
+      <c r="I12" s="7">
+        <f t="shared" si="0"/>
+        <v>1429.2044039665213</v>
+      </c>
+      <c r="J12" s="7">
+        <f>175000000/($B$4*$B$5*SQRT($E12))*(EXP(-$G12*$E12))</f>
+        <v>3228.1497780927662</v>
+      </c>
+      <c r="K12" s="7">
+        <f>250000000/($B$4*$B$5)*($C12^2.43/$F12^1.8)*(1-EXP(-2*PI()*$B$5*$F12/$C12))</f>
+        <v>1380.809616979338</v>
+      </c>
+      <c r="L12" s="7">
+        <f t="shared" ref="L12:L13" si="1">IF(AND($B12&gt;$E12,$B12&lt;$F12),$J12 + ($B12-$E12) * ($K12-$J12)/($F12-$E12), "N/A")</f>
+        <v>1600.7425670341886</v>
+      </c>
+      <c r="M12" s="7">
+        <f>IF($B12&gt;=F12,I12, IF($B12&lt;=E12,H12,L12))</f>
+        <v>1600.7425670341886</v>
+      </c>
+      <c r="N12" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="56" t="s">
+        <v>132</v>
+      </c>
+      <c r="B13" s="10">
+        <f>$B$3</f>
+        <v>8.7618923090782665</v>
+      </c>
+      <c r="C13" s="56">
+        <v>2.1</v>
+      </c>
+      <c r="D13" s="56">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="E13" s="56">
+        <v>8</v>
+      </c>
+      <c r="F13" s="56">
+        <v>10</v>
+      </c>
+      <c r="G13" s="56">
+        <v>0.08</v>
+      </c>
+      <c r="H13" s="7">
+        <f>175000000/($B$4*$B$5*SQRT($B13))*(EXP(-$G13*$B13))</f>
+        <v>2687.7566577999919</v>
+      </c>
+      <c r="I13" s="7">
+        <f t="shared" si="0"/>
+        <v>1815.3442636622767</v>
+      </c>
+      <c r="J13" s="7">
+        <f>175000000/($B$4*$B$5*SQRT($E13))*(EXP(-$G13*$E13))</f>
+        <v>2989.611520406525</v>
+      </c>
+      <c r="K13" s="7">
+        <f>250000000/($B$4*$B$5)*($C13^2.43/$F13^1.8)*(1-EXP(-2*PI()*$B$5*$F13/$C13))</f>
+        <v>1537.3001262352725</v>
+      </c>
+      <c r="L13" s="7">
+        <f t="shared" si="1"/>
+        <v>2436.3590796036187</v>
+      </c>
+      <c r="M13" s="7">
+        <f>IF($B13&gt;=F13,I13, IF($B13&lt;=E13,H13,L13))</f>
+        <v>2436.3590796036187</v>
+      </c>
+      <c r="N13" t="s">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EB7F394-EE42-4FAF-93E6-B2553F751B52}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AI42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="13.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="18" customHeight="1">
@@ -4016,6 +4382,15 @@
       <c r="O3" s="59">
         <v>11</v>
       </c>
+      <c r="P3">
+        <v>3.3500000000000001E-3</v>
+      </c>
+      <c r="Q3">
+        <v>2.7899999999999999E-3</v>
+      </c>
+      <c r="R3">
+        <v>5.64E-3</v>
+      </c>
       <c r="S3" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -4025,9 +4400,15 @@
       <c r="U3" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V3" s="56"/>
-      <c r="W3" s="56"/>
-      <c r="X3" s="56"/>
+      <c r="V3" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W3" s="56">
+        <v>5.2300000000000003E-3</v>
+      </c>
+      <c r="X3" s="56">
+        <v>5.2300000000000003E-3</v>
+      </c>
       <c r="Y3" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -4047,19 +4428,19 @@
         <v>186.11600000000001</v>
       </c>
       <c r="AE3" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF3" s="56">
-        <v>3382</v>
+        <v>3130</v>
       </c>
       <c r="AG3" s="56">
-        <v>12010</v>
+        <v>9008</v>
       </c>
       <c r="AH3" s="56">
-        <v>12430</v>
+        <v>9322</v>
       </c>
       <c r="AI3" s="56">
-        <v>12863</v>
+        <v>9647</v>
       </c>
     </row>
     <row r="4" spans="1:35">
@@ -4108,6 +4489,15 @@
       <c r="O4" s="59">
         <v>11</v>
       </c>
+      <c r="P4">
+        <v>3.32E-3</v>
+      </c>
+      <c r="Q4">
+        <v>2.7599999999999999E-3</v>
+      </c>
+      <c r="R4">
+        <v>5.5799999999999999E-3</v>
+      </c>
       <c r="S4" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -4117,9 +4507,15 @@
       <c r="U4" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V4" s="56"/>
-      <c r="W4" s="56"/>
-      <c r="X4" s="56"/>
+      <c r="V4" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W4" s="56">
+        <v>5.1799999999999997E-3</v>
+      </c>
+      <c r="X4" s="56">
+        <v>5.1799999999999997E-3</v>
+      </c>
       <c r="Y4" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -4139,19 +4535,19 @@
         <v>186.11600000000001</v>
       </c>
       <c r="AE4" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF4" s="56">
-        <v>2972</v>
+        <v>2725</v>
       </c>
       <c r="AG4" s="56">
-        <v>10796</v>
+        <v>8097</v>
       </c>
       <c r="AH4" s="56">
-        <v>11223</v>
+        <v>8417</v>
       </c>
       <c r="AI4" s="56">
-        <v>11667</v>
+        <v>8750</v>
       </c>
     </row>
     <row r="5" spans="1:35">
@@ -4200,6 +4596,15 @@
       <c r="O5" s="59">
         <v>11</v>
       </c>
+      <c r="P5">
+        <v>3.2799999999999999E-3</v>
+      </c>
+      <c r="Q5">
+        <v>2.7399999999999998E-3</v>
+      </c>
+      <c r="R5">
+        <v>5.5199999999999997E-3</v>
+      </c>
       <c r="S5" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -4209,9 +4614,15 @@
       <c r="U5" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V5" s="56"/>
-      <c r="W5" s="56"/>
-      <c r="X5" s="56"/>
+      <c r="V5" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W5" s="56">
+        <v>5.13E-3</v>
+      </c>
+      <c r="X5" s="56">
+        <v>5.13E-3</v>
+      </c>
       <c r="Y5" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -4231,19 +4642,19 @@
         <v>186.11600000000001</v>
       </c>
       <c r="AE5" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF5" s="56">
-        <v>2884</v>
+        <v>2640</v>
       </c>
       <c r="AG5" s="56">
-        <v>10529</v>
+        <v>7897</v>
       </c>
       <c r="AH5" s="56">
-        <v>10958</v>
+        <v>8218</v>
       </c>
       <c r="AI5" s="56">
-        <v>11404</v>
+        <v>8553</v>
       </c>
     </row>
     <row r="6" spans="1:35">
@@ -4292,6 +4703,15 @@
       <c r="O6" s="59">
         <v>11</v>
       </c>
+      <c r="P6">
+        <v>3.2499999999999999E-3</v>
+      </c>
+      <c r="Q6">
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="R6">
+        <v>5.4599999999999996E-3</v>
+      </c>
       <c r="S6" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -4301,9 +4721,15 @@
       <c r="U6" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V6" s="56"/>
-      <c r="W6" s="56"/>
-      <c r="X6" s="56"/>
+      <c r="V6" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W6" s="56">
+        <v>5.0800000000000003E-3</v>
+      </c>
+      <c r="X6" s="56">
+        <v>5.0800000000000003E-3</v>
+      </c>
       <c r="Y6" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -4323,19 +4749,19 @@
         <v>186.11600000000001</v>
       </c>
       <c r="AE6" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF6" s="56">
-        <v>2794</v>
+        <v>2551</v>
       </c>
       <c r="AG6" s="56">
-        <v>10251</v>
+        <v>7688</v>
       </c>
       <c r="AH6" s="56">
-        <v>10681</v>
+        <v>8011</v>
       </c>
       <c r="AI6" s="56">
-        <v>11129</v>
+        <v>8347</v>
       </c>
     </row>
     <row r="7" spans="1:35">
@@ -4384,6 +4810,15 @@
       <c r="O7" s="59">
         <v>11</v>
       </c>
+      <c r="P7">
+        <v>3.2100000000000002E-3</v>
+      </c>
+      <c r="Q7">
+        <v>2.6800000000000001E-3</v>
+      </c>
+      <c r="R7">
+        <v>5.4000000000000003E-3</v>
+      </c>
       <c r="S7" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -4393,9 +4828,15 @@
       <c r="U7" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V7" s="56"/>
-      <c r="W7" s="56"/>
-      <c r="X7" s="56"/>
+      <c r="V7" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W7" s="56">
+        <v>5.0200000000000002E-3</v>
+      </c>
+      <c r="X7" s="56">
+        <v>5.0200000000000002E-3</v>
+      </c>
       <c r="Y7" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -4415,19 +4856,19 @@
         <v>186.11600000000001</v>
       </c>
       <c r="AE7" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF7" s="56">
-        <v>2688</v>
+        <v>2447</v>
       </c>
       <c r="AG7" s="56">
-        <v>9919</v>
+        <v>7439</v>
       </c>
       <c r="AH7" s="56">
-        <v>10350</v>
+        <v>7763</v>
       </c>
       <c r="AI7" s="56">
-        <v>10801</v>
+        <v>8101</v>
       </c>
     </row>
     <row r="8" spans="1:35">
@@ -4476,6 +4917,15 @@
       <c r="O8" s="59">
         <v>11</v>
       </c>
+      <c r="P8">
+        <v>2.9399999999999999E-3</v>
+      </c>
+      <c r="Q8">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R8">
+        <v>4.9500000000000004E-3</v>
+      </c>
       <c r="S8" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -4485,9 +4935,15 @@
       <c r="U8" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V8" s="56"/>
-      <c r="W8" s="56"/>
-      <c r="X8" s="56"/>
+      <c r="V8" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W8" s="56">
+        <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="X8" s="56">
+        <v>4.5999999999999999E-3</v>
+      </c>
       <c r="Y8" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -4507,19 +4963,19 @@
         <v>200.566</v>
       </c>
       <c r="AE8" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF8" s="56">
-        <v>2083</v>
+        <v>1871</v>
       </c>
       <c r="AG8" s="56">
-        <v>7872</v>
+        <v>5904</v>
       </c>
       <c r="AH8" s="56">
-        <v>8276</v>
+        <v>6207</v>
       </c>
       <c r="AI8" s="56">
-        <v>8702</v>
+        <v>6526</v>
       </c>
     </row>
     <row r="9" spans="1:35">
@@ -4568,6 +5024,15 @@
       <c r="O9" s="59">
         <v>11</v>
       </c>
+      <c r="P9">
+        <v>2.9099999999999998E-3</v>
+      </c>
+      <c r="Q9">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R9">
+        <v>4.8999999999999998E-3</v>
+      </c>
       <c r="S9" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -4577,9 +5042,15 @@
       <c r="U9" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V9" s="56"/>
-      <c r="W9" s="56"/>
-      <c r="X9" s="56"/>
+      <c r="V9" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W9" s="56">
+        <v>4.5500000000000002E-3</v>
+      </c>
+      <c r="X9" s="56">
+        <v>4.5500000000000002E-3</v>
+      </c>
       <c r="Y9" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -4599,19 +5070,19 @@
         <v>200.566</v>
       </c>
       <c r="AE9" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF9" s="56">
-        <v>1853</v>
+        <v>1648</v>
       </c>
       <c r="AG9" s="56">
-        <v>7086</v>
+        <v>5315</v>
       </c>
       <c r="AH9" s="56">
-        <v>7490</v>
+        <v>5618</v>
       </c>
       <c r="AI9" s="56">
-        <v>7918</v>
+        <v>5938</v>
       </c>
     </row>
     <row r="10" spans="1:35">
@@ -4660,6 +5131,15 @@
       <c r="O10" s="59">
         <v>11</v>
       </c>
+      <c r="P10">
+        <v>2.8800000000000002E-3</v>
+      </c>
+      <c r="Q10">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R10">
+        <v>4.8500000000000001E-3</v>
+      </c>
       <c r="S10" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -4669,9 +5149,15 @@
       <c r="U10" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V10" s="56"/>
-      <c r="W10" s="56"/>
-      <c r="X10" s="56"/>
+      <c r="V10" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W10" s="56">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="X10" s="56">
+        <v>4.4999999999999997E-3</v>
+      </c>
       <c r="Y10" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -4691,19 +5177,19 @@
         <v>200.566</v>
       </c>
       <c r="AE10" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF10" s="56">
-        <v>1845</v>
+        <v>1640</v>
       </c>
       <c r="AG10" s="56">
-        <v>7059</v>
+        <v>5294</v>
       </c>
       <c r="AH10" s="56">
-        <v>7464</v>
+        <v>5598</v>
       </c>
       <c r="AI10" s="56">
-        <v>7891</v>
+        <v>5918</v>
       </c>
     </row>
     <row r="11" spans="1:35">
@@ -4752,6 +5238,15 @@
       <c r="O11" s="59">
         <v>11</v>
       </c>
+      <c r="P11">
+        <v>2.8500000000000001E-3</v>
+      </c>
+      <c r="Q11">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R11">
+        <v>4.7999999999999996E-3</v>
+      </c>
       <c r="S11" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -4761,9 +5256,15 @@
       <c r="U11" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V11" s="56"/>
-      <c r="W11" s="56"/>
-      <c r="X11" s="56"/>
+      <c r="V11" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W11" s="56">
+        <v>4.4600000000000004E-3</v>
+      </c>
+      <c r="X11" s="56">
+        <v>4.4600000000000004E-3</v>
+      </c>
       <c r="Y11" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -4783,19 +5284,19 @@
         <v>200.566</v>
       </c>
       <c r="AE11" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF11" s="56">
-        <v>1837</v>
+        <v>1633</v>
       </c>
       <c r="AG11" s="56">
-        <v>7032</v>
+        <v>5274</v>
       </c>
       <c r="AH11" s="56">
-        <v>7437</v>
+        <v>5578</v>
       </c>
       <c r="AI11" s="56">
-        <v>7864</v>
+        <v>5898</v>
       </c>
     </row>
     <row r="12" spans="1:35">
@@ -4844,6 +5345,15 @@
       <c r="O12" s="59">
         <v>11</v>
       </c>
+      <c r="P12">
+        <v>2.82E-3</v>
+      </c>
+      <c r="Q12">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R12">
+        <v>4.7400000000000003E-3</v>
+      </c>
       <c r="S12" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -4853,9 +5363,15 @@
       <c r="U12" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V12" s="56"/>
-      <c r="W12" s="56"/>
-      <c r="X12" s="56"/>
+      <c r="V12" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W12" s="56">
+        <v>4.4099999999999999E-3</v>
+      </c>
+      <c r="X12" s="56">
+        <v>4.4099999999999999E-3</v>
+      </c>
       <c r="Y12" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -4875,19 +5391,19 @@
         <v>200.566</v>
       </c>
       <c r="AE12" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF12" s="56">
-        <v>1830</v>
+        <v>1626</v>
       </c>
       <c r="AG12" s="56">
-        <v>7006</v>
+        <v>5254</v>
       </c>
       <c r="AH12" s="56">
-        <v>7410</v>
+        <v>5558</v>
       </c>
       <c r="AI12" s="56">
-        <v>7838</v>
+        <v>5878</v>
       </c>
     </row>
     <row r="13" spans="1:35">
@@ -4936,6 +5452,15 @@
       <c r="O13" s="59">
         <v>11</v>
       </c>
+      <c r="P13">
+        <v>2.9399999999999999E-3</v>
+      </c>
+      <c r="Q13">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R13">
+        <v>4.9500000000000004E-3</v>
+      </c>
       <c r="S13" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -4945,9 +5470,15 @@
       <c r="U13" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V13" s="56"/>
-      <c r="W13" s="56"/>
-      <c r="X13" s="56"/>
+      <c r="V13" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W13" s="56">
+        <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="X13" s="56">
+        <v>4.5999999999999999E-3</v>
+      </c>
       <c r="Y13" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -4967,19 +5498,19 @@
         <v>200.566</v>
       </c>
       <c r="AE13" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF13" s="56">
-        <v>2083</v>
+        <v>1871</v>
       </c>
       <c r="AG13" s="56">
-        <v>7872</v>
+        <v>5904</v>
       </c>
       <c r="AH13" s="56">
-        <v>8276</v>
+        <v>6207</v>
       </c>
       <c r="AI13" s="56">
-        <v>8702</v>
+        <v>6526</v>
       </c>
     </row>
     <row r="14" spans="1:35">
@@ -5028,6 +5559,15 @@
       <c r="O14" s="59">
         <v>11</v>
       </c>
+      <c r="P14">
+        <v>2.9099999999999998E-3</v>
+      </c>
+      <c r="Q14">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R14">
+        <v>4.8999999999999998E-3</v>
+      </c>
       <c r="S14" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -5037,9 +5577,15 @@
       <c r="U14" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V14" s="56"/>
-      <c r="W14" s="56"/>
-      <c r="X14" s="56"/>
+      <c r="V14" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W14" s="56">
+        <v>4.5500000000000002E-3</v>
+      </c>
+      <c r="X14" s="56">
+        <v>4.5500000000000002E-3</v>
+      </c>
       <c r="Y14" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -5059,19 +5605,19 @@
         <v>200.566</v>
       </c>
       <c r="AE14" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF14" s="56">
-        <v>1853</v>
+        <v>1648</v>
       </c>
       <c r="AG14" s="56">
-        <v>7086</v>
+        <v>5315</v>
       </c>
       <c r="AH14" s="56">
-        <v>7490</v>
+        <v>5618</v>
       </c>
       <c r="AI14" s="56">
-        <v>7918</v>
+        <v>5938</v>
       </c>
     </row>
     <row r="15" spans="1:35">
@@ -5120,6 +5666,15 @@
       <c r="O15" s="59">
         <v>11</v>
       </c>
+      <c r="P15">
+        <v>2.8800000000000002E-3</v>
+      </c>
+      <c r="Q15">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R15">
+        <v>4.8500000000000001E-3</v>
+      </c>
       <c r="S15" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -5129,9 +5684,15 @@
       <c r="U15" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V15" s="56"/>
-      <c r="W15" s="56"/>
-      <c r="X15" s="56"/>
+      <c r="V15" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W15" s="56">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="X15" s="56">
+        <v>4.4999999999999997E-3</v>
+      </c>
       <c r="Y15" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -5151,19 +5712,19 @@
         <v>200.566</v>
       </c>
       <c r="AE15" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF15" s="56">
-        <v>1845</v>
+        <v>1640</v>
       </c>
       <c r="AG15" s="56">
-        <v>7059</v>
+        <v>5294</v>
       </c>
       <c r="AH15" s="56">
-        <v>7464</v>
+        <v>5598</v>
       </c>
       <c r="AI15" s="56">
-        <v>7891</v>
+        <v>5918</v>
       </c>
     </row>
     <row r="16" spans="1:35">
@@ -5212,6 +5773,15 @@
       <c r="O16" s="59">
         <v>11</v>
       </c>
+      <c r="P16">
+        <v>2.5300000000000001E-3</v>
+      </c>
+      <c r="Q16">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R16">
+        <v>4.2599999999999999E-3</v>
+      </c>
       <c r="S16" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -5221,9 +5791,15 @@
       <c r="U16" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V16" s="56"/>
-      <c r="W16" s="56"/>
-      <c r="X16" s="56"/>
+      <c r="V16" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W16" s="56">
+        <v>3.96E-3</v>
+      </c>
+      <c r="X16" s="56">
+        <v>3.96E-3</v>
+      </c>
       <c r="Y16" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -5243,19 +5819,19 @@
         <v>215.01599999999999</v>
       </c>
       <c r="AE16" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF16" s="56">
-        <v>1417</v>
+        <v>1240</v>
       </c>
       <c r="AG16" s="56">
-        <v>4869</v>
+        <v>3715</v>
       </c>
       <c r="AH16" s="56">
-        <v>5870</v>
+        <v>4402</v>
       </c>
       <c r="AI16" s="56">
-        <v>6268</v>
+        <v>4701</v>
       </c>
     </row>
     <row r="17" spans="1:35">
@@ -5304,6 +5880,15 @@
       <c r="O17" s="59">
         <v>11</v>
       </c>
+      <c r="P17">
+        <v>2.5100000000000001E-3</v>
+      </c>
+      <c r="Q17">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R17">
+        <v>4.2199999999999998E-3</v>
+      </c>
       <c r="S17" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -5313,9 +5898,15 @@
       <c r="U17" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V17" s="56"/>
-      <c r="W17" s="56"/>
-      <c r="X17" s="56"/>
+      <c r="V17" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W17" s="56">
+        <v>3.9199999999999999E-3</v>
+      </c>
+      <c r="X17" s="56">
+        <v>3.9199999999999999E-3</v>
+      </c>
       <c r="Y17" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -5335,19 +5926,19 @@
         <v>215.01599999999999</v>
       </c>
       <c r="AE17" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF17" s="56">
-        <v>1420</v>
+        <v>1242</v>
       </c>
       <c r="AG17" s="56">
-        <v>4890</v>
+        <v>3730</v>
       </c>
       <c r="AH17" s="56">
-        <v>5880</v>
+        <v>4410</v>
       </c>
       <c r="AI17" s="56">
-        <v>6278</v>
+        <v>4708</v>
       </c>
     </row>
     <row r="18" spans="1:35">
@@ -5396,6 +5987,15 @@
       <c r="O18" s="59">
         <v>11</v>
       </c>
+      <c r="P18">
+        <v>2.6099999999999999E-3</v>
+      </c>
+      <c r="Q18">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R18">
+        <v>4.4000000000000003E-3</v>
+      </c>
       <c r="S18" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -5405,9 +6005,15 @@
       <c r="U18" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V18" s="56"/>
-      <c r="W18" s="56"/>
-      <c r="X18" s="56"/>
+      <c r="V18" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W18" s="56">
+        <v>4.0800000000000003E-3</v>
+      </c>
+      <c r="X18" s="56">
+        <v>4.0800000000000003E-3</v>
+      </c>
       <c r="Y18" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -5427,19 +6033,19 @@
         <v>215.01599999999999</v>
       </c>
       <c r="AE18" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF18" s="56">
-        <v>1665</v>
+        <v>1477</v>
       </c>
       <c r="AG18" s="56">
-        <v>6391</v>
+        <v>4793</v>
       </c>
       <c r="AH18" s="56">
-        <v>6768</v>
+        <v>5076</v>
       </c>
       <c r="AI18" s="56">
-        <v>7167</v>
+        <v>5375</v>
       </c>
     </row>
     <row r="19" spans="1:35">
@@ -5488,6 +6094,15 @@
       <c r="O19" s="59">
         <v>11</v>
       </c>
+      <c r="P19">
+        <v>2.5899999999999999E-3</v>
+      </c>
+      <c r="Q19">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R19">
+        <v>4.3499999999999997E-3</v>
+      </c>
       <c r="S19" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -5497,9 +6112,15 @@
       <c r="U19" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V19" s="56"/>
-      <c r="W19" s="56"/>
-      <c r="X19" s="56"/>
+      <c r="V19" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W19" s="56">
+        <v>4.0400000000000002E-3</v>
+      </c>
+      <c r="X19" s="56">
+        <v>4.0400000000000002E-3</v>
+      </c>
       <c r="Y19" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -5519,19 +6140,19 @@
         <v>215.01599999999999</v>
       </c>
       <c r="AE19" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF19" s="56">
-        <v>1452</v>
+        <v>1273</v>
       </c>
       <c r="AG19" s="56">
-        <v>5150</v>
+        <v>3911</v>
       </c>
       <c r="AH19" s="56">
-        <v>5999</v>
+        <v>4499</v>
       </c>
       <c r="AI19" s="56">
-        <v>6397</v>
+        <v>4798</v>
       </c>
     </row>
     <row r="20" spans="1:35">
@@ -5580,6 +6201,15 @@
       <c r="O20" s="59">
         <v>11</v>
       </c>
+      <c r="P20">
+        <v>2.5600000000000002E-3</v>
+      </c>
+      <c r="Q20">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R20">
+        <v>4.3099999999999996E-3</v>
+      </c>
       <c r="S20" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -5589,9 +6219,15 @@
       <c r="U20" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V20" s="56"/>
-      <c r="W20" s="56"/>
-      <c r="X20" s="56"/>
+      <c r="V20" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W20" s="56">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="X20" s="56">
+        <v>4.0000000000000001E-3</v>
+      </c>
       <c r="Y20" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -5611,19 +6247,19 @@
         <v>215.01599999999999</v>
       </c>
       <c r="AE20" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF20" s="56">
-        <v>1417</v>
+        <v>1240</v>
       </c>
       <c r="AG20" s="56">
-        <v>4869</v>
+        <v>3715</v>
       </c>
       <c r="AH20" s="56">
-        <v>5870</v>
+        <v>4402</v>
       </c>
       <c r="AI20" s="56">
-        <v>6268</v>
+        <v>4701</v>
       </c>
     </row>
     <row r="21" spans="1:35">
@@ -5672,6 +6308,15 @@
       <c r="O21" s="59">
         <v>11</v>
       </c>
+      <c r="P21">
+        <v>2.5300000000000001E-3</v>
+      </c>
+      <c r="Q21">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R21">
+        <v>4.2599999999999999E-3</v>
+      </c>
       <c r="S21" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -5681,9 +6326,15 @@
       <c r="U21" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V21" s="56"/>
-      <c r="W21" s="56"/>
-      <c r="X21" s="56"/>
+      <c r="V21" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W21" s="56">
+        <v>3.96E-3</v>
+      </c>
+      <c r="X21" s="56">
+        <v>3.96E-3</v>
+      </c>
       <c r="Y21" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -5703,19 +6354,19 @@
         <v>215.01599999999999</v>
       </c>
       <c r="AE21" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF21" s="56">
-        <v>1417</v>
+        <v>1240</v>
       </c>
       <c r="AG21" s="56">
-        <v>4869</v>
+        <v>3715</v>
       </c>
       <c r="AH21" s="56">
-        <v>5870</v>
+        <v>4402</v>
       </c>
       <c r="AI21" s="56">
-        <v>6268</v>
+        <v>4701</v>
       </c>
     </row>
     <row r="22" spans="1:35">
@@ -5764,6 +6415,15 @@
       <c r="O22" s="59">
         <v>11</v>
       </c>
+      <c r="P22">
+        <v>2.5100000000000001E-3</v>
+      </c>
+      <c r="Q22">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R22">
+        <v>4.2199999999999998E-3</v>
+      </c>
       <c r="S22" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -5773,9 +6433,15 @@
       <c r="U22" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V22" s="56"/>
-      <c r="W22" s="56"/>
-      <c r="X22" s="56"/>
+      <c r="V22" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W22" s="56">
+        <v>3.9199999999999999E-3</v>
+      </c>
+      <c r="X22" s="56">
+        <v>3.9199999999999999E-3</v>
+      </c>
       <c r="Y22" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -5795,19 +6461,19 @@
         <v>215.01599999999999</v>
       </c>
       <c r="AE22" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF22" s="56">
-        <v>1420</v>
+        <v>1242</v>
       </c>
       <c r="AG22" s="56">
-        <v>4890</v>
+        <v>3730</v>
       </c>
       <c r="AH22" s="56">
-        <v>5880</v>
+        <v>4410</v>
       </c>
       <c r="AI22" s="56">
-        <v>6278</v>
+        <v>4708</v>
       </c>
     </row>
     <row r="23" spans="1:35">
@@ -5856,6 +6522,15 @@
       <c r="O23" s="59">
         <v>11</v>
       </c>
+      <c r="P23">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="Q23">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R23">
+        <v>3.9500000000000004E-3</v>
+      </c>
       <c r="S23" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -5865,9 +6540,15 @@
       <c r="U23" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V23" s="56"/>
-      <c r="W23" s="56"/>
-      <c r="X23" s="56"/>
+      <c r="V23" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W23" s="56">
+        <v>3.6700000000000001E-3</v>
+      </c>
+      <c r="X23" s="56">
+        <v>3.6700000000000001E-3</v>
+      </c>
       <c r="Y23" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -5887,19 +6568,19 @@
         <v>229.46600000000001</v>
       </c>
       <c r="AE23" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF23" s="56">
-        <v>1373</v>
+        <v>1205</v>
       </c>
       <c r="AG23" s="56">
-        <v>4926</v>
+        <v>3734</v>
       </c>
       <c r="AH23" s="56">
-        <v>5667</v>
+        <v>4250</v>
       </c>
       <c r="AI23" s="56">
-        <v>6040</v>
+        <v>4530</v>
       </c>
     </row>
     <row r="24" spans="1:35">
@@ -5948,6 +6629,15 @@
       <c r="O24" s="59">
         <v>11</v>
       </c>
+      <c r="P24">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="Q24">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R24">
+        <v>3.9100000000000003E-3</v>
+      </c>
       <c r="S24" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -5957,9 +6647,15 @@
       <c r="U24" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V24" s="56"/>
-      <c r="W24" s="56"/>
-      <c r="X24" s="56"/>
+      <c r="V24" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W24" s="56">
+        <v>3.63E-3</v>
+      </c>
+      <c r="X24" s="56">
+        <v>3.63E-3</v>
+      </c>
       <c r="Y24" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -5979,19 +6675,19 @@
         <v>229.46600000000001</v>
       </c>
       <c r="AE24" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF24" s="56">
-        <v>1213</v>
+        <v>1053</v>
       </c>
       <c r="AG24" s="56">
-        <v>3549</v>
+        <v>2774</v>
       </c>
       <c r="AH24" s="56">
-        <v>5019</v>
+        <v>3771</v>
       </c>
       <c r="AI24" s="56">
-        <v>5438</v>
+        <v>4079</v>
       </c>
     </row>
     <row r="25" spans="1:35">
@@ -6040,6 +6736,15 @@
       <c r="O25" s="59">
         <v>11</v>
       </c>
+      <c r="P25">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="Q25">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R25">
+        <v>3.8700000000000002E-3</v>
+      </c>
       <c r="S25" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -6049,9 +6754,15 @@
       <c r="U25" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V25" s="56"/>
-      <c r="W25" s="56"/>
-      <c r="X25" s="56"/>
+      <c r="V25" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W25" s="56">
+        <v>3.5899999999999999E-3</v>
+      </c>
+      <c r="X25" s="56">
+        <v>3.5899999999999999E-3</v>
+      </c>
       <c r="Y25" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -6071,19 +6782,19 @@
         <v>229.46600000000001</v>
       </c>
       <c r="AE25" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF25" s="56">
-        <v>1213</v>
+        <v>1053</v>
       </c>
       <c r="AG25" s="56">
-        <v>3549</v>
+        <v>2774</v>
       </c>
       <c r="AH25" s="56">
-        <v>5019</v>
+        <v>3771</v>
       </c>
       <c r="AI25" s="56">
-        <v>5438</v>
+        <v>4079</v>
       </c>
     </row>
     <row r="26" spans="1:35">
@@ -6132,6 +6843,15 @@
       <c r="O26" s="59">
         <v>11</v>
       </c>
+      <c r="P26">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="Q26">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R26">
+        <v>3.8300000000000001E-3</v>
+      </c>
       <c r="S26" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -6141,9 +6861,15 @@
       <c r="U26" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V26" s="56"/>
-      <c r="W26" s="56"/>
-      <c r="X26" s="56"/>
+      <c r="V26" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W26" s="56">
+        <v>3.5500000000000002E-3</v>
+      </c>
+      <c r="X26" s="56">
+        <v>3.5500000000000002E-3</v>
+      </c>
       <c r="Y26" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -6163,19 +6889,19 @@
         <v>229.46600000000001</v>
       </c>
       <c r="AE26" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF26" s="56">
-        <v>1211</v>
+        <v>1051</v>
       </c>
       <c r="AG26" s="56">
-        <v>3528</v>
+        <v>2760</v>
       </c>
       <c r="AH26" s="56">
-        <v>5003</v>
+        <v>3760</v>
       </c>
       <c r="AI26" s="56">
-        <v>5430</v>
+        <v>4072</v>
       </c>
     </row>
     <row r="27" spans="1:35">
@@ -6224,6 +6950,15 @@
       <c r="O27" s="59">
         <v>11</v>
       </c>
+      <c r="P27">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="Q27">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R27">
+        <v>3.79E-3</v>
+      </c>
       <c r="S27" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -6233,9 +6968,15 @@
       <c r="U27" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V27" s="56"/>
-      <c r="W27" s="56"/>
-      <c r="X27" s="56"/>
+      <c r="V27" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W27" s="56">
+        <v>3.5200000000000001E-3</v>
+      </c>
+      <c r="X27" s="56">
+        <v>3.5200000000000001E-3</v>
+      </c>
       <c r="Y27" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -6255,19 +6996,19 @@
         <v>229.46600000000001</v>
       </c>
       <c r="AE27" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF27" s="56">
-        <v>1211</v>
+        <v>1051</v>
       </c>
       <c r="AG27" s="56">
-        <v>3528</v>
+        <v>2760</v>
       </c>
       <c r="AH27" s="56">
-        <v>5003</v>
+        <v>3760</v>
       </c>
       <c r="AI27" s="56">
-        <v>5430</v>
+        <v>4072</v>
       </c>
     </row>
     <row r="28" spans="1:35">
@@ -6316,6 +7057,15 @@
       <c r="O28" s="59">
         <v>11</v>
       </c>
+      <c r="P28">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="Q28">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R28">
+        <v>3.5799999999999998E-3</v>
+      </c>
       <c r="S28" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -6325,9 +7075,15 @@
       <c r="U28" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V28" s="56"/>
-      <c r="W28" s="56"/>
-      <c r="X28" s="56"/>
+      <c r="V28" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W28" s="56">
+        <v>3.32E-3</v>
+      </c>
+      <c r="X28" s="56">
+        <v>3.32E-3</v>
+      </c>
       <c r="Y28" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -6347,19 +7103,19 @@
         <v>243.916</v>
       </c>
       <c r="AE28" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF28" s="56">
-        <v>1183</v>
+        <v>1030</v>
       </c>
       <c r="AG28" s="56">
-        <v>3720</v>
+        <v>2876</v>
       </c>
       <c r="AH28" s="56">
-        <v>4925</v>
+        <v>3694</v>
       </c>
       <c r="AI28" s="56">
-        <v>5275</v>
+        <v>3956</v>
       </c>
     </row>
     <row r="29" spans="1:35">
@@ -6408,6 +7164,15 @@
       <c r="O29" s="59">
         <v>11</v>
       </c>
+      <c r="P29">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="Q29">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R29">
+        <v>3.5400000000000002E-3</v>
+      </c>
       <c r="S29" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -6417,9 +7182,15 @@
       <c r="U29" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V29" s="56"/>
-      <c r="W29" s="56"/>
-      <c r="X29" s="56"/>
+      <c r="V29" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W29" s="56">
+        <v>3.29E-3</v>
+      </c>
+      <c r="X29" s="56">
+        <v>3.29E-3</v>
+      </c>
       <c r="Y29" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -6439,19 +7210,19 @@
         <v>243.916</v>
       </c>
       <c r="AE29" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF29" s="56">
-        <v>1043</v>
+        <v>898</v>
       </c>
       <c r="AG29" s="56">
-        <v>2328</v>
+        <v>1905</v>
       </c>
       <c r="AH29" s="56">
-        <v>3911</v>
+        <v>3002</v>
       </c>
       <c r="AI29" s="56">
-        <v>4730</v>
+        <v>3548</v>
       </c>
     </row>
     <row r="30" spans="1:35">
@@ -6500,6 +7271,15 @@
       <c r="O30" s="59">
         <v>11</v>
       </c>
+      <c r="P30">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="Q30">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R30">
+        <v>3.5000000000000001E-3</v>
+      </c>
       <c r="S30" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -6509,9 +7289,15 @@
       <c r="U30" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V30" s="56"/>
-      <c r="W30" s="56"/>
-      <c r="X30" s="56"/>
+      <c r="V30" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W30" s="56">
+        <v>3.2499999999999999E-3</v>
+      </c>
+      <c r="X30" s="56">
+        <v>3.2499999999999999E-3</v>
+      </c>
       <c r="Y30" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -6531,19 +7317,19 @@
         <v>243.916</v>
       </c>
       <c r="AE30" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF30" s="56">
-        <v>1043</v>
+        <v>898</v>
       </c>
       <c r="AG30" s="56">
-        <v>2328</v>
+        <v>1905</v>
       </c>
       <c r="AH30" s="56">
-        <v>3911</v>
+        <v>3002</v>
       </c>
       <c r="AI30" s="56">
-        <v>4730</v>
+        <v>3548</v>
       </c>
     </row>
     <row r="31" spans="1:35">
@@ -6592,6 +7378,15 @@
       <c r="O31" s="59">
         <v>11</v>
       </c>
+      <c r="P31">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="Q31">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R31">
+        <v>3.47E-3</v>
+      </c>
       <c r="S31" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -6601,9 +7396,15 @@
       <c r="U31" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V31" s="56"/>
-      <c r="W31" s="56"/>
-      <c r="X31" s="56"/>
+      <c r="V31" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W31" s="56">
+        <v>3.2200000000000002E-3</v>
+      </c>
+      <c r="X31" s="56">
+        <v>3.2200000000000002E-3</v>
+      </c>
       <c r="Y31" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -6623,19 +7424,19 @@
         <v>243.916</v>
       </c>
       <c r="AE31" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF31" s="56">
-        <v>1041</v>
+        <v>896</v>
       </c>
       <c r="AG31" s="56">
-        <v>2309</v>
+        <v>1892</v>
       </c>
       <c r="AH31" s="56">
-        <v>3895</v>
+        <v>2991</v>
       </c>
       <c r="AI31" s="56">
-        <v>4723</v>
+        <v>3542</v>
       </c>
     </row>
     <row r="32" spans="1:35">
@@ -6684,6 +7485,15 @@
       <c r="O32" s="59">
         <v>11</v>
       </c>
+      <c r="P32">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="Q32">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R32">
+        <v>3.4299999999999999E-3</v>
+      </c>
       <c r="S32" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -6693,9 +7503,15 @@
       <c r="U32" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V32" s="56"/>
-      <c r="W32" s="56"/>
-      <c r="X32" s="56"/>
+      <c r="V32" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W32" s="56">
+        <v>3.1900000000000001E-3</v>
+      </c>
+      <c r="X32" s="56">
+        <v>3.1900000000000001E-3</v>
+      </c>
       <c r="Y32" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -6715,19 +7531,19 @@
         <v>243.916</v>
       </c>
       <c r="AE32" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF32" s="56">
-        <v>1041</v>
+        <v>896</v>
       </c>
       <c r="AG32" s="56">
-        <v>2309</v>
+        <v>1892</v>
       </c>
       <c r="AH32" s="56">
-        <v>3895</v>
+        <v>2991</v>
       </c>
       <c r="AI32" s="56">
-        <v>4723</v>
+        <v>3542</v>
       </c>
     </row>
     <row r="33" spans="1:35">
@@ -6776,6 +7592,15 @@
       <c r="O33" s="59">
         <v>11</v>
       </c>
+      <c r="P33">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="Q33">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R33">
+        <v>3.2699999999999999E-3</v>
+      </c>
       <c r="S33" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -6785,9 +7610,15 @@
       <c r="U33" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V33" s="56"/>
-      <c r="W33" s="56"/>
-      <c r="X33" s="56"/>
+      <c r="V33" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W33" s="56">
+        <v>3.0300000000000001E-3</v>
+      </c>
+      <c r="X33" s="56">
+        <v>3.0300000000000001E-3</v>
+      </c>
       <c r="Y33" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -6807,19 +7638,19 @@
         <v>258.36599999999999</v>
       </c>
       <c r="AE33" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF33" s="56">
-        <v>1025</v>
+        <v>886</v>
       </c>
       <c r="AG33" s="56">
-        <v>2630</v>
+        <v>2099</v>
       </c>
       <c r="AH33" s="56">
-        <v>4038</v>
+        <v>3067</v>
       </c>
       <c r="AI33" s="56">
-        <v>4625</v>
+        <v>3469</v>
       </c>
     </row>
     <row r="34" spans="1:35">
@@ -6868,6 +7699,15 @@
       <c r="O34" s="59">
         <v>11</v>
       </c>
+      <c r="P34">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="Q34">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R34">
+        <v>3.2299999999999998E-3</v>
+      </c>
       <c r="S34" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -6877,9 +7717,15 @@
       <c r="U34" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V34" s="56"/>
-      <c r="W34" s="56"/>
-      <c r="X34" s="56"/>
+      <c r="V34" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W34" s="56">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="X34" s="56">
+        <v>3.0000000000000001E-3</v>
+      </c>
       <c r="Y34" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -6899,19 +7745,19 @@
         <v>258.36599999999999</v>
       </c>
       <c r="AE34" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF34" s="56">
-        <v>902</v>
+        <v>770</v>
       </c>
       <c r="AG34" s="56">
-        <v>1433</v>
+        <v>1257</v>
       </c>
       <c r="AH34" s="56">
-        <v>2911</v>
+        <v>2306</v>
       </c>
       <c r="AI34" s="56">
-        <v>4055</v>
+        <v>3056</v>
       </c>
     </row>
     <row r="35" spans="1:35">
@@ -6960,6 +7806,15 @@
       <c r="O35" s="59">
         <v>11</v>
       </c>
+      <c r="P35">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="Q35">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R35">
+        <v>3.2000000000000002E-3</v>
+      </c>
       <c r="S35" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -6969,9 +7824,15 @@
       <c r="U35" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V35" s="56"/>
-      <c r="W35" s="56"/>
-      <c r="X35" s="56"/>
+      <c r="V35" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W35" s="56">
+        <v>2.97E-3</v>
+      </c>
+      <c r="X35" s="56">
+        <v>2.97E-3</v>
+      </c>
       <c r="Y35" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -6991,19 +7852,19 @@
         <v>258.36599999999999</v>
       </c>
       <c r="AE35" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF35" s="56">
-        <v>900</v>
+        <v>769</v>
       </c>
       <c r="AG35" s="56">
-        <v>1431</v>
+        <v>1255</v>
       </c>
       <c r="AH35" s="56">
-        <v>2897</v>
+        <v>2296</v>
       </c>
       <c r="AI35" s="56">
-        <v>4043</v>
+        <v>3049</v>
       </c>
     </row>
     <row r="36" spans="1:35">
@@ -7052,6 +7913,15 @@
       <c r="O36" s="59">
         <v>11</v>
       </c>
+      <c r="P36">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="Q36">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R36">
+        <v>3.1700000000000001E-3</v>
+      </c>
       <c r="S36" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -7061,9 +7931,15 @@
       <c r="U36" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V36" s="56"/>
-      <c r="W36" s="56"/>
-      <c r="X36" s="56"/>
+      <c r="V36" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W36" s="56">
+        <v>2.9399999999999999E-3</v>
+      </c>
+      <c r="X36" s="56">
+        <v>2.9399999999999999E-3</v>
+      </c>
       <c r="Y36" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -7083,19 +7959,19 @@
         <v>258.36599999999999</v>
       </c>
       <c r="AE36" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF36" s="56">
-        <v>899</v>
+        <v>768</v>
       </c>
       <c r="AG36" s="56">
-        <v>1428</v>
+        <v>1253</v>
       </c>
       <c r="AH36" s="56">
-        <v>2882</v>
+        <v>2287</v>
       </c>
       <c r="AI36" s="56">
-        <v>4031</v>
+        <v>3041</v>
       </c>
     </row>
     <row r="37" spans="1:35">
@@ -7144,6 +8020,15 @@
       <c r="O37" s="59">
         <v>11</v>
       </c>
+      <c r="P37">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="Q37">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R37">
+        <v>3.13E-3</v>
+      </c>
       <c r="S37" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -7153,9 +8038,15 @@
       <c r="U37" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V37" s="56"/>
-      <c r="W37" s="56"/>
-      <c r="X37" s="56"/>
+      <c r="V37" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W37" s="56">
+        <v>2.9099999999999998E-3</v>
+      </c>
+      <c r="X37" s="56">
+        <v>2.9099999999999998E-3</v>
+      </c>
       <c r="Y37" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -7175,19 +8066,19 @@
         <v>258.36599999999999</v>
       </c>
       <c r="AE37" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF37" s="56">
-        <v>897</v>
+        <v>766</v>
       </c>
       <c r="AG37" s="56">
-        <v>1426</v>
+        <v>1251</v>
       </c>
       <c r="AH37" s="56">
-        <v>2868</v>
+        <v>2277</v>
       </c>
       <c r="AI37" s="56">
-        <v>4019</v>
+        <v>3033</v>
       </c>
     </row>
     <row r="38" spans="1:35">
@@ -7236,6 +8127,15 @@
       <c r="O38" s="59">
         <v>11</v>
       </c>
+      <c r="P38">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="Q38">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R38">
+        <v>3.0000000000000001E-3</v>
+      </c>
       <c r="S38" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -7245,9 +8145,15 @@
       <c r="U38" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V38" s="56"/>
-      <c r="W38" s="56"/>
-      <c r="X38" s="56"/>
+      <c r="V38" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W38" s="56">
+        <v>2.7899999999999999E-3</v>
+      </c>
+      <c r="X38" s="56">
+        <v>2.7899999999999999E-3</v>
+      </c>
       <c r="Y38" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -7267,19 +8173,19 @@
         <v>272.81599999999997</v>
       </c>
       <c r="AE38" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF38" s="56">
-        <v>890</v>
+        <v>764</v>
       </c>
       <c r="AG38" s="56">
-        <v>1605</v>
+        <v>1371</v>
       </c>
       <c r="AH38" s="56">
-        <v>3113</v>
+        <v>2425</v>
       </c>
       <c r="AI38" s="56">
-        <v>4061</v>
+        <v>3046</v>
       </c>
     </row>
     <row r="39" spans="1:35">
@@ -7328,6 +8234,15 @@
       <c r="O39" s="59">
         <v>11</v>
       </c>
+      <c r="P39">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="Q39">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R39">
+        <v>2.97E-3</v>
+      </c>
       <c r="S39" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -7337,9 +8252,15 @@
       <c r="U39" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V39" s="56"/>
-      <c r="W39" s="56"/>
-      <c r="X39" s="56"/>
+      <c r="V39" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W39" s="56">
+        <v>2.7599999999999999E-3</v>
+      </c>
+      <c r="X39" s="56">
+        <v>2.7599999999999999E-3</v>
+      </c>
       <c r="Y39" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -7359,19 +8280,19 @@
         <v>272.81599999999997</v>
       </c>
       <c r="AE39" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF39" s="56">
-        <v>781</v>
+        <v>662</v>
       </c>
       <c r="AG39" s="56">
-        <v>1248</v>
+        <v>1087</v>
       </c>
       <c r="AH39" s="56">
-        <v>1963</v>
+        <v>1649</v>
       </c>
       <c r="AI39" s="56">
-        <v>3189</v>
+        <v>2474</v>
       </c>
     </row>
     <row r="40" spans="1:35">
@@ -7420,6 +8341,15 @@
       <c r="O40" s="59">
         <v>11</v>
       </c>
+      <c r="P40">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="Q40">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R40">
+        <v>2.9399999999999999E-3</v>
+      </c>
       <c r="S40" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -7429,9 +8359,15 @@
       <c r="U40" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V40" s="56"/>
-      <c r="W40" s="56"/>
-      <c r="X40" s="56"/>
+      <c r="V40" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W40" s="56">
+        <v>2.7299999999999998E-3</v>
+      </c>
+      <c r="X40" s="56">
+        <v>2.7299999999999998E-3</v>
+      </c>
       <c r="Y40" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -7451,19 +8387,19 @@
         <v>272.81599999999997</v>
       </c>
       <c r="AE40" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF40" s="56">
-        <v>778</v>
+        <v>660</v>
       </c>
       <c r="AG40" s="56">
-        <v>1245</v>
+        <v>1084</v>
       </c>
       <c r="AH40" s="56">
-        <v>1936</v>
+        <v>1630</v>
       </c>
       <c r="AI40" s="56">
-        <v>3166</v>
+        <v>2460</v>
       </c>
     </row>
     <row r="41" spans="1:35">
@@ -7512,6 +8448,15 @@
       <c r="O41" s="59">
         <v>11</v>
       </c>
+      <c r="P41">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="Q41">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R41">
+        <v>2.9099999999999998E-3</v>
+      </c>
       <c r="S41" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -7521,9 +8466,15 @@
       <c r="U41" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V41" s="56"/>
-      <c r="W41" s="56"/>
-      <c r="X41" s="56"/>
+      <c r="V41" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W41" s="56">
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="X41" s="56">
+        <v>2.7000000000000001E-3</v>
+      </c>
       <c r="Y41" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -7543,19 +8494,19 @@
         <v>272.81599999999997</v>
       </c>
       <c r="AE41" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF41" s="56">
-        <v>777</v>
+        <v>659</v>
       </c>
       <c r="AG41" s="56">
-        <v>1243</v>
+        <v>1082</v>
       </c>
       <c r="AH41" s="56">
-        <v>1922</v>
+        <v>1621</v>
       </c>
       <c r="AI41" s="56">
-        <v>3155</v>
+        <v>2452</v>
       </c>
     </row>
     <row r="42" spans="1:35">
@@ -7604,6 +8555,15 @@
       <c r="O42" s="59">
         <v>11</v>
       </c>
+      <c r="P42">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="Q42">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R42">
+        <v>2.8800000000000002E-3</v>
+      </c>
       <c r="S42" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -7613,9 +8573,15 @@
       <c r="U42" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="V42" s="56"/>
-      <c r="W42" s="56"/>
-      <c r="X42" s="56"/>
+      <c r="V42" s="56">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="W42" s="56">
+        <v>2.6700000000000001E-3</v>
+      </c>
+      <c r="X42" s="56">
+        <v>2.6700000000000001E-3</v>
+      </c>
       <c r="Y42" s="56">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -7635,19 +8601,19 @@
         <v>272.81599999999997</v>
       </c>
       <c r="AE42" s="56">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="AF42" s="56">
-        <v>775</v>
+        <v>656</v>
       </c>
       <c r="AG42" s="56">
-        <v>1239</v>
+        <v>1079</v>
       </c>
       <c r="AH42" s="56">
-        <v>1895</v>
+        <v>1603</v>
       </c>
       <c r="AI42" s="56">
-        <v>3133</v>
+        <v>2438</v>
       </c>
     </row>
   </sheetData>
@@ -7661,306 +8627,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="13.140625" style="8" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="52" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="18" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B3" s="4">
-        <f>f_n</f>
-        <v>7.9328615571404866</v>
-      </c>
-      <c r="C3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B4" s="6">
-        <f>Slab_Properties!B127</f>
-        <v>74875</v>
-      </c>
-      <c r="C4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="B5">
-        <f>Slab_Properties!B128</f>
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="11"/>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="52" t="s">
-        <v>147</v>
-      </c>
-      <c r="H7" s="56" t="s">
-        <v>148</v>
-      </c>
-      <c r="I7" s="56" t="s">
-        <v>149</v>
-      </c>
-      <c r="J7" s="56" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="18" customHeight="1">
-      <c r="A8" s="56" t="s">
-        <v>151</v>
-      </c>
-      <c r="B8" s="56" t="s">
-        <v>126</v>
-      </c>
-      <c r="C8" s="56" t="s">
-        <v>152</v>
-      </c>
-      <c r="D8" s="56" t="s">
-        <v>153</v>
-      </c>
-      <c r="E8" s="56" t="s">
-        <v>154</v>
-      </c>
-      <c r="F8" s="56" t="s">
-        <v>155</v>
-      </c>
-      <c r="G8" s="57" t="s">
-        <v>156</v>
-      </c>
-      <c r="H8" s="56" t="s">
-        <v>157</v>
-      </c>
-      <c r="I8" s="56" t="s">
-        <v>158</v>
-      </c>
-      <c r="J8" s="56" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="56"/>
-      <c r="B9" s="56" t="s">
-        <v>107</v>
-      </c>
-      <c r="C9" s="56" t="s">
-        <v>107</v>
-      </c>
-      <c r="D9" s="56" t="s">
-        <v>107</v>
-      </c>
-      <c r="E9" s="56" t="s">
-        <v>107</v>
-      </c>
-      <c r="F9" s="56" t="s">
-        <v>107</v>
-      </c>
-      <c r="G9" s="57"/>
-      <c r="H9" s="56" t="s">
-        <v>143</v>
-      </c>
-      <c r="I9" s="56" t="s">
-        <v>143</v>
-      </c>
-      <c r="J9" s="56" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="56" t="s">
-        <v>129</v>
-      </c>
-      <c r="B10" s="10">
-        <f>$B$3</f>
-        <v>7.9328615571404866</v>
-      </c>
-      <c r="C10" s="56">
-        <v>1.25</v>
-      </c>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7">
-        <f>250000000/($B$4*$B$5)*($C10^2.43/$B10^1.8)*(1-EXP(-2*PI()*$B$5*$B10/$C10))</f>
-        <v>3211.0837356966122</v>
-      </c>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7">
-        <f>I10</f>
-        <v>3211.0837356966122</v>
-      </c>
-      <c r="L10" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="56" t="s">
-        <v>130</v>
-      </c>
-      <c r="B11" s="10">
-        <f>$B$3</f>
-        <v>7.9328615571404866</v>
-      </c>
-      <c r="C11" s="56">
-        <v>1.6</v>
-      </c>
-      <c r="D11" s="56">
-        <v>6.8</v>
-      </c>
-      <c r="E11" s="56">
-        <v>6</v>
-      </c>
-      <c r="F11" s="56">
-        <v>8</v>
-      </c>
-      <c r="G11" s="56">
-        <v>0.1</v>
-      </c>
-      <c r="H11" s="7">
-        <f>175000000/($B$4*$B$5*SQRT($B11))*(EXP(-$G11*$B11))</f>
-        <v>12512.532571651907</v>
-      </c>
-      <c r="I11" s="7">
-        <f>250000000/($B$4*$B$5)*($C11^2.43/$B11^1.8)*(1-EXP(-2*PI()*$B$5*$B11/$C11))</f>
-        <v>5091.9409379106901</v>
-      </c>
-      <c r="J11" s="7">
-        <f>IF(AND($B11&gt;$E11,$B11&lt;$F11),$H11+($I11-$H11)/($F11-$E11)*($B11-$E11)/($F11-$E11), "N/A")</f>
-        <v>8926.7884966277288</v>
-      </c>
-      <c r="K11" s="7">
-        <f>IF($B11&gt;=F11,I11, IF($B11&lt;=E11,H11,J11))</f>
-        <v>8926.7884966277288</v>
-      </c>
-      <c r="L11" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="56" t="s">
-        <v>131</v>
-      </c>
-      <c r="B12" s="10">
-        <f>$B$3</f>
-        <v>7.9328615571404866</v>
-      </c>
-      <c r="C12" s="56">
-        <v>1.85</v>
-      </c>
-      <c r="D12" s="56">
-        <v>8</v>
-      </c>
-      <c r="E12" s="56">
-        <v>7</v>
-      </c>
-      <c r="F12" s="56">
-        <v>9</v>
-      </c>
-      <c r="G12" s="56">
-        <v>0.09</v>
-      </c>
-      <c r="H12" s="7">
-        <f>175000000/($B$4*$B$5*SQRT($B12))*(EXP(-$G12*$B12))</f>
-        <v>13545.567382152003</v>
-      </c>
-      <c r="I12" s="7">
-        <f>250000000/($B$4*$B$5)*($C12^2.43/$B12^1.8)*(1-EXP(-2*PI()*$B$5*$B12/$C12))</f>
-        <v>6615.128613505025</v>
-      </c>
-      <c r="J12" s="7">
-        <f>IF(AND($B12&gt;$E12,$B12&lt;$F12),$H12+($I12-$H12)/($F12-$E12)*($B12-$E12)/($F12-$E12), "N/A")</f>
-        <v>11929.2824068053</v>
-      </c>
-      <c r="K12" s="7">
-        <f>IF($B12&gt;=F12,I12, IF($B12&lt;=E12,H12,J12))</f>
-        <v>11929.2824068053</v>
-      </c>
-      <c r="L12" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="56" t="s">
-        <v>132</v>
-      </c>
-      <c r="B13" s="10">
-        <f>$B$3</f>
-        <v>7.9328615571404866</v>
-      </c>
-      <c r="C13" s="56">
-        <v>2.1</v>
-      </c>
-      <c r="D13" s="56">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="E13" s="56">
-        <v>8</v>
-      </c>
-      <c r="F13" s="56">
-        <v>10</v>
-      </c>
-      <c r="G13" s="56">
-        <v>0.08</v>
-      </c>
-      <c r="H13" s="7">
-        <f>175000000/($B$4*$B$5*SQRT($B13))*(EXP(-$G13*$B13))</f>
-        <v>14663.889556628494</v>
-      </c>
-      <c r="I13" s="7">
-        <f>250000000/($B$4*$B$5)*($C13^2.43/$B13^1.8)*(1-EXP(-2*PI()*$B$5*$B13/$C13))</f>
-        <v>8270.4463690391931</v>
-      </c>
-      <c r="J13" s="7" t="str">
-        <f>IF(AND($B13&gt;$E13,$B13&lt;$F13),$H13+($I13-$H13)/($F13-$E13)*($B13-$E13)/($F13-$E13), "N/A")</f>
-        <v>N/A</v>
-      </c>
-      <c r="K13" s="7">
-        <f>IF($B13&gt;=F13,I13, IF($B13&lt;=E13,H13,J13))</f>
-        <v>14663.889556628494</v>
-      </c>
-      <c r="L13" t="s">
-        <v>143</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:Q128"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G130" sqref="G130"/>
+    <sheetView topLeftCell="A100" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O126" sqref="O126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
improved plotting, added damping studies
</commit_message>
<xml_diff>
--- a/Flat_Plate_Vibration_Template.xlsx
+++ b/Flat_Plate_Vibration_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mwachter\workspaces\vibraslab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D3492F-BD9D-4D3B-841E-548169A3D806}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41ADD1EB-B9E9-4EDF-AB85-A75FD11E60A8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="6480" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="6480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Slab_Properties" sheetId="1" r:id="rId1"/>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="173">
   <si>
     <t>Slab properties:</t>
   </si>
@@ -611,14 +611,45 @@
   </si>
   <si>
     <t>* does not consider mode scaling</t>
+  </si>
+  <si>
+    <t>* must be &lt; 2.0, otherwise exhibits one way behavior</t>
+  </si>
+  <si>
+    <t>*single layer of reinforcement</t>
+  </si>
+  <si>
+    <t>*lightweight concrete factor, ACI 318-14, 19.2.4.2</t>
+  </si>
+  <si>
+    <t>* reduced modulus of rupture, per CRSI Design Guide p4-6</t>
+  </si>
+  <si>
+    <t>References:</t>
+  </si>
+  <si>
+    <t>CRSI Design Guide for Vibration of Reinforced Concrete Floor Systems, First Edition</t>
+  </si>
+  <si>
+    <t>ACI 318-14 Building Code Requirements for Structural Concrete</t>
+  </si>
+  <si>
+    <t>AISC Steel Design Guide 11: Vibration of Steel-Framed Structural Systems Due to Human Activity</t>
+  </si>
+  <si>
+    <t>Velocity</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -921,7 +952,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1072,6 +1103,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="167" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1395,10 +1431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:Q128"/>
+  <dimension ref="A1:Q128"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B122" sqref="B122"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1412,7 +1448,12 @@
     <col min="10" max="13" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5">
+    <row r="1" spans="1:9">
+      <c r="I1" s="8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="52" t="s">
         <v>0</v>
       </c>
@@ -1420,7 +1461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18" customHeight="1">
+    <row r="3" spans="1:9" ht="18" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1436,8 +1477,11 @@
       <c r="E3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="18" customHeight="1">
+      <c r="I3" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="18" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1450,8 +1494,11 @@
       <c r="D4" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="18" customHeight="1">
+      <c r="I4" s="8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="18" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -1459,11 +1506,14 @@
         <f>l_1/l_2</f>
         <v>1</v>
       </c>
-      <c r="D5" s="56" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1">
+      <c r="D5" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="18" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -1474,7 +1524,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1">
+    <row r="7" spans="1:9" ht="18" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
@@ -1485,7 +1535,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:9">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -1493,7 +1543,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1">
+    <row r="9" spans="1:9" ht="18" customHeight="1">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
@@ -1504,7 +1554,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="18" customHeight="1">
+    <row r="10" spans="1:9" ht="18" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
@@ -1515,7 +1565,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="18" customHeight="1">
+    <row r="11" spans="1:9" ht="18" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
@@ -1530,7 +1580,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:9">
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
@@ -1541,7 +1591,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:9">
       <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
@@ -1552,8 +1602,11 @@
       <c r="C13" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="18" customHeight="1">
+      <c r="D13" s="8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="18" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
@@ -1564,7 +1617,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="18" customHeight="1">
+    <row r="15" spans="1:9" ht="18" customHeight="1">
       <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
@@ -1576,7 +1629,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:9">
       <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
@@ -1593,6 +1646,9 @@
         <f>IF(AND(w_c&lt;150, w_c&gt;140), 0.85,IF(w_c=150, 1, "ERROR"))</f>
         <v>1</v>
       </c>
+      <c r="D17" s="8" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="18" customHeight="1">
       <c r="A18" s="3" t="s">
@@ -1604,6 +1660,9 @@
       </c>
       <c r="C18" t="s">
         <v>14</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -3759,10 +3818,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3770,42 +3829,53 @@
     <col min="1" max="1" width="13.140625" style="8" customWidth="1"/>
     <col min="10" max="10" width="12.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="52" t="s">
         <v>145</v>
       </c>
+      <c r="I1" s="8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="I2" s="8"/>
     </row>
     <row r="3" spans="1:15" ht="18" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="62">
         <f>f_n</f>
         <v>8.7618923090782665</v>
       </c>
       <c r="C3" t="s">
         <v>107</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="61">
         <f>Slab_Properties!B127</f>
         <v>272816</v>
       </c>
       <c r="C4" t="s">
         <v>110</v>
       </c>
+      <c r="I4" s="8"/>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="61">
         <f>Slab_Properties!B128</f>
         <v>0.04</v>
       </c>
@@ -3900,7 +3970,9 @@
       <c r="L9" s="56" t="s">
         <v>143</v>
       </c>
-      <c r="M9" s="8"/>
+      <c r="M9" s="56" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="56" t="s">
@@ -3913,22 +3985,36 @@
       <c r="C10" s="56">
         <v>1.25</v>
       </c>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="7"/>
+      <c r="D10" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="E10" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="F10" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="G10" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>172</v>
+      </c>
       <c r="I10" s="7">
         <f>250000000/($B$4*$B$5)*($C10^2.43/$B10^1.8)*(1-EXP(-2*PI()*$B$5*$B10/$C10))</f>
         <v>656.12079321093131</v>
       </c>
-      <c r="J10" s="7"/>
+      <c r="J10" s="7" t="s">
+        <v>172</v>
+      </c>
       <c r="K10" s="7">
         <f>250000000/($B$4*$B$5)*($C10^2.43/$B10^1.8)*(1-EXP(-2*PI()*$B$5*$B10/$C10))</f>
         <v>656.12079321093131</v>
       </c>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7">
+      <c r="L10" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="M10" s="60">
         <f>I10</f>
         <v>656.12079321093131</v>
       </c>
@@ -3964,7 +4050,7 @@
         <v>2255.7196184024665</v>
       </c>
       <c r="I11" s="7">
-        <f t="shared" ref="I11:K13" si="0">250000000/($B$4*$B$5)*($C11^2.43/$B11^1.8)*(1-EXP(-2*PI()*$B$5*$B11/$C11))</f>
+        <f t="shared" ref="I11:I13" si="0">250000000/($B$4*$B$5)*($C11^2.43/$B11^1.8)*(1-EXP(-2*PI()*$B$5*$B11/$C11))</f>
         <v>1078.8284997051478</v>
       </c>
       <c r="J11" s="7">
@@ -3979,7 +4065,7 @@
         <f>IF(AND($B11&gt;$E11,$B11&lt;$F11),$J11 + ($B11-$E11) * ($K11-$J11)/($F11-$E11), "N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="M11" s="7">
+      <c r="M11" s="60">
         <f>IF($B11&gt;=F11,I11, IF($B11&lt;=E11,H11,L11))</f>
         <v>1078.8284997051478</v>
       </c>
@@ -4033,7 +4119,7 @@
         <f t="shared" ref="L12:L13" si="1">IF(AND($B12&gt;$E12,$B12&lt;$F12),$J12 + ($B12-$E12) * ($K12-$J12)/($F12-$E12), "N/A")</f>
         <v>1600.7425670341886</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M12" s="60">
         <f>IF($B12&gt;=F12,I12, IF($B12&lt;=E12,H12,L12))</f>
         <v>1600.7425670341886</v>
       </c>
@@ -4084,7 +4170,7 @@
         <f t="shared" si="1"/>
         <v>2436.3590796036187</v>
       </c>
-      <c r="M13" s="7">
+      <c r="M13" s="60">
         <f>IF($B13&gt;=F13,I13, IF($B13&lt;=E13,H13,L13))</f>
         <v>2436.3590796036187</v>
       </c>
@@ -4092,9 +4178,12 @@
         <v>143</v>
       </c>
     </row>
+    <row r="14" spans="1:15">
+      <c r="M14" s="52"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4116,7 +4205,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AI42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed template calculation of drop panel period (shows 10% difference for one test)
</commit_message>
<xml_diff>
--- a/Flat_Plate_Vibration_Template.xlsx
+++ b/Flat_Plate_Vibration_Template.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27809"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mwachter\workspaces\vibraslab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maryannewachter/workspaces/vibraslab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7936AE1-4840-4610-8A2F-4DAC8582F532}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="6480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18980" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Slab_Properties" sheetId="1" r:id="rId1"/>
@@ -154,7 +153,15 @@
     <definedName name="y_t">#REF!</definedName>
     <definedName name="y_tdrop">Drop_Slab_Properties!$B$17</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -996,8 +1003,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <family val="1"/>
-        <charset val="2"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> =</t>
@@ -1667,8 +1673,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <family val="1"/>
-        <charset val="2"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> =</t>
@@ -1730,8 +1735,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <family val="1"/>
-        <charset val="2"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> =</t>
@@ -1880,12 +1884,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2004,190 +2008,190 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2195,23 +2199,23 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2702,29 +2706,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A82" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="B124" sqref="B124"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" style="8" customWidth="1"/>
     <col min="4" max="5" width="12" style="8" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="8" customWidth="1"/>
-    <col min="8" max="9" width="11.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="8" customWidth="1"/>
+    <col min="8" max="9" width="11.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="11.5" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="I1" s="8" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="52" t="s">
         <v>0</v>
       </c>
@@ -2732,7 +2736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="18" customHeight="1">
+    <row r="3" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>176</v>
       </c>
@@ -2752,7 +2756,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="18" customHeight="1">
+    <row r="4" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>177</v>
       </c>
@@ -2769,7 +2773,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="18" customHeight="1">
+    <row r="5" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>178</v>
       </c>
@@ -2784,7 +2788,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="18" customHeight="1">
+    <row r="6" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>179</v>
       </c>
@@ -2795,7 +2799,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="18" customHeight="1">
+    <row r="7" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>180</v>
       </c>
@@ -2806,7 +2810,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -2814,7 +2818,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="18" customHeight="1">
+    <row r="9" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>181</v>
       </c>
@@ -2825,7 +2829,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="18" customHeight="1">
+    <row r="10" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>182</v>
       </c>
@@ -2836,7 +2840,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="18" customHeight="1">
+    <row r="11" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>183</v>
       </c>
@@ -2851,7 +2855,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="18">
+    <row r="12" spans="1:19" ht="17" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
@@ -2907,7 +2911,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
@@ -2922,7 +2926,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="18" customHeight="1">
+    <row r="14" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>184</v>
       </c>
@@ -2933,7 +2937,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="18" customHeight="1">
+    <row r="15" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>185</v>
       </c>
@@ -2945,7 +2949,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
@@ -2954,7 +2958,7 @@
         <v>5.6374268708751352</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="18" customHeight="1">
+    <row r="17" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>186</v>
       </c>
@@ -2966,7 +2970,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="18" customHeight="1">
+    <row r="18" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>187</v>
       </c>
@@ -2981,15 +2985,15 @@
         <v>166</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="21" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>27</v>
       </c>
@@ -3000,7 +3004,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="18" customHeight="1">
+    <row r="22" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>188</v>
       </c>
@@ -3019,7 +3023,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="18" customHeight="1">
+    <row r="23" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>189</v>
       </c>
@@ -3035,12 +3039,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>34</v>
       </c>
@@ -3051,7 +3055,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>36</v>
       </c>
@@ -3062,7 +3066,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="18" customHeight="1">
+    <row r="28" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>37</v>
       </c>
@@ -3073,7 +3077,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>38</v>
       </c>
@@ -3085,7 +3089,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="17.25" customHeight="1">
+    <row r="30" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>39</v>
       </c>
@@ -3097,7 +3101,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>41</v>
       </c>
@@ -3109,11 +3113,11 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="6"/>
     </row>
-    <row r="33" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
+    <row r="33" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
         <v>43</v>
       </c>
@@ -3124,7 +3128,7 @@
       <c r="G33" s="54"/>
       <c r="H33" s="55"/>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="F34" s="45" t="s">
         <v>45</v>
@@ -3151,7 +3155,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="18" customHeight="1">
+    <row r="35" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="21" t="s">
         <v>47</v>
       </c>
@@ -3180,7 +3184,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="18.75" customHeight="1" thickBot="1">
+    <row r="36" spans="1:14" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>191</v>
       </c>
@@ -3216,7 +3220,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="18" customHeight="1">
+    <row r="37" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>192</v>
       </c>
@@ -3255,7 +3259,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="18" customHeight="1">
+    <row r="38" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>193</v>
       </c>
@@ -3297,7 +3301,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="18.75" customHeight="1" thickBot="1">
+    <row r="39" spans="1:14" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E39" s="3" t="s">
         <v>58</v>
       </c>
@@ -3326,7 +3330,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="18">
+    <row r="40" spans="1:14" ht="17" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>194</v>
       </c>
@@ -3347,7 +3351,7 @@
       <c r="L40" s="56"/>
       <c r="M40" s="56"/>
     </row>
-    <row r="41" spans="1:14" ht="18">
+    <row r="41" spans="1:14" ht="17" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>195</v>
       </c>
@@ -3368,7 +3372,7 @@
       <c r="L41" s="56"/>
       <c r="M41" s="56"/>
     </row>
-    <row r="42" spans="1:14" ht="18">
+    <row r="42" spans="1:14" ht="17" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>196</v>
       </c>
@@ -3389,7 +3393,7 @@
       <c r="L42" s="56"/>
       <c r="M42" s="56"/>
     </row>
-    <row r="43" spans="1:14" ht="18">
+    <row r="43" spans="1:14" ht="17" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>197</v>
       </c>
@@ -3410,7 +3414,7 @@
       <c r="L43" s="56"/>
       <c r="M43" s="56"/>
     </row>
-    <row r="44" spans="1:14" ht="18">
+    <row r="44" spans="1:14" ht="17" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>198</v>
       </c>
@@ -3431,7 +3435,7 @@
       <c r="L44" s="56"/>
       <c r="M44" s="56"/>
     </row>
-    <row r="45" spans="1:14" ht="18">
+    <row r="45" spans="1:14" ht="17" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>199</v>
       </c>
@@ -3452,7 +3456,7 @@
       <c r="L45" s="56"/>
       <c r="M45" s="56"/>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E46" s="3"/>
       <c r="F46" s="56"/>
       <c r="G46" s="56"/>
@@ -3463,7 +3467,7 @@
       <c r="L46" s="56"/>
       <c r="M46" s="56"/>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="21" t="s">
         <v>65</v>
       </c>
@@ -3477,7 +3481,7 @@
       <c r="L47" s="56"/>
       <c r="M47" s="56"/>
     </row>
-    <row r="48" spans="1:14" ht="18" customHeight="1">
+    <row r="48" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>200</v>
       </c>
@@ -3501,7 +3505,7 @@
       <c r="L48" s="56"/>
       <c r="M48" s="56"/>
     </row>
-    <row r="49" spans="1:13" ht="18" customHeight="1">
+    <row r="49" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>201</v>
       </c>
@@ -3522,7 +3526,7 @@
       <c r="L49" s="56"/>
       <c r="M49" s="56"/>
     </row>
-    <row r="50" spans="1:13" ht="18" customHeight="1">
+    <row r="50" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>202</v>
       </c>
@@ -3543,7 +3547,7 @@
       <c r="L50" s="56"/>
       <c r="M50" s="56"/>
     </row>
-    <row r="51" spans="1:13" ht="18" customHeight="1">
+    <row r="51" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>203</v>
       </c>
@@ -3564,7 +3568,7 @@
       <c r="L51" s="56"/>
       <c r="M51" s="56"/>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="3"/>
       <c r="B52" s="7"/>
       <c r="E52" s="3"/>
@@ -3577,12 +3581,12 @@
       <c r="L52" s="56"/>
       <c r="M52" s="56"/>
     </row>
-    <row r="53" spans="1:13" ht="18" customHeight="1">
+    <row r="53" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="21" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="56" t="s">
         <v>27</v>
       </c>
@@ -3599,7 +3603,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="18" customHeight="1">
+    <row r="55" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="56" t="s">
         <v>188</v>
       </c>
@@ -3621,7 +3625,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="18" customHeight="1">
+    <row r="56" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="56" t="s">
         <v>188</v>
       </c>
@@ -3643,7 +3647,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="18" customHeight="1">
+    <row r="57" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="56" t="s">
         <v>188</v>
       </c>
@@ -3658,14 +3662,14 @@
         <v>391.55338541666663</v>
       </c>
       <c r="E57" s="7">
-        <f>IF($D$4="interior", H39*I39*B48,  IF($D$4="exterior", L39*M39*B48, "ERROR"))</f>
-        <v>121.19509548611113</v>
+        <f>IF($D$3="interior", H39*I39*B48,  IF($D$3="exterior", L39*M39*B48, "ERROR"))</f>
+        <v>130.51779513888889</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="18" customHeight="1">
+    <row r="58" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="56" t="s">
         <v>188</v>
       </c>
@@ -3687,7 +3691,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="18" customHeight="1">
+    <row r="59" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="56" t="s">
         <v>188</v>
       </c>
@@ -3709,7 +3713,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="18" customHeight="1">
+    <row r="60" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="56" t="s">
         <v>188</v>
       </c>
@@ -3731,7 +3735,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="18" customHeight="1">
+    <row r="61" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="56" t="s">
         <v>189</v>
       </c>
@@ -3753,7 +3757,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="18" customHeight="1">
+    <row r="62" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="56" t="s">
         <v>189</v>
       </c>
@@ -3775,7 +3779,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="18" customHeight="1">
+    <row r="63" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="56" t="s">
         <v>189</v>
       </c>
@@ -3797,7 +3801,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="18" customHeight="1">
+    <row r="64" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="56" t="s">
         <v>189</v>
       </c>
@@ -3819,7 +3823,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="18" customHeight="1">
+    <row r="65" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="56" t="s">
         <v>189</v>
       </c>
@@ -3841,7 +3845,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="66" spans="1:19" ht="18" customHeight="1">
+    <row r="66" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="56" t="s">
         <v>189</v>
       </c>
@@ -3863,12 +3867,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="69" spans="1:19" ht="18" customHeight="1">
+    <row r="69" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="52" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="70" spans="1:19">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A70" s="56" t="s">
         <v>27</v>
       </c>
@@ -3882,7 +3886,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="71" spans="1:19" ht="18" customHeight="1">
+    <row r="71" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="56" t="s">
         <v>188</v>
       </c>
@@ -3901,7 +3905,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="72" spans="1:19" ht="18" customHeight="1">
+    <row r="72" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="56" t="s">
         <v>188</v>
       </c>
@@ -3920,7 +3924,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="73" spans="1:19" ht="18" customHeight="1">
+    <row r="73" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="56" t="s">
         <v>188</v>
       </c>
@@ -3933,13 +3937,13 @@
       </c>
       <c r="D73" s="7">
         <f t="shared" si="0"/>
-        <v>240.89855902777779</v>
+        <v>252.0857986111111</v>
       </c>
       <c r="E73" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="74" spans="1:19" ht="18" customHeight="1">
+    <row r="74" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="56" t="s">
         <v>189</v>
       </c>
@@ -3958,7 +3962,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="75" spans="1:19" ht="18" customHeight="1">
+    <row r="75" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="56" t="s">
         <v>189</v>
       </c>
@@ -3977,7 +3981,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="76" spans="1:19" ht="18" customHeight="1">
+    <row r="76" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="56" t="s">
         <v>189</v>
       </c>
@@ -3996,7 +4000,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="78" spans="1:19" ht="18" customHeight="1">
+    <row r="78" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="21" t="s">
         <v>80</v>
       </c>
@@ -4012,7 +4016,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="79" spans="1:19">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A79" s="56" t="s">
         <v>27</v>
       </c>
@@ -4063,7 +4067,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="80" spans="1:19" ht="18.75" customHeight="1">
+    <row r="80" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="56" t="s">
         <v>188</v>
       </c>
@@ -4126,7 +4130,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:19" ht="18.75" customHeight="1">
+    <row r="81" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="56" t="s">
         <v>188</v>
       </c>
@@ -4189,7 +4193,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:19" ht="18.75" customHeight="1">
+    <row r="82" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="56" t="s">
         <v>188</v>
       </c>
@@ -4252,7 +4256,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:19" ht="18.75" customHeight="1">
+    <row r="83" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="56" t="s">
         <v>189</v>
       </c>
@@ -4315,7 +4319,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:19" ht="18.75" customHeight="1">
+    <row r="84" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="56" t="s">
         <v>189</v>
       </c>
@@ -4378,7 +4382,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="85" spans="1:19" ht="18.75" customHeight="1">
+    <row r="85" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="56" t="s">
         <v>189</v>
       </c>
@@ -4441,12 +4445,12 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="87" spans="1:19" ht="18" customHeight="1">
+    <row r="87" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="21" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="88" spans="1:19">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A88" s="56" t="s">
         <v>27</v>
       </c>
@@ -4460,7 +4464,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="89" spans="1:19" ht="18.75" customHeight="1">
+    <row r="89" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="56" t="s">
         <v>188</v>
       </c>
@@ -4479,7 +4483,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="90" spans="1:19" ht="18.75" customHeight="1">
+    <row r="90" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="56" t="s">
         <v>188</v>
       </c>
@@ -4498,7 +4502,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="91" spans="1:19" ht="18.75" customHeight="1">
+    <row r="91" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="56" t="s">
         <v>188</v>
       </c>
@@ -4517,7 +4521,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="92" spans="1:19" ht="18.75" customHeight="1">
+    <row r="92" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="56" t="s">
         <v>189</v>
       </c>
@@ -4536,7 +4540,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="93" spans="1:19" ht="18.75" customHeight="1">
+    <row r="93" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="56" t="s">
         <v>189</v>
       </c>
@@ -4555,7 +4559,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="94" spans="1:19" ht="18.75" customHeight="1">
+    <row r="94" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="56" t="s">
         <v>189</v>
       </c>
@@ -4574,8 +4578,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="95" spans="1:19" ht="15.75" customHeight="1" thickBot="1"/>
-    <row r="96" spans="1:19">
+    <row r="95" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="96" spans="1:19" x14ac:dyDescent="0.2">
       <c r="F96" s="38" t="s">
         <v>28</v>
       </c>
@@ -4613,7 +4617,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="97" spans="1:17" ht="18" customHeight="1">
+    <row r="97" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="21" t="s">
         <v>86</v>
       </c>
@@ -4654,7 +4658,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="98" spans="1:17" ht="18" customHeight="1" thickBot="1">
+    <row r="98" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A98" s="56" t="s">
         <v>27</v>
       </c>
@@ -4696,7 +4700,7 @@
       <c r="P98" s="26"/>
       <c r="Q98" s="29"/>
     </row>
-    <row r="99" spans="1:17" ht="18.75" customHeight="1">
+    <row r="99" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="56" t="s">
         <v>188</v>
       </c>
@@ -4763,7 +4767,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:17" ht="18.75" customHeight="1">
+    <row r="100" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="56" t="s">
         <v>188</v>
       </c>
@@ -4830,7 +4834,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:17" ht="18.75" customHeight="1">
+    <row r="101" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="56" t="s">
         <v>188</v>
       </c>
@@ -4843,7 +4847,7 @@
       </c>
       <c r="D101" s="7">
         <f t="shared" si="3"/>
-        <v>31181.406061892005</v>
+        <v>18710.318714874153</v>
       </c>
       <c r="E101" s="8" t="s">
         <v>205</v>
@@ -4886,7 +4890,7 @@
       </c>
       <c r="O101" s="22">
         <f t="shared" si="6"/>
-        <v>0.97702985695319178</v>
+        <v>0.92913623651430988</v>
       </c>
       <c r="P101" s="22">
         <f>C82/(l_1c*d)</f>
@@ -4897,7 +4901,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:17" ht="18.75" customHeight="1">
+    <row r="102" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="56" t="s">
         <v>189</v>
       </c>
@@ -4964,7 +4968,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:17" ht="18.75" customHeight="1">
+    <row r="103" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="56" t="s">
         <v>189</v>
       </c>
@@ -5031,7 +5035,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:17" ht="19.5" customHeight="1" thickBot="1">
+    <row r="104" spans="1:17" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="56" t="s">
         <v>189</v>
       </c>
@@ -5098,12 +5102,12 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:17" ht="18" customHeight="1">
+    <row r="106" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="21" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="107" spans="1:17">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A107" s="56" t="s">
         <v>27</v>
       </c>
@@ -5114,7 +5118,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="108" spans="1:17" ht="18.75" customHeight="1">
+    <row r="108" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="56" t="s">
         <v>188</v>
       </c>
@@ -5124,13 +5128,13 @@
       </c>
       <c r="C108" s="7">
         <f>0.7*D99+ 0.15*SUM(D100:D101)</f>
-        <v>17896.724752525424</v>
+        <v>16026.061650472744</v>
       </c>
       <c r="D108" s="8" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="109" spans="1:17" ht="18.75" customHeight="1">
+    <row r="109" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="56" t="s">
         <v>189</v>
       </c>
@@ -5146,38 +5150,38 @@
         <v>205</v>
       </c>
     </row>
-    <row r="110" spans="1:17">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" s="56"/>
       <c r="B110" s="56"/>
     </row>
-    <row r="111" spans="1:17" ht="18" customHeight="1">
+    <row r="111" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="21" t="s">
         <v>207</v>
       </c>
       <c r="B111" s="56"/>
     </row>
-    <row r="112" spans="1:17" ht="18.75" customHeight="1">
+    <row r="112" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>209</v>
       </c>
       <c r="B112" s="7">
-        <f>IF(l_1/l_2&lt;1.05, B108+C109, (B108+C108+B109+C109)/2)</f>
-        <v>53902.817902803879</v>
+        <f>(B108+C108+B109+C109)/2</f>
+        <v>39298.260405496512</v>
       </c>
       <c r="C112" s="8" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="56"/>
       <c r="B113" s="56"/>
     </row>
-    <row r="114" spans="1:5" ht="18" customHeight="1">
+    <row r="114" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="21" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="18.75" customHeight="1">
+    <row r="115" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
         <v>210</v>
       </c>
@@ -5189,21 +5193,21 @@
         <v>205</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="18" customHeight="1">
+    <row r="117" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="52" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="18" customHeight="1">
+    <row r="118" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
         <v>212</v>
       </c>
       <c r="B118" s="10">
         <f>B112/B115</f>
-        <v>0.57776129633428952</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" ht="19.5" customHeight="1" thickBot="1">
+        <v>0.42122127857031932</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="52" t="s">
         <v>100</v>
       </c>
@@ -5211,7 +5215,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="18" customHeight="1">
+    <row r="121" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>213</v>
       </c>
@@ -5226,7 +5230,7 @@
         <v>7.12</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="18.75" customHeight="1">
+    <row r="122" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="11" t="s">
         <v>214</v>
       </c>
@@ -5245,7 +5249,7 @@
         <v>8.92</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="18" customHeight="1" thickBot="1">
+    <row r="123" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A123" s="11" t="s">
         <v>104</v>
       </c>
@@ -5263,24 +5267,24 @@
         <v>9.2899999999999991</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="18" customHeight="1">
+    <row r="124" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
         <v>106</v>
       </c>
       <c r="B124" s="4">
         <f>k_2*lambda_i_sq / (2 * PI() * l_1^2) * SQRT(k_1 * E_c*144*(h/12)^3 / (12*gamma*(1-nu^2)))</f>
-        <v>6.5787139276963806</v>
+        <v>5.6172264218657322</v>
       </c>
       <c r="C124" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="21" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
         <v>109</v>
       </c>
@@ -5292,7 +5296,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="11" t="s">
         <v>216</v>
       </c>
@@ -5307,31 +5311,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0D748F3-C8FC-4371-B094-6649B9A32C29}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S134"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O109" sqref="O109"/>
+    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="G129" sqref="G129:G130"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" style="8" customWidth="1"/>
-    <col min="2" max="3" width="9.140625" style="8"/>
+    <col min="2" max="3" width="8.83203125" style="8"/>
     <col min="4" max="5" width="12" style="8" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="8" customWidth="1"/>
-    <col min="8" max="9" width="11.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="8"/>
+    <col min="6" max="6" width="11.83203125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="8" customWidth="1"/>
+    <col min="8" max="9" width="11.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="11.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="I1" s="8" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="52" t="s">
         <v>0</v>
       </c>
@@ -5339,7 +5343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="18" customHeight="1">
+    <row r="3" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>176</v>
       </c>
@@ -5359,7 +5363,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="18" customHeight="1">
+    <row r="4" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>177</v>
       </c>
@@ -5376,7 +5380,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="18" customHeight="1">
+    <row r="5" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>178</v>
       </c>
@@ -5391,7 +5395,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="18" customHeight="1">
+    <row r="6" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>179</v>
       </c>
@@ -5402,7 +5406,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="18" customHeight="1">
+    <row r="7" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>180</v>
       </c>
@@ -5413,7 +5417,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -5421,7 +5425,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="18" customHeight="1">
+    <row r="9" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>181</v>
       </c>
@@ -5432,7 +5436,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="18" customHeight="1">
+    <row r="10" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>182</v>
       </c>
@@ -5443,7 +5447,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="18" customHeight="1">
+    <row r="11" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>183</v>
       </c>
@@ -5458,13 +5462,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="18">
+    <row r="12" spans="1:19" ht="17" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="8">
-        <f>IF(ISBLANK(R12),D12,R12)</f>
-        <v>15.166666666666668</v>
+        <v>14</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>10</v>
@@ -5517,7 +5520,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
@@ -5532,7 +5535,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="18">
+    <row r="14" spans="1:19" ht="17" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>222</v>
       </c>
@@ -5544,7 +5547,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="18" customHeight="1">
+    <row r="15" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>184</v>
       </c>
@@ -5555,7 +5558,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="18" customHeight="1">
+    <row r="16" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>185</v>
       </c>
@@ -5567,7 +5570,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="18" customHeight="1">
+    <row r="17" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>223</v>
       </c>
@@ -5579,7 +5582,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>23</v>
       </c>
@@ -5588,7 +5591,7 @@
         <v>5.6374268708751352</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="18" customHeight="1">
+    <row r="19" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>186</v>
       </c>
@@ -5600,7 +5603,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="18" customHeight="1">
+    <row r="20" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>187</v>
       </c>
@@ -5615,15 +5618,15 @@
         <v>166</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="21" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>27</v>
       </c>
@@ -5634,7 +5637,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="18" customHeight="1">
+    <row r="24" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>188</v>
       </c>
@@ -5653,7 +5656,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="18" customHeight="1">
+    <row r="25" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>189</v>
       </c>
@@ -5669,12 +5672,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>34</v>
       </c>
@@ -5685,7 +5688,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>36</v>
       </c>
@@ -5696,7 +5699,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="18" customHeight="1">
+    <row r="30" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>37</v>
       </c>
@@ -5707,47 +5710,47 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B31" s="6">
         <f>(h/12*w_c)</f>
-        <v>189.58333333333337</v>
+        <v>175</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="17.25" customHeight="1">
+    <row r="32" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B32" s="6">
         <f>(h / 12 * w_c +SDL+LLvib)*l_1*l_2/32.2</f>
-        <v>7201.0662525879925</v>
+        <v>6677.5155279503097</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B33" s="6">
         <f>mass * 32.2/1000</f>
-        <v>231.87433333333337</v>
+        <v>215.01599999999999</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
+    <row r="34" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="6"/>
     </row>
-    <row r="35" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
+    <row r="35" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="21" t="s">
         <v>43</v>
       </c>
@@ -5758,7 +5761,7 @@
       <c r="G35" s="54"/>
       <c r="H35" s="55"/>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="F36" s="45" t="s">
         <v>45</v>
@@ -5785,7 +5788,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="18" customHeight="1">
+    <row r="37" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="21" t="s">
         <v>47</v>
       </c>
@@ -5814,13 +5817,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="18.75" customHeight="1" thickBot="1">
+    <row r="38" spans="1:14" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>191</v>
       </c>
       <c r="B38" s="6">
         <f>1.2*(SDL+SW) +1.6*LL</f>
-        <v>355.5</v>
+        <v>338</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>49</v>
@@ -5850,13 +5853,13 @@
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="18" customHeight="1">
+    <row r="39" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>192</v>
       </c>
       <c r="B39" s="6">
         <f>(q_u*l_2*(l_1-c_1 / 12)^2 / 8) / 1000</f>
-        <v>1515.0718750000001</v>
+        <v>1440.4902777777777</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>53</v>
@@ -5889,13 +5892,13 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="18" customHeight="1">
+    <row r="40" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>193</v>
       </c>
       <c r="B40" s="6">
         <f>(q_u*l_1*(l_2 - c_2 / 12) ^2 / 8) / 1000</f>
-        <v>1515.0718750000001</v>
+        <v>1440.4902777777777</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>53</v>
@@ -5931,7 +5934,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="18.75" customHeight="1" thickBot="1">
+    <row r="41" spans="1:14" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E41" s="3" t="s">
         <v>58</v>
       </c>
@@ -5960,13 +5963,13 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="18">
+    <row r="42" spans="1:14" ht="17" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>194</v>
       </c>
       <c r="B42" s="6">
         <f>IF($D$3="interior", F39*B39,  IF($D$3="exterior", J39*B39, "ERROR"))</f>
-        <v>787.83737500000007</v>
+        <v>749.05494444444446</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>53</v>
@@ -5981,13 +5984,13 @@
       <c r="L42" s="56"/>
       <c r="M42" s="56"/>
     </row>
-    <row r="43" spans="1:14" ht="18">
+    <row r="43" spans="1:14" ht="17" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>195</v>
       </c>
       <c r="B43" s="6">
         <f>IF($D$3="interior", F40*B39,  IF($D$3="exterior", J40*B39, "ERROR"))</f>
-        <v>393.91868750000003</v>
+        <v>374.52747222222223</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>53</v>
@@ -6002,13 +6005,13 @@
       <c r="L43" s="56"/>
       <c r="M43" s="56"/>
     </row>
-    <row r="44" spans="1:14" ht="18">
+    <row r="44" spans="1:14" ht="17" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>196</v>
       </c>
       <c r="B44" s="6">
         <f>IF($D$3="interior", F41*B39,  IF($D$3="exterior", J41*B39, "ERROR"))</f>
-        <v>1060.5503125</v>
+        <v>1008.3431944444443</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>53</v>
@@ -6023,13 +6026,13 @@
       <c r="L44" s="56"/>
       <c r="M44" s="56"/>
     </row>
-    <row r="45" spans="1:14" ht="18">
+    <row r="45" spans="1:14" ht="17" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>197</v>
       </c>
       <c r="B45" s="6">
         <f>IF($D$4="interior", F39*B40,  IF($D$4="exterior", J39*B40, "ERROR"))</f>
-        <v>530.27515625000001</v>
+        <v>504.17159722222215</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>53</v>
@@ -6044,13 +6047,13 @@
       <c r="L45" s="56"/>
       <c r="M45" s="56"/>
     </row>
-    <row r="46" spans="1:14" ht="18">
+    <row r="46" spans="1:14" ht="17" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>198</v>
       </c>
       <c r="B46" s="6">
         <f>IF($D$4="interior", F40*B40,  IF($D$4="exterior", J40*B40, "ERROR"))</f>
-        <v>984.79671875000008</v>
+        <v>936.31868055555549</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>53</v>
@@ -6065,13 +6068,13 @@
       <c r="L46" s="56"/>
       <c r="M46" s="56"/>
     </row>
-    <row r="47" spans="1:14" ht="18">
+    <row r="47" spans="1:14" ht="17" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>199</v>
       </c>
       <c r="B47" s="6">
         <f>IF($D$4="interior", F41*B40,  IF($D$4="exterior", J41*B40, "ERROR"))</f>
-        <v>984.79671875000008</v>
+        <v>936.31868055555549</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>53</v>
@@ -6086,7 +6089,7 @@
       <c r="L47" s="56"/>
       <c r="M47" s="56"/>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E48" s="3"/>
       <c r="F48" s="56"/>
       <c r="G48" s="56"/>
@@ -6097,7 +6100,7 @@
       <c r="L48" s="56"/>
       <c r="M48" s="56"/>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="21" t="s">
         <v>65</v>
       </c>
@@ -6111,13 +6114,13 @@
       <c r="L49" s="56"/>
       <c r="M49" s="56"/>
     </row>
-    <row r="50" spans="1:13" ht="18" customHeight="1">
+    <row r="50" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>200</v>
       </c>
       <c r="B50" s="7">
         <f>((SW+SDL)*l_2*(l_1-c_1 / 12) ^ 2 / 8) / 1000</f>
-        <v>807.96730324074099</v>
+        <v>745.81597222222229</v>
       </c>
       <c r="C50" s="8" t="s">
         <v>53</v>
@@ -6135,7 +6138,7 @@
       <c r="L50" s="56"/>
       <c r="M50" s="56"/>
     </row>
-    <row r="51" spans="1:13" ht="18" customHeight="1">
+    <row r="51" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>201</v>
       </c>
@@ -6156,13 +6159,13 @@
       <c r="L51" s="56"/>
       <c r="M51" s="56"/>
     </row>
-    <row r="52" spans="1:13" ht="18" customHeight="1">
+    <row r="52" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>202</v>
       </c>
       <c r="B52" s="7">
         <f>((SW+SDL)*l_1*(l_2-c_2 / 12) ^ 2 / 8) / 1000</f>
-        <v>807.96730324074099</v>
+        <v>745.81597222222229</v>
       </c>
       <c r="C52" s="8" t="s">
         <v>53</v>
@@ -6177,7 +6180,7 @@
       <c r="L52" s="56"/>
       <c r="M52" s="56"/>
     </row>
-    <row r="53" spans="1:13" ht="18" customHeight="1">
+    <row r="53" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>203</v>
       </c>
@@ -6198,7 +6201,7 @@
       <c r="L53" s="56"/>
       <c r="M53" s="56"/>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="3"/>
       <c r="B54" s="7"/>
       <c r="E54" s="3"/>
@@ -6211,12 +6214,12 @@
       <c r="L54" s="56"/>
       <c r="M54" s="56"/>
     </row>
-    <row r="55" spans="1:13" ht="18" customHeight="1">
+    <row r="55" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="21" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" s="56" t="s">
         <v>27</v>
       </c>
@@ -6233,7 +6236,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="18" customHeight="1">
+    <row r="57" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="56" t="s">
         <v>188</v>
       </c>
@@ -6245,17 +6248,17 @@
       </c>
       <c r="D57" s="7">
         <f>IF($D$3="interior", F39*G39*B50,  IF($D$3="exterior", J39*K39*B50, "ERROR"))</f>
-        <v>252.08579861111119</v>
+        <v>232.69458333333336</v>
       </c>
       <c r="E57" s="7">
         <f>IF($D$3="interior", H39*I39*B50,  IF($D$3="exterior", L39*M39*B50, "ERROR"))</f>
-        <v>168.05719907407413</v>
+        <v>155.12972222222226</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="18" customHeight="1">
+    <row r="58" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="56" t="s">
         <v>188</v>
       </c>
@@ -6267,7 +6270,7 @@
       </c>
       <c r="D58" s="7">
         <f>IF($D$3="interior", F40*G40*B50,  IF($D$3="exterior", J40*K40*B50, "ERROR"))</f>
-        <v>210.07149884259266</v>
+        <v>193.91215277777781</v>
       </c>
       <c r="E58" s="7">
         <f>IF($D$3="interior", H40*I40*B50,  IF($D$3="exterior", L40*M40*B50, "ERROR"))</f>
@@ -6277,7 +6280,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="18" customHeight="1">
+    <row r="59" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="56" t="s">
         <v>188</v>
       </c>
@@ -6289,17 +6292,17 @@
       </c>
       <c r="D59" s="7">
         <f>IF($D$3="interior", F41*G41*B50,  IF($D$3="exterior", J41*K41*B50, "ERROR"))</f>
-        <v>424.18283420138897</v>
+        <v>391.55338541666663</v>
       </c>
       <c r="E59" s="7">
         <f>IF($D$3="interior", H41*I41*B50,  IF($D$3="exterior", L41*M41*B50, "ERROR"))</f>
-        <v>141.39427806712968</v>
+        <v>130.51779513888889</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="18" customHeight="1">
+    <row r="60" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="56" t="s">
         <v>188</v>
       </c>
@@ -6321,7 +6324,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="18" customHeight="1">
+    <row r="61" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="56" t="s">
         <v>188</v>
       </c>
@@ -6343,7 +6346,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="18" customHeight="1">
+    <row r="62" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="56" t="s">
         <v>188</v>
       </c>
@@ -6365,7 +6368,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="18" customHeight="1">
+    <row r="63" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="56" t="s">
         <v>189</v>
       </c>
@@ -6377,17 +6380,17 @@
       </c>
       <c r="D63" s="7">
         <f>IF($D$4="interior", F39*G39*B52,  IF($D$4="exterior", J39*K39*B52, "ERROR"))</f>
-        <v>169.67313368055559</v>
+        <v>156.62135416666666</v>
       </c>
       <c r="E63" s="7">
         <f>IF($D$4="interior", H39*I39*B52,  IF($D$4="exterior", L39*M39*B52, "ERROR"))</f>
-        <v>113.11542245370373</v>
+        <v>104.41423611111111</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="18" customHeight="1">
+    <row r="64" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="56" t="s">
         <v>189</v>
       </c>
@@ -6399,17 +6402,17 @@
       </c>
       <c r="D64" s="7">
         <f>IF($D$4="interior", F40*G40*B52,  IF($D$4="exterior", J40*K40*B52, "ERROR"))</f>
-        <v>393.88406032986126</v>
+        <v>363.58528645833337</v>
       </c>
       <c r="E64" s="7">
         <f>IF($D$4="interior", H40*I40*B52,  IF($D$4="exterior", L40*M40*B52, "ERROR"))</f>
-        <v>131.29468677662041</v>
+        <v>121.19509548611113</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="65" spans="1:18" ht="18" customHeight="1">
+    <row r="65" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="56" t="s">
         <v>189</v>
       </c>
@@ -6421,17 +6424,17 @@
       </c>
       <c r="D65" s="7">
         <f>IF($D$4="interior", F41*G41*B52,  IF($D$4="exterior", J41*K41*B52, "ERROR"))</f>
-        <v>393.88406032986126</v>
+        <v>363.58528645833337</v>
       </c>
       <c r="E65" s="7">
         <f>IF($D$4="interior", H41*I41*B52,  IF($D$4="exterior", L41*M41*B52, "ERROR"))</f>
-        <v>131.29468677662041</v>
+        <v>121.19509548611113</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="66" spans="1:18" ht="18" customHeight="1">
+    <row r="66" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="56" t="s">
         <v>189</v>
       </c>
@@ -6453,7 +6456,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="67" spans="1:18" ht="18" customHeight="1">
+    <row r="67" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="56" t="s">
         <v>189</v>
       </c>
@@ -6475,7 +6478,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="1:18" ht="18" customHeight="1">
+    <row r="68" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="56" t="s">
         <v>189</v>
       </c>
@@ -6497,12 +6500,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="71" spans="1:18" ht="18" customHeight="1">
+    <row r="71" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="52" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="72" spans="1:18">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A72" s="56" t="s">
         <v>27</v>
       </c>
@@ -6516,7 +6519,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="73" spans="1:18" ht="18" customHeight="1">
+    <row r="73" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="56" t="s">
         <v>188</v>
       </c>
@@ -6525,17 +6528,17 @@
       </c>
       <c r="C73" s="7">
         <f t="shared" ref="C73:D75" si="0">1.2*D57+1.6*D60</f>
-        <v>472.70242500000012</v>
+        <v>449.43296666666669</v>
       </c>
       <c r="D73" s="7">
         <f t="shared" si="0"/>
-        <v>315.13495000000006</v>
+        <v>299.62197777777783</v>
       </c>
       <c r="E73" s="8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="74" spans="1:18" ht="18" customHeight="1">
+    <row r="74" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="56" t="s">
         <v>188</v>
       </c>
@@ -6544,7 +6547,7 @@
       </c>
       <c r="C74" s="7">
         <f t="shared" si="0"/>
-        <v>393.91868750000009</v>
+        <v>374.52747222222229</v>
       </c>
       <c r="D74" s="7">
         <f t="shared" si="0"/>
@@ -6554,7 +6557,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="75" spans="1:18" ht="18" customHeight="1">
+    <row r="75" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="56" t="s">
         <v>188</v>
       </c>
@@ -6563,17 +6566,17 @@
       </c>
       <c r="C75" s="7">
         <f t="shared" si="0"/>
-        <v>795.41273437500013</v>
+        <v>756.25739583333325</v>
       </c>
       <c r="D75" s="7">
         <f t="shared" si="0"/>
-        <v>265.137578125</v>
+        <v>252.0857986111111</v>
       </c>
       <c r="E75" s="8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="76" spans="1:18" ht="18" customHeight="1">
+    <row r="76" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="56" t="s">
         <v>189</v>
       </c>
@@ -6582,17 +6585,17 @@
       </c>
       <c r="C76" s="7">
         <f t="shared" ref="C76:D78" si="1">1.2*D63+1.6*D66</f>
-        <v>318.16509375000004</v>
+        <v>302.50295833333331</v>
       </c>
       <c r="D76" s="7">
         <f t="shared" si="1"/>
-        <v>212.11006250000003</v>
+        <v>201.66863888888889</v>
       </c>
       <c r="E76" s="8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="77" spans="1:18" ht="18" customHeight="1">
+    <row r="77" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="56" t="s">
         <v>189</v>
       </c>
@@ -6601,17 +6604,17 @@
       </c>
       <c r="C77" s="7">
         <f t="shared" si="1"/>
-        <v>738.59753906250012</v>
+        <v>702.2390104166667</v>
       </c>
       <c r="D77" s="7">
         <f t="shared" si="1"/>
-        <v>246.19917968750005</v>
+        <v>234.07967013888893</v>
       </c>
       <c r="E77" s="8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="78" spans="1:18" ht="18" customHeight="1">
+    <row r="78" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="56" t="s">
         <v>189</v>
       </c>
@@ -6620,17 +6623,17 @@
       </c>
       <c r="C78" s="7">
         <f t="shared" si="1"/>
-        <v>738.59753906250012</v>
+        <v>702.2390104166667</v>
       </c>
       <c r="D78" s="7">
         <f t="shared" si="1"/>
-        <v>246.19917968750005</v>
+        <v>234.07967013888893</v>
       </c>
       <c r="E78" s="8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="80" spans="1:18" ht="18" customHeight="1">
+    <row r="80" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="21" t="s">
         <v>80</v>
       </c>
@@ -6644,7 +6647,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="81" spans="1:19">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A81" s="56" t="s">
         <v>27</v>
       </c>
@@ -6694,7 +6697,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="82" spans="1:19" ht="18.75" customHeight="1">
+    <row r="82" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="56" t="s">
         <v>188</v>
       </c>
@@ -6720,7 +6723,7 @@
       </c>
       <c r="H82" s="10">
         <f>MAX(C73*12000/d*0.85/54000, 0.0025*l_1c*12*d)</f>
-        <v>7.0029988888888912</v>
+        <v>6.6582661728395065</v>
       </c>
       <c r="I82" s="10">
         <f>MAX(D73*12000/d*0.85/54000, 0.0025*l_1m*12*d)</f>
@@ -6756,7 +6759,7 @@
         <v>2.15E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:19" ht="18.75" customHeight="1">
+    <row r="83" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="56" t="s">
         <v>188</v>
       </c>
@@ -6818,7 +6821,7 @@
         <v>1.98E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:19" ht="18.75" customHeight="1">
+    <row r="84" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="56" t="s">
         <v>188</v>
       </c>
@@ -6844,7 +6847,7 @@
       </c>
       <c r="H84" s="10">
         <f>MAX(C75*12000/d_drop*0.85/54000, 0.0025*l_1c*12*d_drop)</f>
-        <v>9.2458232371794882</v>
+        <v>8.7906842592592565</v>
       </c>
       <c r="I84" s="10">
         <f>MAX(D75*12000/d*0.85/54000, 0.0025*l_1m*12*d)</f>
@@ -6880,7 +6883,7 @@
         <v>1.98E-3</v>
       </c>
     </row>
-    <row r="85" spans="1:19" ht="18.75" customHeight="1">
+    <row r="85" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="56" t="s">
         <v>189</v>
       </c>
@@ -6942,7 +6945,7 @@
         <v>1.98E-3</v>
       </c>
     </row>
-    <row r="86" spans="1:19" ht="18.75" customHeight="1">
+    <row r="86" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="56" t="s">
         <v>189</v>
       </c>
@@ -6968,7 +6971,7 @@
       </c>
       <c r="H86" s="10">
         <f>MAX(C77*12000/d_drop*0.85/54000, 0.0025*l_2c*12*d_drop)</f>
-        <v>8.5854072916666677</v>
+        <v>8.2874999999999996</v>
       </c>
       <c r="I86" s="10">
         <f>MAX(D77*12000/d*0.85/54000, 0.0025*l_2m*12*d)</f>
@@ -7004,7 +7007,7 @@
         <v>1.98E-3</v>
       </c>
     </row>
-    <row r="87" spans="1:19" ht="18.75" customHeight="1">
+    <row r="87" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="56" t="s">
         <v>189</v>
       </c>
@@ -7030,7 +7033,7 @@
       </c>
       <c r="H87" s="10">
         <f>MAX(C78*12000/d_drop*0.85/54000, 0.0025*l_2c*12*d_drop)</f>
-        <v>8.5854072916666677</v>
+        <v>8.2874999999999996</v>
       </c>
       <c r="I87" s="10">
         <f>MAX(D78*12000/d*0.85/54000, 0.0025*l_2m*12*d)</f>
@@ -7066,12 +7069,12 @@
         <v>1.98E-3</v>
       </c>
     </row>
-    <row r="89" spans="1:19" ht="18" customHeight="1">
+    <row r="89" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="21" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="90" spans="1:19">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A90" s="56" t="s">
         <v>27</v>
       </c>
@@ -7085,7 +7088,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="91" spans="1:19" ht="18.75" customHeight="1">
+    <row r="91" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="56" t="s">
         <v>188</v>
       </c>
@@ -7104,7 +7107,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="92" spans="1:19" ht="18.75" customHeight="1">
+    <row r="92" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="56" t="s">
         <v>188</v>
       </c>
@@ -7123,7 +7126,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="93" spans="1:19" ht="18.75" customHeight="1">
+    <row r="93" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="56" t="s">
         <v>188</v>
       </c>
@@ -7142,7 +7145,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="94" spans="1:19" ht="18.75" customHeight="1">
+    <row r="94" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="56" t="s">
         <v>189</v>
       </c>
@@ -7161,7 +7164,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="95" spans="1:19" ht="18.75" customHeight="1">
+    <row r="95" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="56" t="s">
         <v>189</v>
       </c>
@@ -7180,7 +7183,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="96" spans="1:19" ht="18.75" customHeight="1">
+    <row r="96" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="56" t="s">
         <v>189</v>
       </c>
@@ -7199,13 +7202,13 @@
         <v>205</v>
       </c>
     </row>
-    <row r="97" spans="1:17" ht="18.75" customHeight="1">
+    <row r="97" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="56"/>
       <c r="B97" s="56"/>
       <c r="C97" s="7"/>
       <c r="D97" s="7"/>
     </row>
-    <row r="98" spans="1:17" ht="18.75" customHeight="1">
+    <row r="98" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="21" t="s">
         <v>224</v>
       </c>
@@ -7213,7 +7216,7 @@
       <c r="C98" s="7"/>
       <c r="D98" s="7"/>
     </row>
-    <row r="99" spans="1:17" ht="18.75" customHeight="1">
+    <row r="99" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="56"/>
       <c r="B99" s="56" t="s">
         <v>28</v>
@@ -7223,7 +7226,7 @@
       </c>
       <c r="D99" s="7"/>
     </row>
-    <row r="100" spans="1:17" ht="18.75" customHeight="1">
+    <row r="100" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="56" t="s">
         <v>30</v>
       </c>
@@ -7237,7 +7240,7 @@
       </c>
       <c r="D100" s="7"/>
     </row>
-    <row r="101" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
+    <row r="101" spans="1:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="56" t="s">
         <v>32</v>
       </c>
@@ -7250,7 +7253,7 @@
         <v>46648</v>
       </c>
     </row>
-    <row r="102" spans="1:17">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.2">
       <c r="F102" s="38" t="s">
         <v>28</v>
       </c>
@@ -7288,7 +7291,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="103" spans="1:17" ht="18" customHeight="1">
+    <row r="103" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="21" t="s">
         <v>86</v>
       </c>
@@ -7329,7 +7332,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="104" spans="1:17" ht="18" customHeight="1" thickBot="1">
+    <row r="104" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="56" t="s">
         <v>27</v>
       </c>
@@ -7371,7 +7374,7 @@
       <c r="P104" s="26"/>
       <c r="Q104" s="29"/>
     </row>
-    <row r="105" spans="1:17" ht="18.75" customHeight="1">
+    <row r="105" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="56" t="s">
         <v>188</v>
       </c>
@@ -7379,12 +7382,12 @@
         <v>75</v>
       </c>
       <c r="C105" s="7">
-        <f>IF(N105&lt;1, J105/(1-N105^2*(1-J105/C91)), C91)</f>
-        <v>7632.8953688240254</v>
+        <f t="shared" ref="C105:D110" si="3">IF(N105&lt;1, J105/(1-N105^2*(1-J105/C91)), C91)</f>
+        <v>7874.8617574285854</v>
       </c>
       <c r="D105" s="7">
-        <f>IF(O105&lt;1, K105/(1-O105^2*(1-K105/D91)), D91)</f>
-        <v>8315.7449091231047</v>
+        <f t="shared" si="3"/>
+        <v>9413.6407212070608</v>
       </c>
       <c r="E105" s="8" t="s">
         <v>205</v>
@@ -7398,11 +7401,11 @@
         <v>6.470985610616304</v>
       </c>
       <c r="H105" s="24">
-        <f t="shared" ref="H105:I110" si="3">(SQRT(2*d*F105+1) - 1)/F105</f>
+        <f t="shared" ref="H105:I110" si="4">(SQRT(2*d*F105+1) - 1)/F105</f>
         <v>2.2151227422204598</v>
       </c>
       <c r="I105" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.8365814228723776</v>
       </c>
       <c r="J105" s="25">
@@ -7413,20 +7416,21 @@
         <f>MIN(l_1m * 12*I105^3/3+n*D82*(d-I105)^2,D91)</f>
         <v>4176.0024486993134</v>
       </c>
-      <c r="L105" s="25">
-        <v>177</v>
+      <c r="L105" s="23">
+        <f>f_r*C91/y_t* 1 / 12000</f>
+        <v>176.70598461851824</v>
       </c>
       <c r="M105" s="25">
-        <f>f_r*D91/y_t * 1 / 12000</f>
+        <f t="shared" ref="M105:M110" si="5">f_r*D91/y_t * 1 / 12000</f>
         <v>176.70598461851824</v>
       </c>
       <c r="N105" s="24">
-        <f>IF((D57+D60)=0, 1.1, L105/(D57+D60))</f>
-        <v>0.49377830233757947</v>
+        <f t="shared" ref="N105:O107" si="6">IF((D57+D60)=0, 1.1, L105/(D57+D60))</f>
+        <v>0.52115013266026999</v>
       </c>
       <c r="O105" s="24">
-        <f>IF((E57+E60)=0, 1.1, M105/(E57+E60))</f>
-        <v>0.73943712794764704</v>
+        <f t="shared" si="6"/>
+        <v>0.78172519899040482</v>
       </c>
       <c r="P105" s="24">
         <f>C82/(l_1c*d)</f>
@@ -7437,7 +7441,7 @@
         <v>2.58E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:17" ht="18.75" customHeight="1">
+    <row r="106" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="56" t="s">
         <v>188</v>
       </c>
@@ -7445,11 +7449,11 @@
         <v>76</v>
       </c>
       <c r="C106" s="7">
-        <f>IF(N106&lt;1, J106/(1-N106^2*(1-J106/C92)), C92)</f>
-        <v>35890.036145126192</v>
+        <f t="shared" si="3"/>
+        <v>61684.775215579633</v>
       </c>
       <c r="D106" s="7">
-        <f>IF(O106&lt;1, K106/(1-O106^2*(1-K106/D92)), D92)</f>
+        <f t="shared" si="3"/>
         <v>46648</v>
       </c>
       <c r="E106" s="8" t="s">
@@ -7468,7 +7472,7 @@
         <v>2.2321515926606925</v>
       </c>
       <c r="I106" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.7680060470309131</v>
       </c>
       <c r="J106" s="23">
@@ -7484,15 +7488,15 @@
         <v>276.10310096643474</v>
       </c>
       <c r="M106" s="23">
-        <f>f_r*D92/y_t * 1 / 12000</f>
+        <f t="shared" si="5"/>
         <v>176.70598461851824</v>
       </c>
       <c r="N106" s="22">
-        <f>IF((D58+D61)=0, 1.1, L106/(D58+D61))</f>
-        <v>0.92429640993455897</v>
+        <f t="shared" si="6"/>
+        <v>0.97715649873800592</v>
       </c>
       <c r="O106" s="22">
-        <f>IF((E58+E61)=0, 1.1, M106/(E58+E61))</f>
+        <f t="shared" si="6"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="P106" s="22">
@@ -7504,7 +7508,7 @@
         <v>2.3760000000000007E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:17" ht="18.75" customHeight="1">
+    <row r="107" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="56" t="s">
         <v>188</v>
       </c>
@@ -7512,12 +7516,12 @@
         <v>77</v>
       </c>
       <c r="C107" s="7">
-        <f>IF(N107&lt;1, J107/(1-N107^2*(1-J107/C93)), C93)</f>
-        <v>15668.93444982568</v>
+        <f t="shared" si="3"/>
+        <v>16084.270712410156</v>
       </c>
       <c r="D107" s="7">
-        <f>IF(O107&lt;1, K107/(1-O107^2*(1-K107/D93)), D93)</f>
-        <v>13288.198723877413</v>
+        <f t="shared" si="3"/>
+        <v>18599.486494407964</v>
       </c>
       <c r="E107" s="8" t="s">
         <v>205</v>
@@ -7535,7 +7539,7 @@
         <v>2.8699877039560753</v>
       </c>
       <c r="I107" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.7680060470309131</v>
       </c>
       <c r="J107" s="23">
@@ -7551,16 +7555,16 @@
         <v>276.10310096643474</v>
       </c>
       <c r="M107" s="23">
-        <f>f_r*D93/y_t * 1 / 12000</f>
+        <f t="shared" si="5"/>
         <v>176.70598461851824</v>
       </c>
       <c r="N107" s="22">
-        <f>IF((D59+D62)=0, 1.1, L107/(D59+D62))</f>
-        <v>0.45774679349140063</v>
+        <f t="shared" si="6"/>
+        <v>0.48392512318453645</v>
       </c>
       <c r="O107" s="22">
-        <f>IF((E59+E62)=0, 1.1, M107/(E59+E62))</f>
-        <v>0.87887384350348929</v>
+        <f t="shared" si="6"/>
+        <v>0.92913623651430988</v>
       </c>
       <c r="P107" s="22">
         <f>C84/(l_1c*d)</f>
@@ -7571,7 +7575,7 @@
         <v>2.3760000000000007E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:17" ht="18.75" customHeight="1">
+    <row r="108" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="56" t="s">
         <v>189</v>
       </c>
@@ -7579,11 +7583,11 @@
         <v>75</v>
       </c>
       <c r="C108" s="7">
-        <f>IF(N108&lt;1, J108/(1-N108^2*(1-J108/C94)), C94)</f>
-        <v>8224.1243014172051</v>
+        <f t="shared" si="3"/>
+        <v>9262.7209415245434</v>
       </c>
       <c r="D108" s="7">
-        <f>IF(O108&lt;1, K108/(1-O108^2*(1-K108/D94)), D94)</f>
+        <f t="shared" si="3"/>
         <v>46648</v>
       </c>
       <c r="E108" s="8" t="s">
@@ -7598,11 +7602,11 @@
         <v>7.0265752842550766</v>
       </c>
       <c r="H108" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.8444394963833231</v>
       </c>
       <c r="I108" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.7680060470309131</v>
       </c>
       <c r="J108" s="23">
@@ -7618,16 +7622,16 @@
         <v>176.70598461851824</v>
       </c>
       <c r="M108" s="23">
-        <f>f_r*D94/y_t * 1 / 12000</f>
+        <f t="shared" si="5"/>
         <v>176.70598461851824</v>
       </c>
       <c r="N108" s="22">
-        <f>IF((D63+D66)=0, 1.1, L108/(D63+D66))</f>
-        <v>0.73239486958624112</v>
+        <f t="shared" ref="N108:O110" si="7">IF((D63+D66)=0, 1.1, L108/(D63+D66))</f>
+        <v>0.7742801970952583</v>
       </c>
       <c r="O108" s="22">
-        <f>IF((E63+E66)=0, 1.1, M108/(E63+E66))</f>
-        <v>1.0985923043793615</v>
+        <f t="shared" si="7"/>
+        <v>1.1614202956428874</v>
       </c>
       <c r="P108" s="22">
         <f>C85/(l_2c*d)</f>
@@ -7638,7 +7642,7 @@
         <v>2.3760000000000007E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:17" ht="18.75" customHeight="1">
+    <row r="109" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="56" t="s">
         <v>189</v>
       </c>
@@ -7646,12 +7650,12 @@
         <v>76</v>
       </c>
       <c r="C109" s="7">
-        <f>IF(N109&lt;1, J109/(1-N109^2*(1-J109/C95)), C95)</f>
-        <v>15258.022394227726</v>
+        <f t="shared" si="3"/>
+        <v>15753.350109341574</v>
       </c>
       <c r="D109" s="7">
-        <f>IF(O109&lt;1, K109/(1-O109^2*(1-K109/D95)), D95)</f>
-        <v>21704.927967948592</v>
+        <f t="shared" si="3"/>
+        <v>46648</v>
       </c>
       <c r="E109" s="8" t="s">
         <v>205</v>
@@ -7669,7 +7673,7 @@
         <v>2.7753524617466026</v>
       </c>
       <c r="I109" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.7680060470309131</v>
       </c>
       <c r="J109" s="23">
@@ -7685,16 +7689,16 @@
         <v>276.10310096643474</v>
       </c>
       <c r="M109" s="23">
-        <f>f_r*D95/y_t * 1 / 12000</f>
+        <f t="shared" si="5"/>
         <v>176.70598461851824</v>
       </c>
       <c r="N109" s="22">
-        <f>IF((D64+D67)=0, 1.1, L109/(D64+D67))</f>
-        <v>0.49295808529843144</v>
+        <f t="shared" si="7"/>
+        <v>0.52115013266026988</v>
       </c>
       <c r="O109" s="22">
-        <f>IF((E64+E67)=0, 1.1, M109/(E64+E67))</f>
-        <v>0.94647952377298838</v>
+        <f t="shared" si="7"/>
+        <v>1.0006082547077182</v>
       </c>
       <c r="P109" s="22">
         <f>C86/(l_2c*d)</f>
@@ -7705,7 +7709,7 @@
         <v>2.3760000000000007E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:17" ht="19.5" customHeight="1" thickBot="1">
+    <row r="110" spans="1:17" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="56" t="s">
         <v>189</v>
       </c>
@@ -7713,12 +7717,12 @@
         <v>77</v>
       </c>
       <c r="C110" s="7">
-        <f>IF(N110&lt;1, J110/(1-N110^2*(1-J110/C96)), C96)</f>
-        <v>15258.022394227726</v>
+        <f t="shared" si="3"/>
+        <v>15753.350109341574</v>
       </c>
       <c r="D110" s="7">
-        <f>IF(O110&lt;1, K110/(1-O110^2*(1-K110/D96)), D96)</f>
-        <v>21704.927967948592</v>
+        <f t="shared" si="3"/>
+        <v>46648</v>
       </c>
       <c r="E110" s="8" t="s">
         <v>205</v>
@@ -7736,7 +7740,7 @@
         <v>2.7753524617466026</v>
       </c>
       <c r="I110" s="35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.7680060470309131</v>
       </c>
       <c r="J110" s="36">
@@ -7752,16 +7756,16 @@
         <v>276.10310096643474</v>
       </c>
       <c r="M110" s="36">
-        <f>f_r*D96/y_t * 1 / 12000</f>
+        <f t="shared" si="5"/>
         <v>176.70598461851824</v>
       </c>
       <c r="N110" s="35">
-        <f>IF((D65+D68)=0, 1.1, L110/(D65+D68))</f>
-        <v>0.49295808529843144</v>
+        <f t="shared" si="7"/>
+        <v>0.52115013266026988</v>
       </c>
       <c r="O110" s="35">
-        <f>IF((E65+E68)=0, 1.1, M110/(E65+E68))</f>
-        <v>0.94647952377298838</v>
+        <f t="shared" si="7"/>
+        <v>1.0006082547077182</v>
       </c>
       <c r="P110" s="35">
         <f>C87/(l_2c*d)</f>
@@ -7772,12 +7776,12 @@
         <v>2.3760000000000007E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:17" ht="18" customHeight="1">
+    <row r="112" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="21" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="56" t="s">
         <v>27</v>
       </c>
@@ -7788,70 +7792,70 @@
         <v>29</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="18.75" customHeight="1">
+    <row r="114" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="56" t="s">
         <v>188</v>
       </c>
       <c r="B114" s="7">
         <f>0.7*C105+ 0.15*SUM(C106:C107)</f>
-        <v>13076.872347419598</v>
+        <v>17177.760119398477</v>
       </c>
       <c r="C114" s="7">
         <f>0.7*D105+ 0.15*SUM(D106:D107)</f>
-        <v>14811.451244967786</v>
+        <v>16376.671479006134</v>
       </c>
       <c r="D114" s="8" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="18.75" customHeight="1">
+    <row r="115" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="56" t="s">
         <v>189</v>
       </c>
       <c r="B115" s="7">
         <f>0.7*C108+ 0.15*SUM(C109:C110)</f>
-        <v>10334.29372926036</v>
+        <v>11209.909691869652</v>
       </c>
       <c r="C115" s="7">
         <f>0.7*D108+ 0.15*SUM(D109:D110)</f>
-        <v>39165.078390384573</v>
+        <v>46648</v>
       </c>
       <c r="D115" s="8" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="56"/>
       <c r="B116" s="56"/>
     </row>
-    <row r="117" spans="1:5" ht="18" customHeight="1">
+    <row r="117" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="21" t="s">
         <v>207</v>
       </c>
       <c r="B117" s="56"/>
     </row>
-    <row r="118" spans="1:5" ht="18.75" customHeight="1">
+    <row r="118" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
         <v>209</v>
       </c>
       <c r="B118" s="7">
         <f>(B114+C114+B115+C115)/2</f>
-        <v>38693.84785601616</v>
+        <v>45706.170645137128</v>
       </c>
       <c r="C118" s="8" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="56"/>
       <c r="B119" s="56"/>
     </row>
-    <row r="120" spans="1:5" ht="18" customHeight="1">
+    <row r="120" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="21" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="18.75" customHeight="1">
+    <row r="121" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>210</v>
       </c>
@@ -7863,21 +7867,21 @@
         <v>205</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="18" customHeight="1">
+    <row r="123" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="52" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="18" customHeight="1">
+    <row r="124" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>212</v>
       </c>
       <c r="B124" s="10">
         <f>B118/B121</f>
-        <v>0.36286454765262721</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" ht="19.5" customHeight="1" thickBot="1">
+        <v>0.42862495861865535</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="52" t="s">
         <v>100</v>
       </c>
@@ -7885,7 +7889,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="127" spans="1:5" ht="18" customHeight="1">
+    <row r="127" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
         <v>213</v>
       </c>
@@ -7900,7 +7904,7 @@
         <v>7.12</v>
       </c>
     </row>
-    <row r="128" spans="1:5" ht="18.75" customHeight="1">
+    <row r="128" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="11" t="s">
         <v>214</v>
       </c>
@@ -7919,12 +7923,12 @@
         <v>8.92</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="18" customHeight="1" thickBot="1">
+    <row r="129" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A129" s="11" t="s">
         <v>104</v>
       </c>
       <c r="B129" s="4">
-        <f>(SW+SDL+LLvib)/32.2</f>
+        <f>(R12 / 12 * w_c +SDL+LLvib)/32.2</f>
         <v>6.2292960662525889</v>
       </c>
       <c r="C129" s="8" t="s">
@@ -7937,24 +7941,24 @@
         <v>9.2899999999999991</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="18" customHeight="1">
+    <row r="130" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
         <v>106</v>
       </c>
       <c r="B130" s="4">
-        <f>k_2*lambda_i_sq / (2 * PI() * l_1^2) * SQRT(k_1 * E_c*144*(h/12)^3 / (12*gamma*(1-nu^2)))</f>
-        <v>5.6609752730228546</v>
+        <f>k_2*lambda_i_sq / (2 * PI() * l_1^2) * SQRT(k_1 * E_c*144*(R12/12)^3 / (12*gamma*(1-nu^2)))</f>
+        <v>6.1525863330777328</v>
       </c>
       <c r="C130" s="8" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="21" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="133" spans="1:5">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
         <v>109</v>
       </c>
@@ -7966,7 +7970,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="134" spans="1:5">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" s="11" t="s">
         <v>216</v>
       </c>
@@ -7981,22 +7985,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="8" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" style="8" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="52" t="s">
         <v>145</v>
       </c>
@@ -8004,10 +8008,10 @@
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="1:15" ht="18" customHeight="1">
+    <row r="3" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>146</v>
       </c>
@@ -8021,7 +8025,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>109</v>
       </c>
@@ -8033,7 +8037,7 @@
       </c>
       <c r="I4" s="8"/>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>216</v>
       </c>
@@ -8042,10 +8046,10 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="11"/>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="52" t="s">
         <v>147</v>
       </c>
@@ -8060,7 +8064,7 @@
       </c>
       <c r="M7" s="8"/>
     </row>
-    <row r="8" spans="1:15" ht="18" customHeight="1">
+    <row r="8" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="56" t="s">
         <v>151</v>
       </c>
@@ -8099,7 +8103,7 @@
       </c>
       <c r="M8" s="8"/>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="56"/>
       <c r="B9" s="56" t="s">
         <v>107</v>
@@ -8136,7 +8140,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="56" t="s">
         <v>129</v>
       </c>
@@ -8184,7 +8188,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="56" t="s">
         <v>130</v>
       </c>
@@ -8238,7 +8242,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="56" t="s">
         <v>131</v>
       </c>
@@ -8289,7 +8293,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="56" t="s">
         <v>132</v>
       </c>
@@ -8340,7 +8344,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="M14" s="52"/>
     </row>
   </sheetData>
@@ -8350,35 +8354,35 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EB7F394-EE42-4FAF-93E6-B2553F751B52}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.83203125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="18" customHeight="1">
+    <row r="1" spans="1:35" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="56" t="s">
         <v>112</v>
       </c>
@@ -8482,7 +8486,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="18" customHeight="1">
+    <row r="2" spans="1:35" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>133</v>
       </c>
@@ -8587,7 +8591,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A3"/>
       <c r="B3" s="59"/>
       <c r="C3" s="59"/>
@@ -8621,7 +8625,7 @@
       <c r="AH3" s="56"/>
       <c r="AI3" s="56"/>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A4"/>
       <c r="B4" s="59"/>
       <c r="C4" s="59"/>
@@ -8655,7 +8659,7 @@
       <c r="AH4" s="56"/>
       <c r="AI4" s="56"/>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5"/>
       <c r="B5" s="59"/>
       <c r="C5" s="59"/>
@@ -8689,7 +8693,7 @@
       <c r="AH5" s="56"/>
       <c r="AI5" s="56"/>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A6"/>
       <c r="B6" s="59"/>
       <c r="C6" s="59"/>
@@ -8723,7 +8727,7 @@
       <c r="AH6" s="56"/>
       <c r="AI6" s="56"/>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A7"/>
       <c r="B7" s="59"/>
       <c r="C7" s="59"/>
@@ -8757,7 +8761,7 @@
       <c r="AH7" s="56"/>
       <c r="AI7" s="56"/>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A8"/>
       <c r="B8" s="59"/>
       <c r="C8" s="59"/>
@@ -8791,7 +8795,7 @@
       <c r="AH8" s="56"/>
       <c r="AI8" s="56"/>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A9"/>
       <c r="B9" s="59"/>
       <c r="C9" s="59"/>
@@ -8825,7 +8829,7 @@
       <c r="AH9" s="56"/>
       <c r="AI9" s="56"/>
     </row>
-    <row r="10" spans="1:35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A10"/>
       <c r="B10" s="59"/>
       <c r="C10" s="59"/>
@@ -8859,7 +8863,7 @@
       <c r="AH10" s="56"/>
       <c r="AI10" s="56"/>
     </row>
-    <row r="11" spans="1:35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A11"/>
       <c r="B11" s="59"/>
       <c r="C11" s="59"/>
@@ -8893,7 +8897,7 @@
       <c r="AH11" s="56"/>
       <c r="AI11" s="56"/>
     </row>
-    <row r="12" spans="1:35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A12"/>
       <c r="B12" s="59"/>
       <c r="C12" s="59"/>
@@ -8927,7 +8931,7 @@
       <c r="AH12" s="56"/>
       <c r="AI12" s="56"/>
     </row>
-    <row r="13" spans="1:35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A13"/>
       <c r="B13" s="59"/>
       <c r="C13" s="59"/>
@@ -8961,7 +8965,7 @@
       <c r="AH13" s="56"/>
       <c r="AI13" s="56"/>
     </row>
-    <row r="14" spans="1:35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A14"/>
       <c r="B14" s="59"/>
       <c r="C14" s="59"/>
@@ -8995,7 +8999,7 @@
       <c r="AH14" s="56"/>
       <c r="AI14" s="56"/>
     </row>
-    <row r="15" spans="1:35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A15"/>
       <c r="B15" s="59"/>
       <c r="C15" s="59"/>
@@ -9029,7 +9033,7 @@
       <c r="AH15" s="56"/>
       <c r="AI15" s="56"/>
     </row>
-    <row r="16" spans="1:35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A16"/>
       <c r="B16" s="59"/>
       <c r="C16" s="59"/>
@@ -9063,7 +9067,7 @@
       <c r="AH16" s="56"/>
       <c r="AI16" s="56"/>
     </row>
-    <row r="17" spans="1:35">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A17"/>
       <c r="B17" s="59"/>
       <c r="C17" s="59"/>
@@ -9097,7 +9101,7 @@
       <c r="AH17" s="56"/>
       <c r="AI17" s="56"/>
     </row>
-    <row r="18" spans="1:35">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A18"/>
       <c r="B18" s="59"/>
       <c r="C18" s="59"/>
@@ -9131,7 +9135,7 @@
       <c r="AH18" s="56"/>
       <c r="AI18" s="56"/>
     </row>
-    <row r="19" spans="1:35">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A19"/>
       <c r="B19" s="59"/>
       <c r="C19" s="59"/>
@@ -9165,7 +9169,7 @@
       <c r="AH19" s="56"/>
       <c r="AI19" s="56"/>
     </row>
-    <row r="20" spans="1:35">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A20"/>
       <c r="B20" s="59"/>
       <c r="C20" s="59"/>
@@ -9199,7 +9203,7 @@
       <c r="AH20" s="56"/>
       <c r="AI20" s="56"/>
     </row>
-    <row r="21" spans="1:35">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A21"/>
       <c r="B21" s="59"/>
       <c r="C21" s="59"/>
@@ -9233,7 +9237,7 @@
       <c r="AH21" s="56"/>
       <c r="AI21" s="56"/>
     </row>
-    <row r="22" spans="1:35">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A22"/>
       <c r="B22" s="59"/>
       <c r="C22" s="59"/>
@@ -9267,7 +9271,7 @@
       <c r="AH22" s="56"/>
       <c r="AI22" s="56"/>
     </row>
-    <row r="23" spans="1:35">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A23"/>
       <c r="B23" s="59"/>
       <c r="C23" s="59"/>
@@ -9301,7 +9305,7 @@
       <c r="AH23" s="56"/>
       <c r="AI23" s="56"/>
     </row>
-    <row r="24" spans="1:35">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A24"/>
       <c r="B24" s="59"/>
       <c r="C24" s="59"/>
@@ -9335,7 +9339,7 @@
       <c r="AH24" s="56"/>
       <c r="AI24" s="56"/>
     </row>
-    <row r="25" spans="1:35">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A25"/>
       <c r="B25" s="59"/>
       <c r="C25" s="59"/>
@@ -9369,7 +9373,7 @@
       <c r="AH25" s="56"/>
       <c r="AI25" s="56"/>
     </row>
-    <row r="26" spans="1:35">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A26"/>
       <c r="B26" s="59"/>
       <c r="C26" s="59"/>
@@ -9403,7 +9407,7 @@
       <c r="AH26" s="56"/>
       <c r="AI26" s="56"/>
     </row>
-    <row r="27" spans="1:35">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A27"/>
       <c r="B27" s="59"/>
       <c r="C27" s="59"/>
@@ -9437,7 +9441,7 @@
       <c r="AH27" s="56"/>
       <c r="AI27" s="56"/>
     </row>
-    <row r="28" spans="1:35">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A28"/>
       <c r="B28" s="59"/>
       <c r="C28" s="59"/>
@@ -9471,7 +9475,7 @@
       <c r="AH28" s="56"/>
       <c r="AI28" s="56"/>
     </row>
-    <row r="29" spans="1:35">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A29"/>
       <c r="B29" s="59"/>
       <c r="C29" s="59"/>
@@ -9505,7 +9509,7 @@
       <c r="AH29" s="56"/>
       <c r="AI29" s="56"/>
     </row>
-    <row r="30" spans="1:35">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A30"/>
       <c r="B30" s="59"/>
       <c r="C30" s="59"/>
@@ -9539,7 +9543,7 @@
       <c r="AH30" s="56"/>
       <c r="AI30" s="56"/>
     </row>
-    <row r="31" spans="1:35">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A31"/>
       <c r="B31" s="59"/>
       <c r="C31" s="59"/>
@@ -9573,7 +9577,7 @@
       <c r="AH31" s="56"/>
       <c r="AI31" s="56"/>
     </row>
-    <row r="32" spans="1:35">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A32"/>
       <c r="B32" s="59"/>
       <c r="C32" s="59"/>
@@ -9607,7 +9611,7 @@
       <c r="AH32" s="56"/>
       <c r="AI32" s="56"/>
     </row>
-    <row r="33" spans="1:35">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A33"/>
       <c r="B33" s="59"/>
       <c r="C33" s="59"/>
@@ -9641,7 +9645,7 @@
       <c r="AH33" s="56"/>
       <c r="AI33" s="56"/>
     </row>
-    <row r="34" spans="1:35">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A34"/>
       <c r="B34" s="59"/>
       <c r="C34" s="59"/>
@@ -9675,7 +9679,7 @@
       <c r="AH34" s="56"/>
       <c r="AI34" s="56"/>
     </row>
-    <row r="35" spans="1:35">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A35"/>
       <c r="B35" s="59"/>
       <c r="C35" s="59"/>
@@ -9709,7 +9713,7 @@
       <c r="AH35" s="56"/>
       <c r="AI35" s="56"/>
     </row>
-    <row r="36" spans="1:35">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A36"/>
       <c r="B36" s="59"/>
       <c r="C36" s="59"/>
@@ -9743,7 +9747,7 @@
       <c r="AH36" s="56"/>
       <c r="AI36" s="56"/>
     </row>
-    <row r="37" spans="1:35">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A37"/>
       <c r="B37" s="59"/>
       <c r="C37" s="59"/>
@@ -9777,7 +9781,7 @@
       <c r="AH37" s="56"/>
       <c r="AI37" s="56"/>
     </row>
-    <row r="38" spans="1:35">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A38"/>
       <c r="B38" s="59"/>
       <c r="C38" s="59"/>
@@ -9811,7 +9815,7 @@
       <c r="AH38" s="56"/>
       <c r="AI38" s="56"/>
     </row>
-    <row r="39" spans="1:35">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A39"/>
       <c r="B39" s="59"/>
       <c r="C39" s="59"/>
@@ -9845,7 +9849,7 @@
       <c r="AH39" s="56"/>
       <c r="AI39" s="56"/>
     </row>
-    <row r="40" spans="1:35">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A40"/>
       <c r="B40" s="59"/>
       <c r="C40" s="59"/>
@@ -9879,7 +9883,7 @@
       <c r="AH40" s="56"/>
       <c r="AI40" s="56"/>
     </row>
-    <row r="41" spans="1:35">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A41"/>
       <c r="B41" s="59"/>
       <c r="C41" s="59"/>
@@ -9913,7 +9917,7 @@
       <c r="AH41" s="56"/>
       <c r="AI41" s="56"/>
     </row>
-    <row r="42" spans="1:35">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A42"/>
       <c r="B42" s="59"/>
       <c r="C42" s="59"/>
@@ -9959,25 +9963,25 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q128"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A100" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="O126" sqref="O126"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" style="8" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="8" customWidth="1"/>
     <col min="5" max="5" width="12" style="8" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="8" customWidth="1"/>
-    <col min="8" max="9" width="11.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="8" customWidth="1"/>
+    <col min="8" max="9" width="11.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="11.5" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="52" t="s">
         <v>0</v>
       </c>
@@ -9985,7 +9989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18" customHeight="1">
+    <row r="3" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -10002,7 +10006,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18" customHeight="1">
+    <row r="4" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -10016,7 +10020,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18" customHeight="1">
+    <row r="5" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -10028,7 +10032,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1">
+    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -10039,7 +10043,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1">
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
@@ -10050,7 +10054,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -10058,7 +10062,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
@@ -10069,7 +10073,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="18" customHeight="1">
+    <row r="10" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
@@ -10080,7 +10084,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="18" customHeight="1">
+    <row r="11" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
@@ -10095,7 +10099,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
@@ -10106,7 +10110,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
@@ -10117,7 +10121,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="18" customHeight="1">
+    <row r="14" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
@@ -10128,7 +10132,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="18" customHeight="1">
+    <row r="15" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
@@ -10140,7 +10144,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
@@ -10149,7 +10153,7 @@
         <v>5.9315173688353893</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="18" customHeight="1">
+    <row r="17" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>24</v>
       </c>
@@ -10158,7 +10162,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="18" customHeight="1">
+    <row r="18" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>25</v>
       </c>
@@ -10170,15 +10174,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="21" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>27</v>
       </c>
@@ -10189,7 +10193,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="18" customHeight="1">
+    <row r="22" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>30</v>
       </c>
@@ -10208,7 +10212,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="18" customHeight="1">
+    <row r="23" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>32</v>
       </c>
@@ -10224,12 +10228,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>34</v>
       </c>
@@ -10240,7 +10244,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>36</v>
       </c>
@@ -10251,7 +10255,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="18" customHeight="1">
+    <row r="28" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>37</v>
       </c>
@@ -10262,7 +10266,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>38</v>
       </c>
@@ -10274,7 +10278,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="17.25" customHeight="1">
+    <row r="30" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>39</v>
       </c>
@@ -10286,7 +10290,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>41</v>
       </c>
@@ -10298,11 +10302,11 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="6"/>
     </row>
-    <row r="33" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
+    <row r="33" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
         <v>43</v>
       </c>
@@ -10313,7 +10317,7 @@
       <c r="G33" s="54"/>
       <c r="H33" s="55"/>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="F34" s="45" t="s">
         <v>45</v>
@@ -10340,7 +10344,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="18" customHeight="1">
+    <row r="35" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="21" t="s">
         <v>47</v>
       </c>
@@ -10369,7 +10373,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="18.75" customHeight="1" thickBot="1">
+    <row r="36" spans="1:14" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>48</v>
       </c>
@@ -10405,7 +10409,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="18" customHeight="1">
+    <row r="37" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>52</v>
       </c>
@@ -10444,7 +10448,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="18" customHeight="1">
+    <row r="38" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>55</v>
       </c>
@@ -10486,7 +10490,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="18.75" customHeight="1" thickBot="1">
+    <row r="39" spans="1:14" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E39" s="3" t="s">
         <v>58</v>
       </c>
@@ -10515,7 +10519,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>59</v>
       </c>
@@ -10536,7 +10540,7 @@
       <c r="L40" s="56"/>
       <c r="M40" s="56"/>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>60</v>
       </c>
@@ -10557,7 +10561,7 @@
       <c r="L41" s="56"/>
       <c r="M41" s="56"/>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>61</v>
       </c>
@@ -10578,7 +10582,7 @@
       <c r="L42" s="56"/>
       <c r="M42" s="56"/>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>62</v>
       </c>
@@ -10599,7 +10603,7 @@
       <c r="L43" s="56"/>
       <c r="M43" s="56"/>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>63</v>
       </c>
@@ -10620,7 +10624,7 @@
       <c r="L44" s="56"/>
       <c r="M44" s="56"/>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>64</v>
       </c>
@@ -10641,7 +10645,7 @@
       <c r="L45" s="56"/>
       <c r="M45" s="56"/>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E46" s="3"/>
       <c r="F46" s="56"/>
       <c r="G46" s="56"/>
@@ -10652,7 +10656,7 @@
       <c r="L46" s="56"/>
       <c r="M46" s="56"/>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="21" t="s">
         <v>65</v>
       </c>
@@ -10666,7 +10670,7 @@
       <c r="L47" s="56"/>
       <c r="M47" s="56"/>
     </row>
-    <row r="48" spans="1:14" ht="18" customHeight="1">
+    <row r="48" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>66</v>
       </c>
@@ -10687,7 +10691,7 @@
       <c r="L48" s="56"/>
       <c r="M48" s="56"/>
     </row>
-    <row r="49" spans="1:13" ht="18" customHeight="1">
+    <row r="49" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>68</v>
       </c>
@@ -10708,7 +10712,7 @@
       <c r="L49" s="56"/>
       <c r="M49" s="56"/>
     </row>
-    <row r="50" spans="1:13" ht="18" customHeight="1">
+    <row r="50" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>69</v>
       </c>
@@ -10729,7 +10733,7 @@
       <c r="L50" s="56"/>
       <c r="M50" s="56"/>
     </row>
-    <row r="51" spans="1:13" ht="18" customHeight="1">
+    <row r="51" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>70</v>
       </c>
@@ -10750,7 +10754,7 @@
       <c r="L51" s="56"/>
       <c r="M51" s="56"/>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="3"/>
       <c r="B52" s="7"/>
       <c r="E52" s="3"/>
@@ -10763,12 +10767,12 @@
       <c r="L52" s="56"/>
       <c r="M52" s="56"/>
     </row>
-    <row r="53" spans="1:13" ht="18" customHeight="1">
+    <row r="53" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="21" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="56" t="s">
         <v>27</v>
       </c>
@@ -10785,7 +10789,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="18" customHeight="1">
+    <row r="55" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="56" t="s">
         <v>30</v>
       </c>
@@ -10807,7 +10811,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="18" customHeight="1">
+    <row r="56" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="56" t="s">
         <v>30</v>
       </c>
@@ -10829,7 +10833,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="18" customHeight="1">
+    <row r="57" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="56" t="s">
         <v>30</v>
       </c>
@@ -10851,7 +10855,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="18" customHeight="1">
+    <row r="58" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="56" t="s">
         <v>30</v>
       </c>
@@ -10873,7 +10877,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="18" customHeight="1">
+    <row r="59" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="56" t="s">
         <v>30</v>
       </c>
@@ -10895,7 +10899,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="18" customHeight="1">
+    <row r="60" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="56" t="s">
         <v>30</v>
       </c>
@@ -10917,7 +10921,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="18" customHeight="1">
+    <row r="61" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="56" t="s">
         <v>32</v>
       </c>
@@ -10939,7 +10943,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="18" customHeight="1">
+    <row r="62" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="56" t="s">
         <v>32</v>
       </c>
@@ -10961,7 +10965,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="18" customHeight="1">
+    <row r="63" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="56" t="s">
         <v>32</v>
       </c>
@@ -10983,7 +10987,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="18" customHeight="1">
+    <row r="64" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="56" t="s">
         <v>32</v>
       </c>
@@ -11005,7 +11009,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="18" customHeight="1">
+    <row r="65" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="56" t="s">
         <v>32</v>
       </c>
@@ -11027,7 +11031,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="18" customHeight="1">
+    <row r="66" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="56" t="s">
         <v>32</v>
       </c>
@@ -11049,12 +11053,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="18" customHeight="1">
+    <row r="69" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="52" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="70" spans="1:12">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" s="56" t="s">
         <v>27</v>
       </c>
@@ -11068,7 +11072,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="18" customHeight="1">
+    <row r="71" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="56" t="s">
         <v>30</v>
       </c>
@@ -11087,7 +11091,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="18" customHeight="1">
+    <row r="72" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="56" t="s">
         <v>30</v>
       </c>
@@ -11106,7 +11110,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="18" customHeight="1">
+    <row r="73" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="56" t="s">
         <v>30</v>
       </c>
@@ -11125,7 +11129,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="18" customHeight="1">
+    <row r="74" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="56" t="s">
         <v>32</v>
       </c>
@@ -11144,7 +11148,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="18" customHeight="1">
+    <row r="75" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="56" t="s">
         <v>32</v>
       </c>
@@ -11163,7 +11167,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="18" customHeight="1">
+    <row r="76" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="56" t="s">
         <v>32</v>
       </c>
@@ -11182,7 +11186,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="18" customHeight="1">
+    <row r="78" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="21" t="s">
         <v>80</v>
       </c>
@@ -11190,7 +11194,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="79" spans="1:12">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" s="56" t="s">
         <v>27</v>
       </c>
@@ -11219,7 +11223,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="18.75" customHeight="1">
+    <row r="80" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="56" t="s">
         <v>30</v>
       </c>
@@ -11257,7 +11261,7 @@
       <c r="K80" s="9"/>
       <c r="L80" s="9"/>
     </row>
-    <row r="81" spans="1:17" ht="18.75" customHeight="1">
+    <row r="81" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="56" t="s">
         <v>30</v>
       </c>
@@ -11295,7 +11299,7 @@
       <c r="K81" s="9"/>
       <c r="L81" s="9"/>
     </row>
-    <row r="82" spans="1:17" ht="18.75" customHeight="1">
+    <row r="82" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="56" t="s">
         <v>30</v>
       </c>
@@ -11333,7 +11337,7 @@
       <c r="K82" s="9"/>
       <c r="L82" s="9"/>
     </row>
-    <row r="83" spans="1:17" ht="18.75" customHeight="1">
+    <row r="83" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="56" t="s">
         <v>32</v>
       </c>
@@ -11371,7 +11375,7 @@
       <c r="K83" s="9"/>
       <c r="L83" s="9"/>
     </row>
-    <row r="84" spans="1:17" ht="18.75" customHeight="1">
+    <row r="84" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="56" t="s">
         <v>32</v>
       </c>
@@ -11409,7 +11413,7 @@
       <c r="K84" s="9"/>
       <c r="L84" s="9"/>
     </row>
-    <row r="85" spans="1:17" ht="18.75" customHeight="1">
+    <row r="85" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="56" t="s">
         <v>32</v>
       </c>
@@ -11447,12 +11451,12 @@
       <c r="K85" s="9"/>
       <c r="L85" s="9"/>
     </row>
-    <row r="87" spans="1:17" ht="18" customHeight="1">
+    <row r="87" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="21" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="88" spans="1:17">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A88" s="56" t="s">
         <v>27</v>
       </c>
@@ -11466,7 +11470,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="89" spans="1:17" ht="18.75" customHeight="1">
+    <row r="89" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="56" t="s">
         <v>30</v>
       </c>
@@ -11485,7 +11489,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="90" spans="1:17" ht="18.75" customHeight="1">
+    <row r="90" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="56" t="s">
         <v>30</v>
       </c>
@@ -11504,7 +11508,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="91" spans="1:17" ht="18.75" customHeight="1">
+    <row r="91" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="56" t="s">
         <v>30</v>
       </c>
@@ -11523,7 +11527,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="92" spans="1:17" ht="18.75" customHeight="1">
+    <row r="92" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="56" t="s">
         <v>32</v>
       </c>
@@ -11542,7 +11546,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="93" spans="1:17" ht="18.75" customHeight="1">
+    <row r="93" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="56" t="s">
         <v>32</v>
       </c>
@@ -11561,7 +11565,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="94" spans="1:17" ht="18.75" customHeight="1">
+    <row r="94" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="56" t="s">
         <v>32</v>
       </c>
@@ -11580,8 +11584,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="95" spans="1:17" ht="15.75" customHeight="1" thickBot="1"/>
-    <row r="96" spans="1:17">
+    <row r="95" spans="1:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.2">
       <c r="F96" s="38" t="s">
         <v>28</v>
       </c>
@@ -11619,7 +11623,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="97" spans="1:17" ht="18" customHeight="1">
+    <row r="97" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="21" t="s">
         <v>86</v>
       </c>
@@ -11660,7 +11664,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="98" spans="1:17" ht="18" customHeight="1" thickBot="1">
+    <row r="98" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A98" s="56" t="s">
         <v>27</v>
       </c>
@@ -11702,7 +11706,7 @@
       <c r="P98" s="26"/>
       <c r="Q98" s="29"/>
     </row>
-    <row r="99" spans="1:17" ht="18.75" customHeight="1">
+    <row r="99" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="56" t="s">
         <v>30</v>
       </c>
@@ -11769,7 +11773,7 @@
         <v>4.3944649990503321E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:17" ht="18.75" customHeight="1">
+    <row r="100" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="56" t="s">
         <v>30</v>
       </c>
@@ -11836,7 +11840,7 @@
         <v>3.0000000000000002E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:17" ht="18.75" customHeight="1">
+    <row r="101" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="56" t="s">
         <v>30</v>
       </c>
@@ -11903,7 +11907,7 @@
         <v>3.5704726064266931E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:17" ht="18.75" customHeight="1">
+    <row r="102" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="56" t="s">
         <v>32</v>
       </c>
@@ -11970,7 +11974,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="103" spans="1:17" ht="18.75" customHeight="1">
+    <row r="103" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="56" t="s">
         <v>32</v>
       </c>
@@ -12037,7 +12041,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="104" spans="1:17" ht="19.5" customHeight="1" thickBot="1">
+    <row r="104" spans="1:17" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="56" t="s">
         <v>32</v>
       </c>
@@ -12104,12 +12108,12 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="106" spans="1:17" ht="18" customHeight="1">
+    <row r="106" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="21" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="107" spans="1:17">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A107" s="56" t="s">
         <v>27</v>
       </c>
@@ -12120,7 +12124,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="108" spans="1:17" ht="18.75" customHeight="1">
+    <row r="108" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="56" t="s">
         <v>30</v>
       </c>
@@ -12136,7 +12140,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="109" spans="1:17" ht="18.75" customHeight="1">
+    <row r="109" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="56" t="s">
         <v>32</v>
       </c>
@@ -12152,17 +12156,17 @@
         <v>85</v>
       </c>
     </row>
-    <row r="110" spans="1:17">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" s="56"/>
       <c r="B110" s="56"/>
     </row>
-    <row r="111" spans="1:17" ht="18" customHeight="1">
+    <row r="111" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="21" t="s">
         <v>94</v>
       </c>
       <c r="B111" s="56"/>
     </row>
-    <row r="112" spans="1:17" ht="18.75" customHeight="1">
+    <row r="112" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>95</v>
       </c>
@@ -12174,16 +12178,16 @@
         <v>85</v>
       </c>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="56"/>
       <c r="B113" s="56"/>
     </row>
-    <row r="114" spans="1:5" ht="18" customHeight="1">
+    <row r="114" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="21" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="18.75" customHeight="1">
+    <row r="115" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>97</v>
       </c>
@@ -12195,12 +12199,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="18" customHeight="1">
+    <row r="117" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="52" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="18" customHeight="1">
+    <row r="118" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
         <v>99</v>
       </c>
@@ -12209,7 +12213,7 @@
         <v>0.54614289068960964</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="19.5" customHeight="1" thickBot="1">
+    <row r="120" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A120" s="52" t="s">
         <v>100</v>
       </c>
@@ -12217,7 +12221,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="18" customHeight="1">
+    <row r="121" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
         <v>102</v>
       </c>
@@ -12232,7 +12236,7 @@
         <v>7.12</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="18.75" customHeight="1">
+    <row r="122" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="11" t="s">
         <v>103</v>
       </c>
@@ -12251,7 +12255,7 @@
         <v>8.92</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="18" customHeight="1" thickBot="1">
+    <row r="123" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A123" s="11" t="s">
         <v>104</v>
       </c>
@@ -12269,7 +12273,7 @@
         <v>9.2899999999999991</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="18" customHeight="1">
+    <row r="124" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
         <v>106</v>
       </c>
@@ -12281,12 +12285,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="21" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
         <v>109</v>
       </c>
@@ -12298,7 +12302,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="11" t="s">
         <v>111</v>
       </c>

</xml_diff>

<commit_message>
fixed two way drop panel, still need to do significant cleanup for avoiding extraneous code
</commit_message>
<xml_diff>
--- a/Flat_Plate_Vibration_Template.xlsx
+++ b/Flat_Plate_Vibration_Template.xlsx
@@ -1,159 +1,191 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27809"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maryannewachter/workspaces/vibraslab/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mwachter\workspaces\vibraslab\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B60B392F-6317-40CD-853E-658899DD6CBC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18980" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="33600" windowHeight="18975" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Slab_Properties" sheetId="1" r:id="rId1"/>
-    <sheet name="Drop_Slab_Properties" sheetId="6" r:id="rId2"/>
-    <sheet name="AISC_DG_11_Sensitive_Equipment" sheetId="3" r:id="rId3"/>
-    <sheet name="Batch calculations -&gt;" sheetId="5" r:id="rId4"/>
-    <sheet name="Sample_Slabs" sheetId="2" r:id="rId5"/>
-    <sheet name="SSM_Example" sheetId="4" r:id="rId6"/>
+    <sheet name="FP_AISC_DG_11_Sensitive_Equip" sheetId="7" r:id="rId2"/>
+    <sheet name="Drop_Slab_Properties" sheetId="6" r:id="rId3"/>
+    <sheet name="DS_AISC_DG_11_Sensitive_Equip" sheetId="3" r:id="rId4"/>
+    <sheet name="Batch calculations -&gt;" sheetId="5" r:id="rId5"/>
+    <sheet name="Sample_Slabs" sheetId="2" r:id="rId6"/>
+    <sheet name="SSM_Example" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="c_1" localSheetId="1">Drop_Slab_Properties!$B$6</definedName>
+    <definedName name="c_1" localSheetId="2">Drop_Slab_Properties!$B$6</definedName>
+    <definedName name="c_1" localSheetId="1">#REF!</definedName>
     <definedName name="c_1" localSheetId="0">Slab_Properties!$B$6</definedName>
-    <definedName name="c_1" localSheetId="5">SSM_Example!$B$6</definedName>
+    <definedName name="c_1" localSheetId="6">SSM_Example!$B$6</definedName>
     <definedName name="c_1">#REF!</definedName>
-    <definedName name="c_2" localSheetId="1">Drop_Slab_Properties!$B$7</definedName>
+    <definedName name="c_2" localSheetId="2">Drop_Slab_Properties!$B$7</definedName>
+    <definedName name="c_2" localSheetId="1">#REF!</definedName>
     <definedName name="c_2" localSheetId="0">Slab_Properties!$B$7</definedName>
-    <definedName name="c_2" localSheetId="5">SSM_Example!$B$7</definedName>
+    <definedName name="c_2" localSheetId="6">SSM_Example!$B$7</definedName>
     <definedName name="c_2">#REF!</definedName>
-    <definedName name="d" localSheetId="1">Drop_Slab_Properties!$B$13</definedName>
+    <definedName name="d" localSheetId="2">Drop_Slab_Properties!$B$13</definedName>
+    <definedName name="d" localSheetId="1">#REF!</definedName>
     <definedName name="d" localSheetId="0">Slab_Properties!$B$13</definedName>
-    <definedName name="d" localSheetId="5">SSM_Example!$B$13</definedName>
+    <definedName name="d" localSheetId="6">SSM_Example!$B$13</definedName>
     <definedName name="d">#REF!</definedName>
     <definedName name="d_drop">Drop_Slab_Properties!$B$14</definedName>
-    <definedName name="E_c" localSheetId="1">Drop_Slab_Properties!$B$11</definedName>
+    <definedName name="E_c" localSheetId="2">Drop_Slab_Properties!$B$11</definedName>
+    <definedName name="E_c" localSheetId="1">#REF!</definedName>
     <definedName name="E_c" localSheetId="0">Slab_Properties!$B$11</definedName>
-    <definedName name="E_c" localSheetId="5">SSM_Example!$B$11</definedName>
+    <definedName name="E_c" localSheetId="6">SSM_Example!$B$11</definedName>
     <definedName name="E_c">#REF!</definedName>
-    <definedName name="f_c" localSheetId="1">Drop_Slab_Properties!$B$9</definedName>
+    <definedName name="f_c" localSheetId="2">Drop_Slab_Properties!$B$9</definedName>
+    <definedName name="f_c" localSheetId="1">#REF!</definedName>
     <definedName name="f_c" localSheetId="0">Slab_Properties!$B$9</definedName>
-    <definedName name="f_c" localSheetId="5">SSM_Example!$B$9</definedName>
+    <definedName name="f_c" localSheetId="6">SSM_Example!$B$9</definedName>
     <definedName name="f_c">#REF!</definedName>
-    <definedName name="f_n" localSheetId="1">Drop_Slab_Properties!$B$130</definedName>
-    <definedName name="f_n" localSheetId="5">SSM_Example!$B$124</definedName>
+    <definedName name="f_n" localSheetId="2">Drop_Slab_Properties!$B$130</definedName>
+    <definedName name="f_n" localSheetId="6">SSM_Example!$B$124</definedName>
     <definedName name="f_n">Slab_Properties!$B$124</definedName>
-    <definedName name="f_r" localSheetId="1">Drop_Slab_Properties!$B$20</definedName>
+    <definedName name="f_r" localSheetId="2">Drop_Slab_Properties!$B$20</definedName>
+    <definedName name="f_r" localSheetId="1">#REF!</definedName>
     <definedName name="f_r" localSheetId="0">Slab_Properties!$B$18</definedName>
-    <definedName name="f_r" localSheetId="5">SSM_Example!$B$18</definedName>
+    <definedName name="f_r" localSheetId="6">SSM_Example!$B$18</definedName>
     <definedName name="f_r">#REF!</definedName>
-    <definedName name="f_y" localSheetId="1">Drop_Slab_Properties!$B$10</definedName>
+    <definedName name="f_y" localSheetId="2">Drop_Slab_Properties!$B$10</definedName>
+    <definedName name="f_y" localSheetId="1">#REF!</definedName>
     <definedName name="f_y" localSheetId="0">Slab_Properties!$B$10</definedName>
-    <definedName name="f_y" localSheetId="5">SSM_Example!$B$10</definedName>
+    <definedName name="f_y" localSheetId="6">SSM_Example!$B$10</definedName>
     <definedName name="f_y">#REF!</definedName>
-    <definedName name="gamma" localSheetId="1">Drop_Slab_Properties!$B$129</definedName>
+    <definedName name="gamma" localSheetId="2">Drop_Slab_Properties!$B$129</definedName>
+    <definedName name="gamma" localSheetId="1">#REF!</definedName>
     <definedName name="gamma" localSheetId="0">Slab_Properties!$B$123</definedName>
-    <definedName name="gamma" localSheetId="5">SSM_Example!$B$123</definedName>
+    <definedName name="gamma" localSheetId="6">SSM_Example!$B$123</definedName>
     <definedName name="gamma">#REF!</definedName>
-    <definedName name="h" localSheetId="1">Drop_Slab_Properties!$B$12</definedName>
+    <definedName name="h" localSheetId="2">Drop_Slab_Properties!$B$12</definedName>
+    <definedName name="h" localSheetId="1">#REF!</definedName>
     <definedName name="h" localSheetId="0">Slab_Properties!$B$12</definedName>
-    <definedName name="h" localSheetId="5">SSM_Example!$B$12</definedName>
+    <definedName name="h" localSheetId="6">SSM_Example!$B$12</definedName>
     <definedName name="h">#REF!</definedName>
     <definedName name="h_drop">Drop_Slab_Properties!$K$12</definedName>
-    <definedName name="k_1" localSheetId="1">Drop_Slab_Properties!$B$124</definedName>
+    <definedName name="k_1" localSheetId="2">Drop_Slab_Properties!$B$124</definedName>
+    <definedName name="k_1" localSheetId="1">#REF!</definedName>
     <definedName name="k_1" localSheetId="0">Slab_Properties!$B$118</definedName>
-    <definedName name="k_1" localSheetId="5">SSM_Example!$B$118</definedName>
+    <definedName name="k_1" localSheetId="6">SSM_Example!$B$118</definedName>
     <definedName name="k_1">#REF!</definedName>
-    <definedName name="k_2" localSheetId="1">Drop_Slab_Properties!$B$127</definedName>
+    <definedName name="k_2" localSheetId="2">Drop_Slab_Properties!$B$127</definedName>
+    <definedName name="k_2" localSheetId="1">#REF!</definedName>
     <definedName name="k_2" localSheetId="0">Slab_Properties!$B$121</definedName>
-    <definedName name="k_2" localSheetId="5">SSM_Example!$B$121</definedName>
+    <definedName name="k_2" localSheetId="6">SSM_Example!$B$121</definedName>
     <definedName name="k_2">#REF!</definedName>
-    <definedName name="l_1" localSheetId="1">Drop_Slab_Properties!$B$3</definedName>
+    <definedName name="l_1" localSheetId="2">Drop_Slab_Properties!$B$3</definedName>
+    <definedName name="l_1" localSheetId="1">#REF!</definedName>
     <definedName name="l_1" localSheetId="0">Slab_Properties!$B$3</definedName>
-    <definedName name="l_1" localSheetId="5">SSM_Example!$B$3</definedName>
+    <definedName name="l_1" localSheetId="6">SSM_Example!$B$3</definedName>
     <definedName name="l_1">#REF!</definedName>
-    <definedName name="l_1c" localSheetId="1">Drop_Slab_Properties!$B$24</definedName>
+    <definedName name="l_1c" localSheetId="2">Drop_Slab_Properties!$B$24</definedName>
+    <definedName name="l_1c" localSheetId="1">#REF!</definedName>
     <definedName name="l_1c" localSheetId="0">Slab_Properties!$B$22</definedName>
-    <definedName name="l_1c" localSheetId="5">SSM_Example!$B$22</definedName>
+    <definedName name="l_1c" localSheetId="6">SSM_Example!$B$22</definedName>
     <definedName name="l_1c">#REF!</definedName>
-    <definedName name="l_1m" localSheetId="1">Drop_Slab_Properties!$C$24</definedName>
+    <definedName name="l_1m" localSheetId="2">Drop_Slab_Properties!$C$24</definedName>
+    <definedName name="l_1m" localSheetId="1">#REF!</definedName>
     <definedName name="l_1m" localSheetId="0">Slab_Properties!$C$22</definedName>
-    <definedName name="l_1m" localSheetId="5">SSM_Example!$C$22</definedName>
+    <definedName name="l_1m" localSheetId="6">SSM_Example!$C$22</definedName>
     <definedName name="l_1m">#REF!</definedName>
-    <definedName name="l_2" localSheetId="1">Drop_Slab_Properties!$B$4</definedName>
+    <definedName name="l_2" localSheetId="2">Drop_Slab_Properties!$B$4</definedName>
+    <definedName name="l_2" localSheetId="1">#REF!</definedName>
     <definedName name="l_2" localSheetId="0">Slab_Properties!$B$4</definedName>
-    <definedName name="l_2" localSheetId="5">SSM_Example!$B$4</definedName>
+    <definedName name="l_2" localSheetId="6">SSM_Example!$B$4</definedName>
     <definedName name="l_2">#REF!</definedName>
-    <definedName name="l_2c" localSheetId="1">Drop_Slab_Properties!$B$25</definedName>
+    <definedName name="l_2c" localSheetId="2">Drop_Slab_Properties!$B$25</definedName>
+    <definedName name="l_2c" localSheetId="1">#REF!</definedName>
     <definedName name="l_2c" localSheetId="0">Slab_Properties!$B$23</definedName>
-    <definedName name="l_2c" localSheetId="5">SSM_Example!$B$23</definedName>
+    <definedName name="l_2c" localSheetId="6">SSM_Example!$B$23</definedName>
     <definedName name="l_2c">#REF!</definedName>
-    <definedName name="l_2m" localSheetId="1">Drop_Slab_Properties!$C$25</definedName>
+    <definedName name="l_2m" localSheetId="2">Drop_Slab_Properties!$C$25</definedName>
+    <definedName name="l_2m" localSheetId="1">#REF!</definedName>
     <definedName name="l_2m" localSheetId="0">Slab_Properties!$C$23</definedName>
-    <definedName name="l_2m" localSheetId="5">SSM_Example!$C$23</definedName>
+    <definedName name="l_2m" localSheetId="6">SSM_Example!$C$23</definedName>
     <definedName name="l_2m">#REF!</definedName>
-    <definedName name="lambda_cw" localSheetId="1">Drop_Slab_Properties!$B$19</definedName>
+    <definedName name="lambda_cw" localSheetId="2">Drop_Slab_Properties!$B$19</definedName>
+    <definedName name="lambda_cw" localSheetId="1">#REF!</definedName>
     <definedName name="lambda_cw" localSheetId="0">Slab_Properties!$B$17</definedName>
-    <definedName name="lambda_cw" localSheetId="5">SSM_Example!$B$17</definedName>
+    <definedName name="lambda_cw" localSheetId="6">SSM_Example!$B$17</definedName>
     <definedName name="lambda_cw">#REF!</definedName>
-    <definedName name="lambda_i_sq" localSheetId="1">Drop_Slab_Properties!$B$128</definedName>
+    <definedName name="lambda_i_sq" localSheetId="2">Drop_Slab_Properties!$B$128</definedName>
+    <definedName name="lambda_i_sq" localSheetId="1">#REF!</definedName>
     <definedName name="lambda_i_sq" localSheetId="0">Slab_Properties!$B$122</definedName>
-    <definedName name="lambda_i_sq" localSheetId="5">SSM_Example!$B$122</definedName>
+    <definedName name="lambda_i_sq" localSheetId="6">SSM_Example!$B$122</definedName>
     <definedName name="lambda_i_sq">#REF!</definedName>
-    <definedName name="lambda_w" localSheetId="1">Drop_Slab_Properties!$B$19</definedName>
+    <definedName name="lambda_w" localSheetId="2">Drop_Slab_Properties!$B$19</definedName>
+    <definedName name="lambda_w" localSheetId="1">#REF!</definedName>
     <definedName name="lambda_w" localSheetId="0">Slab_Properties!$B$17</definedName>
-    <definedName name="lambda_w" localSheetId="5">SSM_Example!$B$17</definedName>
+    <definedName name="lambda_w" localSheetId="6">SSM_Example!$B$17</definedName>
     <definedName name="lambda_w">#REF!</definedName>
-    <definedName name="LL" localSheetId="1">Drop_Slab_Properties!$B$29</definedName>
+    <definedName name="LL" localSheetId="2">Drop_Slab_Properties!$B$29</definedName>
+    <definedName name="LL" localSheetId="1">#REF!</definedName>
     <definedName name="LL" localSheetId="0">Slab_Properties!$B$27</definedName>
-    <definedName name="LL" localSheetId="5">SSM_Example!$B$27</definedName>
+    <definedName name="LL" localSheetId="6">SSM_Example!$B$27</definedName>
     <definedName name="LL">#REF!</definedName>
-    <definedName name="LLvib" localSheetId="1">Drop_Slab_Properties!$B$30</definedName>
+    <definedName name="LLvib" localSheetId="2">Drop_Slab_Properties!$B$30</definedName>
+    <definedName name="LLvib" localSheetId="1">#REF!</definedName>
     <definedName name="LLvib" localSheetId="0">Slab_Properties!$B$28</definedName>
-    <definedName name="LLvib" localSheetId="5">SSM_Example!$B$28</definedName>
+    <definedName name="LLvib" localSheetId="6">SSM_Example!$B$28</definedName>
     <definedName name="LLvib">#REF!</definedName>
-    <definedName name="mass" localSheetId="1">Drop_Slab_Properties!$B$32</definedName>
+    <definedName name="mass" localSheetId="2">Drop_Slab_Properties!$B$32</definedName>
+    <definedName name="mass" localSheetId="1">#REF!</definedName>
     <definedName name="mass" localSheetId="0">Slab_Properties!$B$30</definedName>
-    <definedName name="mass" localSheetId="5">SSM_Example!$B$30</definedName>
+    <definedName name="mass" localSheetId="6">SSM_Example!$B$30</definedName>
     <definedName name="mass">#REF!</definedName>
-    <definedName name="n" localSheetId="1">Drop_Slab_Properties!$B$18</definedName>
+    <definedName name="n" localSheetId="2">Drop_Slab_Properties!$B$18</definedName>
+    <definedName name="n" localSheetId="1">#REF!</definedName>
     <definedName name="n" localSheetId="0">Slab_Properties!$B$16</definedName>
-    <definedName name="n" localSheetId="5">SSM_Example!$B$16</definedName>
+    <definedName name="n" localSheetId="6">SSM_Example!$B$16</definedName>
     <definedName name="n">#REF!</definedName>
-    <definedName name="nu" localSheetId="1">Drop_Slab_Properties!$B$8</definedName>
+    <definedName name="nu" localSheetId="2">Drop_Slab_Properties!$B$8</definedName>
+    <definedName name="nu" localSheetId="1">#REF!</definedName>
     <definedName name="nu" localSheetId="0">Slab_Properties!$B$8</definedName>
-    <definedName name="nu" localSheetId="5">SSM_Example!$B$8</definedName>
+    <definedName name="nu" localSheetId="6">SSM_Example!$B$8</definedName>
     <definedName name="nu">#REF!</definedName>
-    <definedName name="q_u" localSheetId="1">Drop_Slab_Properties!$B$38</definedName>
-    <definedName name="q_u" localSheetId="5">SSM_Example!$B$36</definedName>
+    <definedName name="q_u" localSheetId="2">Drop_Slab_Properties!$B$38</definedName>
+    <definedName name="q_u" localSheetId="6">SSM_Example!$B$36</definedName>
     <definedName name="q_u">Slab_Properties!$B$36</definedName>
-    <definedName name="qu" localSheetId="1">Drop_Slab_Properties!$B$38</definedName>
-    <definedName name="qu" localSheetId="5">SSM_Example!$B$36</definedName>
+    <definedName name="qu" localSheetId="2">Drop_Slab_Properties!$B$38</definedName>
+    <definedName name="qu" localSheetId="6">SSM_Example!$B$36</definedName>
     <definedName name="qu">Slab_Properties!$B$36</definedName>
-    <definedName name="SDL" localSheetId="1">Drop_Slab_Properties!$B$28</definedName>
+    <definedName name="SDL" localSheetId="2">Drop_Slab_Properties!$B$28</definedName>
+    <definedName name="SDL" localSheetId="1">#REF!</definedName>
     <definedName name="SDL" localSheetId="0">Slab_Properties!$B$26</definedName>
-    <definedName name="SDL" localSheetId="5">SSM_Example!$B$26</definedName>
+    <definedName name="SDL" localSheetId="6">SSM_Example!$B$26</definedName>
     <definedName name="SDL">#REF!</definedName>
-    <definedName name="SW" localSheetId="1">Drop_Slab_Properties!$B$31</definedName>
+    <definedName name="SW" localSheetId="2">Drop_Slab_Properties!$B$31</definedName>
+    <definedName name="SW" localSheetId="1">#REF!</definedName>
     <definedName name="SW" localSheetId="0">Slab_Properties!$B$29</definedName>
-    <definedName name="SW" localSheetId="5">SSM_Example!$B$29</definedName>
+    <definedName name="SW" localSheetId="6">SSM_Example!$B$29</definedName>
     <definedName name="SW">#REF!</definedName>
-    <definedName name="v" localSheetId="1">Drop_Slab_Properties!$B$8</definedName>
+    <definedName name="v" localSheetId="2">Drop_Slab_Properties!$B$8</definedName>
+    <definedName name="v" localSheetId="1">#REF!</definedName>
     <definedName name="v" localSheetId="0">Slab_Properties!$B$8</definedName>
-    <definedName name="v" localSheetId="5">SSM_Example!$B$8</definedName>
+    <definedName name="v" localSheetId="6">SSM_Example!$B$8</definedName>
     <definedName name="v">#REF!</definedName>
-    <definedName name="w_c" localSheetId="1">Drop_Slab_Properties!$B$15</definedName>
+    <definedName name="w_c" localSheetId="2">Drop_Slab_Properties!$B$15</definedName>
+    <definedName name="w_c" localSheetId="1">#REF!</definedName>
     <definedName name="w_c" localSheetId="0">Slab_Properties!$B$14</definedName>
-    <definedName name="w_c" localSheetId="5">SSM_Example!$B$14</definedName>
+    <definedName name="w_c" localSheetId="6">SSM_Example!$B$14</definedName>
     <definedName name="w_c">#REF!</definedName>
-    <definedName name="y_t" localSheetId="1">Drop_Slab_Properties!$B$16</definedName>
+    <definedName name="y_t" localSheetId="2">Drop_Slab_Properties!$B$16</definedName>
+    <definedName name="y_t" localSheetId="1">#REF!</definedName>
     <definedName name="y_t" localSheetId="0">Slab_Properties!$B$15</definedName>
-    <definedName name="y_t" localSheetId="5">SSM_Example!$B$15</definedName>
+    <definedName name="y_t" localSheetId="6">SSM_Example!$B$15</definedName>
     <definedName name="y_t">#REF!</definedName>
     <definedName name="y_tdrop">Drop_Slab_Properties!$B$17</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -166,7 +198,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1265" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1316" uniqueCount="225">
   <si>
     <t>Slab properties:</t>
   </si>
@@ -1884,12 +1916,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2706,29 +2738,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S128"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="B124" sqref="B124"/>
+    <sheetView topLeftCell="A118" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="B128" activeCellId="2" sqref="B124 B127 B128"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" style="8" customWidth="1"/>
     <col min="4" max="5" width="12" style="8" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="8" customWidth="1"/>
-    <col min="8" max="9" width="11.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="11.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="8" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="8" customWidth="1"/>
+    <col min="8" max="9" width="11.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="11.42578125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19">
       <c r="I1" s="8" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19">
       <c r="A2" s="52" t="s">
         <v>0</v>
       </c>
@@ -2736,7 +2768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="18" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>176</v>
       </c>
@@ -2756,7 +2788,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="18" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>177</v>
       </c>
@@ -2773,7 +2805,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="18" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>178</v>
       </c>
@@ -2788,7 +2820,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="18" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>179</v>
       </c>
@@ -2799,7 +2831,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="18" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>180</v>
       </c>
@@ -2810,7 +2842,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -2818,7 +2850,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="18" customHeight="1">
       <c r="A9" s="3" t="s">
         <v>181</v>
       </c>
@@ -2829,7 +2861,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="18" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>182</v>
       </c>
@@ -2840,7 +2872,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="18" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>183</v>
       </c>
@@ -2855,7 +2887,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="18">
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
@@ -2911,7 +2943,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19">
       <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
@@ -2926,7 +2958,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="18" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>184</v>
       </c>
@@ -2937,7 +2969,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="18" customHeight="1">
       <c r="A15" s="3" t="s">
         <v>185</v>
       </c>
@@ -2949,7 +2981,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19">
       <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
@@ -2958,7 +2990,7 @@
         <v>5.6374268708751352</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="18" customHeight="1">
       <c r="A17" s="11" t="s">
         <v>186</v>
       </c>
@@ -2970,7 +3002,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="18" customHeight="1">
       <c r="A18" s="3" t="s">
         <v>187</v>
       </c>
@@ -2985,15 +3017,15 @@
         <v>166</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" s="3"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" s="21" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" s="3" t="s">
         <v>27</v>
       </c>
@@ -3004,7 +3036,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="18" customHeight="1">
       <c r="A22" s="3" t="s">
         <v>188</v>
       </c>
@@ -3023,7 +3055,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="18" customHeight="1">
       <c r="A23" s="3" t="s">
         <v>189</v>
       </c>
@@ -3039,12 +3071,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26" s="3" t="s">
         <v>34</v>
       </c>
@@ -3055,7 +3087,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27" s="3" t="s">
         <v>36</v>
       </c>
@@ -3066,7 +3098,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="18" customHeight="1">
       <c r="A28" s="3" t="s">
         <v>37</v>
       </c>
@@ -3077,7 +3109,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29" s="3" t="s">
         <v>38</v>
       </c>
@@ -3089,7 +3121,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="17.25" customHeight="1">
       <c r="A30" s="3" t="s">
         <v>39</v>
       </c>
@@ -3101,7 +3133,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31" s="3" t="s">
         <v>41</v>
       </c>
@@ -3113,11 +3145,11 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
       <c r="A32" s="3"/>
       <c r="B32" s="6"/>
     </row>
-    <row r="33" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
       <c r="A33" s="21" t="s">
         <v>43</v>
       </c>
@@ -3128,7 +3160,7 @@
       <c r="G33" s="54"/>
       <c r="H33" s="55"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14">
       <c r="A34" s="3"/>
       <c r="F34" s="45" t="s">
         <v>45</v>
@@ -3155,7 +3187,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" ht="18" customHeight="1">
       <c r="A35" s="21" t="s">
         <v>47</v>
       </c>
@@ -3184,7 +3216,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" ht="18.75" customHeight="1" thickBot="1">
       <c r="A36" s="3" t="s">
         <v>191</v>
       </c>
@@ -3220,7 +3252,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="18" customHeight="1">
       <c r="A37" s="3" t="s">
         <v>192</v>
       </c>
@@ -3259,7 +3291,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" ht="18" customHeight="1">
       <c r="A38" s="3" t="s">
         <v>193</v>
       </c>
@@ -3301,7 +3333,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" ht="18.75" customHeight="1" thickBot="1">
       <c r="E39" s="3" t="s">
         <v>58</v>
       </c>
@@ -3330,7 +3362,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" ht="18">
       <c r="A40" s="3" t="s">
         <v>194</v>
       </c>
@@ -3351,7 +3383,7 @@
       <c r="L40" s="56"/>
       <c r="M40" s="56"/>
     </row>
-    <row r="41" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" ht="18">
       <c r="A41" s="3" t="s">
         <v>195</v>
       </c>
@@ -3372,7 +3404,7 @@
       <c r="L41" s="56"/>
       <c r="M41" s="56"/>
     </row>
-    <row r="42" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" ht="18">
       <c r="A42" s="3" t="s">
         <v>196</v>
       </c>
@@ -3393,7 +3425,7 @@
       <c r="L42" s="56"/>
       <c r="M42" s="56"/>
     </row>
-    <row r="43" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="18">
       <c r="A43" s="3" t="s">
         <v>197</v>
       </c>
@@ -3414,7 +3446,7 @@
       <c r="L43" s="56"/>
       <c r="M43" s="56"/>
     </row>
-    <row r="44" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" ht="18">
       <c r="A44" s="3" t="s">
         <v>198</v>
       </c>
@@ -3435,7 +3467,7 @@
       <c r="L44" s="56"/>
       <c r="M44" s="56"/>
     </row>
-    <row r="45" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" ht="18">
       <c r="A45" s="3" t="s">
         <v>199</v>
       </c>
@@ -3456,7 +3488,7 @@
       <c r="L45" s="56"/>
       <c r="M45" s="56"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14">
       <c r="E46" s="3"/>
       <c r="F46" s="56"/>
       <c r="G46" s="56"/>
@@ -3467,7 +3499,7 @@
       <c r="L46" s="56"/>
       <c r="M46" s="56"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14">
       <c r="A47" s="21" t="s">
         <v>65</v>
       </c>
@@ -3481,7 +3513,7 @@
       <c r="L47" s="56"/>
       <c r="M47" s="56"/>
     </row>
-    <row r="48" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" ht="18" customHeight="1">
       <c r="A48" s="3" t="s">
         <v>200</v>
       </c>
@@ -3505,7 +3537,7 @@
       <c r="L48" s="56"/>
       <c r="M48" s="56"/>
     </row>
-    <row r="49" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" ht="18" customHeight="1">
       <c r="A49" s="3" t="s">
         <v>201</v>
       </c>
@@ -3526,7 +3558,7 @@
       <c r="L49" s="56"/>
       <c r="M49" s="56"/>
     </row>
-    <row r="50" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" ht="18" customHeight="1">
       <c r="A50" s="3" t="s">
         <v>202</v>
       </c>
@@ -3547,7 +3579,7 @@
       <c r="L50" s="56"/>
       <c r="M50" s="56"/>
     </row>
-    <row r="51" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" ht="18" customHeight="1">
       <c r="A51" s="3" t="s">
         <v>203</v>
       </c>
@@ -3568,7 +3600,7 @@
       <c r="L51" s="56"/>
       <c r="M51" s="56"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13">
       <c r="A52" s="3"/>
       <c r="B52" s="7"/>
       <c r="E52" s="3"/>
@@ -3581,12 +3613,12 @@
       <c r="L52" s="56"/>
       <c r="M52" s="56"/>
     </row>
-    <row r="53" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" ht="18" customHeight="1">
       <c r="A53" s="21" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13">
       <c r="A54" s="56" t="s">
         <v>27</v>
       </c>
@@ -3603,7 +3635,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" ht="18" customHeight="1">
       <c r="A55" s="56" t="s">
         <v>188</v>
       </c>
@@ -3625,7 +3657,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" ht="18" customHeight="1">
       <c r="A56" s="56" t="s">
         <v>188</v>
       </c>
@@ -3647,7 +3679,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" ht="18" customHeight="1">
       <c r="A57" s="56" t="s">
         <v>188</v>
       </c>
@@ -3669,7 +3701,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" ht="18" customHeight="1">
       <c r="A58" s="56" t="s">
         <v>188</v>
       </c>
@@ -3691,7 +3723,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" ht="18" customHeight="1">
       <c r="A59" s="56" t="s">
         <v>188</v>
       </c>
@@ -3713,7 +3745,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" ht="18" customHeight="1">
       <c r="A60" s="56" t="s">
         <v>188</v>
       </c>
@@ -3735,7 +3767,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" ht="18" customHeight="1">
       <c r="A61" s="56" t="s">
         <v>189</v>
       </c>
@@ -3757,7 +3789,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" ht="18" customHeight="1">
       <c r="A62" s="56" t="s">
         <v>189</v>
       </c>
@@ -3779,7 +3811,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" ht="18" customHeight="1">
       <c r="A63" s="56" t="s">
         <v>189</v>
       </c>
@@ -3801,7 +3833,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" ht="18" customHeight="1">
       <c r="A64" s="56" t="s">
         <v>189</v>
       </c>
@@ -3823,7 +3855,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" ht="18" customHeight="1">
       <c r="A65" s="56" t="s">
         <v>189</v>
       </c>
@@ -3845,7 +3877,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="66" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" ht="18" customHeight="1">
       <c r="A66" s="56" t="s">
         <v>189</v>
       </c>
@@ -3867,12 +3899,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="69" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:19" ht="18" customHeight="1">
       <c r="A69" s="52" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:19">
       <c r="A70" s="56" t="s">
         <v>27</v>
       </c>
@@ -3886,7 +3918,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="71" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" ht="18" customHeight="1">
       <c r="A71" s="56" t="s">
         <v>188</v>
       </c>
@@ -3905,7 +3937,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="72" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" ht="18" customHeight="1">
       <c r="A72" s="56" t="s">
         <v>188</v>
       </c>
@@ -3924,7 +3956,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="73" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" ht="18" customHeight="1">
       <c r="A73" s="56" t="s">
         <v>188</v>
       </c>
@@ -3943,7 +3975,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="74" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" ht="18" customHeight="1">
       <c r="A74" s="56" t="s">
         <v>189</v>
       </c>
@@ -3962,7 +3994,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="75" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" ht="18" customHeight="1">
       <c r="A75" s="56" t="s">
         <v>189</v>
       </c>
@@ -3981,7 +4013,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="76" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" ht="18" customHeight="1">
       <c r="A76" s="56" t="s">
         <v>189</v>
       </c>
@@ -4000,7 +4032,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="78" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:19" ht="18" customHeight="1">
       <c r="A78" s="21" t="s">
         <v>80</v>
       </c>
@@ -4016,7 +4048,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:19">
       <c r="A79" s="56" t="s">
         <v>27</v>
       </c>
@@ -4067,7 +4099,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="80" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" ht="18.75" customHeight="1">
       <c r="A80" s="56" t="s">
         <v>188</v>
       </c>
@@ -4130,7 +4162,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" ht="18.75" customHeight="1">
       <c r="A81" s="56" t="s">
         <v>188</v>
       </c>
@@ -4193,7 +4225,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" ht="18.75" customHeight="1">
       <c r="A82" s="56" t="s">
         <v>188</v>
       </c>
@@ -4256,7 +4288,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" ht="18.75" customHeight="1">
       <c r="A83" s="56" t="s">
         <v>189</v>
       </c>
@@ -4319,7 +4351,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" ht="18.75" customHeight="1">
       <c r="A84" s="56" t="s">
         <v>189</v>
       </c>
@@ -4382,7 +4414,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="85" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" ht="18.75" customHeight="1">
       <c r="A85" s="56" t="s">
         <v>189</v>
       </c>
@@ -4445,12 +4477,12 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="87" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:19" ht="18" customHeight="1">
       <c r="A87" s="21" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:19">
       <c r="A88" s="56" t="s">
         <v>27</v>
       </c>
@@ -4464,7 +4496,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="89" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19" ht="18.75" customHeight="1">
       <c r="A89" s="56" t="s">
         <v>188</v>
       </c>
@@ -4483,7 +4515,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="90" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" ht="18.75" customHeight="1">
       <c r="A90" s="56" t="s">
         <v>188</v>
       </c>
@@ -4502,7 +4534,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="91" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" ht="18.75" customHeight="1">
       <c r="A91" s="56" t="s">
         <v>188</v>
       </c>
@@ -4521,7 +4553,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="92" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" ht="18.75" customHeight="1">
       <c r="A92" s="56" t="s">
         <v>189</v>
       </c>
@@ -4540,7 +4572,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="93" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:19" ht="18.75" customHeight="1">
       <c r="A93" s="56" t="s">
         <v>189</v>
       </c>
@@ -4559,7 +4591,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="94" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" ht="18.75" customHeight="1">
       <c r="A94" s="56" t="s">
         <v>189</v>
       </c>
@@ -4578,8 +4610,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="95" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:19" ht="15.75" customHeight="1" thickBot="1"/>
+    <row r="96" spans="1:19">
       <c r="F96" s="38" t="s">
         <v>28</v>
       </c>
@@ -4617,7 +4649,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="97" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:17" ht="18" customHeight="1">
       <c r="A97" s="21" t="s">
         <v>86</v>
       </c>
@@ -4658,7 +4690,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="98" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" ht="18" customHeight="1" thickBot="1">
       <c r="A98" s="56" t="s">
         <v>27</v>
       </c>
@@ -4700,7 +4732,7 @@
       <c r="P98" s="26"/>
       <c r="Q98" s="29"/>
     </row>
-    <row r="99" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" ht="18.75" customHeight="1">
       <c r="A99" s="56" t="s">
         <v>188</v>
       </c>
@@ -4767,7 +4799,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17" ht="18.75" customHeight="1">
       <c r="A100" s="56" t="s">
         <v>188</v>
       </c>
@@ -4834,7 +4866,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17" ht="18.75" customHeight="1">
       <c r="A101" s="56" t="s">
         <v>188</v>
       </c>
@@ -4901,7 +4933,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" ht="18.75" customHeight="1">
       <c r="A102" s="56" t="s">
         <v>189</v>
       </c>
@@ -4968,7 +5000,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:17" ht="18.75" customHeight="1">
       <c r="A103" s="56" t="s">
         <v>189</v>
       </c>
@@ -5035,7 +5067,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:17" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:17" ht="19.5" customHeight="1" thickBot="1">
       <c r="A104" s="56" t="s">
         <v>189</v>
       </c>
@@ -5102,12 +5134,12 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:17" ht="18" customHeight="1">
       <c r="A106" s="21" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:17">
       <c r="A107" s="56" t="s">
         <v>27</v>
       </c>
@@ -5118,7 +5150,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="108" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:17" ht="18.75" customHeight="1">
       <c r="A108" s="56" t="s">
         <v>188</v>
       </c>
@@ -5134,7 +5166,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="109" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:17" ht="18.75" customHeight="1">
       <c r="A109" s="56" t="s">
         <v>189</v>
       </c>
@@ -5150,17 +5182,17 @@
         <v>205</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:17">
       <c r="A110" s="56"/>
       <c r="B110" s="56"/>
     </row>
-    <row r="111" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:17" ht="18" customHeight="1">
       <c r="A111" s="21" t="s">
         <v>207</v>
       </c>
       <c r="B111" s="56"/>
     </row>
-    <row r="112" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:17" ht="18.75" customHeight="1">
       <c r="A112" s="3" t="s">
         <v>209</v>
       </c>
@@ -5172,16 +5204,16 @@
         <v>205</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:5">
       <c r="A113" s="56"/>
       <c r="B113" s="56"/>
     </row>
-    <row r="114" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" ht="18" customHeight="1">
       <c r="A114" s="21" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" ht="18.75" customHeight="1">
       <c r="A115" s="3" t="s">
         <v>210</v>
       </c>
@@ -5193,12 +5225,12 @@
         <v>205</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" ht="18" customHeight="1">
       <c r="A117" s="52" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" ht="18" customHeight="1">
       <c r="A118" s="3" t="s">
         <v>212</v>
       </c>
@@ -5207,7 +5239,7 @@
         <v>0.42122127857031932</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" ht="19.5" customHeight="1" thickBot="1">
       <c r="A120" s="52" t="s">
         <v>100</v>
       </c>
@@ -5215,7 +5247,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" ht="18" customHeight="1">
       <c r="A121" s="3" t="s">
         <v>213</v>
       </c>
@@ -5230,7 +5262,7 @@
         <v>7.12</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" ht="18.75" customHeight="1">
       <c r="A122" s="11" t="s">
         <v>214</v>
       </c>
@@ -5249,7 +5281,7 @@
         <v>8.92</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A123" s="11" t="s">
         <v>104</v>
       </c>
@@ -5267,7 +5299,7 @@
         <v>9.2899999999999991</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:5" ht="18" customHeight="1">
       <c r="A124" s="3" t="s">
         <v>106</v>
       </c>
@@ -5279,12 +5311,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:5">
       <c r="A126" s="21" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:5">
       <c r="A127" s="3" t="s">
         <v>109</v>
       </c>
@@ -5296,7 +5328,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:5">
       <c r="A128" s="11" t="s">
         <v>216</v>
       </c>
@@ -5311,31 +5343,395 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABE439E0-7694-4CCC-8DF2-04F46C119F4A}">
+  <dimension ref="A1:O14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" style="8" customWidth="1"/>
+    <col min="2" max="9" width="8.85546875" style="8"/>
+    <col min="10" max="10" width="12.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.85546875" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" s="52" t="s">
+        <v>145</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="18" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" s="62">
+        <v>5.6172264218657322</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="6">
+        <v>215016</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="B5" s="61">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="11"/>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="52" t="s">
+        <v>147</v>
+      </c>
+      <c r="H7" s="56" t="s">
+        <v>148</v>
+      </c>
+      <c r="I7" s="56" t="s">
+        <v>149</v>
+      </c>
+      <c r="L7" s="56" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="18" customHeight="1">
+      <c r="A8" s="56" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8" s="56" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" s="56" t="s">
+        <v>152</v>
+      </c>
+      <c r="D8" s="56" t="s">
+        <v>153</v>
+      </c>
+      <c r="E8" s="56" t="s">
+        <v>154</v>
+      </c>
+      <c r="F8" s="56" t="s">
+        <v>155</v>
+      </c>
+      <c r="G8" s="57" t="s">
+        <v>156</v>
+      </c>
+      <c r="H8" s="56" t="s">
+        <v>157</v>
+      </c>
+      <c r="I8" s="56" t="s">
+        <v>158</v>
+      </c>
+      <c r="J8" s="56" t="s">
+        <v>161</v>
+      </c>
+      <c r="K8" s="56" t="s">
+        <v>160</v>
+      </c>
+      <c r="L8" s="56" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="56"/>
+      <c r="B9" s="56" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="56" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" s="56" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="56" t="s">
+        <v>107</v>
+      </c>
+      <c r="F9" s="56" t="s">
+        <v>107</v>
+      </c>
+      <c r="G9" s="57"/>
+      <c r="H9" s="56" t="s">
+        <v>143</v>
+      </c>
+      <c r="I9" s="56" t="s">
+        <v>143</v>
+      </c>
+      <c r="J9" s="56" t="s">
+        <v>143</v>
+      </c>
+      <c r="K9" s="56" t="s">
+        <v>143</v>
+      </c>
+      <c r="L9" s="56" t="s">
+        <v>143</v>
+      </c>
+      <c r="M9" s="56" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10" s="10">
+        <f>$B$3</f>
+        <v>5.6172264218657322</v>
+      </c>
+      <c r="C10" s="56">
+        <v>1.25</v>
+      </c>
+      <c r="D10" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="E10" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="F10" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="G10" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="I10" s="7">
+        <f>250000000/($B$4*$B$5)*($C10^2.43/$B10^1.8)*(1-EXP(-2*PI()*$B$5*$B10/$C10))</f>
+        <v>1514.2800070686451</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="K10" s="7">
+        <f>250000000/($B$4*$B$5)*($C10^2.43/$B10^1.8)*(1-EXP(-2*PI()*$B$5*$B10/$C10))</f>
+        <v>1514.2800070686451</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="M10" s="60">
+        <f>I10</f>
+        <v>1514.2800070686451</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="56" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" s="10">
+        <f>$B$3</f>
+        <v>5.6172264218657322</v>
+      </c>
+      <c r="C11" s="56">
+        <v>1.6</v>
+      </c>
+      <c r="D11" s="56">
+        <v>6.8</v>
+      </c>
+      <c r="E11" s="56">
+        <v>6</v>
+      </c>
+      <c r="F11" s="56">
+        <v>8</v>
+      </c>
+      <c r="G11" s="56">
+        <v>0.1</v>
+      </c>
+      <c r="H11" s="7">
+        <f>175000000/($B$4*$B$5*SQRT($B11))*(EXP(-$G11*$B11))</f>
+        <v>4895.4573378997957</v>
+      </c>
+      <c r="I11" s="7">
+        <f t="shared" ref="I11:I13" si="0">250000000/($B$4*$B$5)*($C11^2.43/$B11^1.8)*(1-EXP(-2*PI()*$B$5*$B11/$C11))</f>
+        <v>2389.5757707542061</v>
+      </c>
+      <c r="J11" s="7">
+        <f>175000000/($B$4*$B$5*SQRT($E11))*(EXP(-$G11*$E11))</f>
+        <v>4558.8464508293391</v>
+      </c>
+      <c r="K11" s="7">
+        <f>250000000/($B$4*$B$5)*($C11^2.43/$F11^1.8)*(1-EXP(-2*PI()*$B$5*$F11/$C11))</f>
+        <v>1543.1280393215177</v>
+      </c>
+      <c r="L11" s="7" t="str">
+        <f>IF(AND($B11&gt;$E11,$B11&lt;$F11),$J11 + ($B11-$E11) * ($K11-$J11)/($F11-$E11), "N/A")</f>
+        <v>N/A</v>
+      </c>
+      <c r="M11" s="60">
+        <f>IF($B11&gt;=F11,I11, IF($B11&lt;=E11,H11,L11))</f>
+        <v>4895.4573378997957</v>
+      </c>
+      <c r="N11" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="O11" s="8" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="56" t="s">
+        <v>131</v>
+      </c>
+      <c r="B12" s="10">
+        <f>$B$3</f>
+        <v>5.6172264218657322</v>
+      </c>
+      <c r="C12" s="56">
+        <v>1.85</v>
+      </c>
+      <c r="D12" s="56">
+        <v>8</v>
+      </c>
+      <c r="E12" s="56">
+        <v>7</v>
+      </c>
+      <c r="F12" s="56">
+        <v>9</v>
+      </c>
+      <c r="G12" s="56">
+        <v>0.09</v>
+      </c>
+      <c r="H12" s="7">
+        <f>175000000/($B$4*$B$5*SQRT($B12))*(EXP(-$G12*$B12))</f>
+        <v>5178.316303177392</v>
+      </c>
+      <c r="I12" s="7">
+        <f t="shared" si="0"/>
+        <v>3096.4636758802635</v>
+      </c>
+      <c r="J12" s="7">
+        <f>175000000/($B$4*$B$5*SQRT($E12))*(EXP(-$G12*$E12))</f>
+        <v>4095.9319765048003</v>
+      </c>
+      <c r="K12" s="7">
+        <f>250000000/($B$4*$B$5)*($C12^2.43/$F12^1.8)*(1-EXP(-2*PI()*$B$5*$F12/$C12))</f>
+        <v>1751.9949978877621</v>
+      </c>
+      <c r="L12" s="7" t="str">
+        <f t="shared" ref="L12:L13" si="1">IF(AND($B12&gt;$E12,$B12&lt;$F12),$J12 + ($B12-$E12) * ($K12-$J12)/($F12-$E12), "N/A")</f>
+        <v>N/A</v>
+      </c>
+      <c r="M12" s="60">
+        <f>IF($B12&gt;=F12,I12, IF($B12&lt;=E12,H12,L12))</f>
+        <v>5178.316303177392</v>
+      </c>
+      <c r="N12" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="56" t="s">
+        <v>132</v>
+      </c>
+      <c r="B13" s="10">
+        <f>$B$3</f>
+        <v>5.6172264218657322</v>
+      </c>
+      <c r="C13" s="56">
+        <v>2.1</v>
+      </c>
+      <c r="D13" s="56">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="E13" s="56">
+        <v>8</v>
+      </c>
+      <c r="F13" s="56">
+        <v>10</v>
+      </c>
+      <c r="G13" s="56">
+        <v>0.08</v>
+      </c>
+      <c r="H13" s="7">
+        <f>175000000/($B$4*$B$5*SQRT($B13))*(EXP(-$G13*$B13))</f>
+        <v>5477.5188271289653</v>
+      </c>
+      <c r="I13" s="7">
+        <f t="shared" si="0"/>
+        <v>3863.4172154762687</v>
+      </c>
+      <c r="J13" s="7">
+        <f>175000000/($B$4*$B$5*SQRT($E13))*(EXP(-$G13*$E13))</f>
+        <v>3793.2705312684943</v>
+      </c>
+      <c r="K13" s="7">
+        <f>250000000/($B$4*$B$5)*($C13^2.43/$F13^1.8)*(1-EXP(-2*PI()*$B$5*$F13/$C13))</f>
+        <v>1950.5528483415283</v>
+      </c>
+      <c r="L13" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>N/A</v>
+      </c>
+      <c r="M13" s="60">
+        <f>IF($B13&gt;=F13,I13, IF($B13&lt;=E13,H13,L13))</f>
+        <v>5477.5188271289653</v>
+      </c>
+      <c r="N13" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="M14" s="52"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="G129" sqref="G129:G130"/>
+    <sheetView topLeftCell="A115" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="B134" activeCellId="2" sqref="B130 B133 B134"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" style="8" customWidth="1"/>
-    <col min="2" max="3" width="8.83203125" style="8"/>
+    <col min="2" max="3" width="8.85546875" style="8"/>
     <col min="4" max="5" width="12" style="8" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="8" customWidth="1"/>
-    <col min="8" max="9" width="11.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="11.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.83203125" style="8"/>
+    <col min="6" max="6" width="11.85546875" style="8" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="8" customWidth="1"/>
+    <col min="8" max="9" width="11.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="11.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19">
       <c r="I1" s="8" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19">
       <c r="A2" s="52" t="s">
         <v>0</v>
       </c>
@@ -5343,7 +5739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="18" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>176</v>
       </c>
@@ -5363,7 +5759,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="18" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>177</v>
       </c>
@@ -5380,7 +5776,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="18" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>178</v>
       </c>
@@ -5395,7 +5791,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="18" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>179</v>
       </c>
@@ -5406,7 +5802,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="18" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>180</v>
       </c>
@@ -5417,7 +5813,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -5425,7 +5821,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="18" customHeight="1">
       <c r="A9" s="3" t="s">
         <v>181</v>
       </c>
@@ -5436,7 +5832,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="18" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>182</v>
       </c>
@@ -5447,7 +5843,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="18" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>183</v>
       </c>
@@ -5462,7 +5858,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="18">
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
@@ -5520,7 +5916,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19">
       <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
@@ -5535,7 +5931,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="18">
       <c r="A14" s="3" t="s">
         <v>222</v>
       </c>
@@ -5547,7 +5943,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="18" customHeight="1">
       <c r="A15" s="3" t="s">
         <v>184</v>
       </c>
@@ -5558,7 +5954,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="18" customHeight="1">
       <c r="A16" s="3" t="s">
         <v>185</v>
       </c>
@@ -5570,7 +5966,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="18" customHeight="1">
       <c r="A17" s="3" t="s">
         <v>223</v>
       </c>
@@ -5582,7 +5978,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" s="3" t="s">
         <v>23</v>
       </c>
@@ -5591,7 +5987,7 @@
         <v>5.6374268708751352</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="18" customHeight="1">
       <c r="A19" s="11" t="s">
         <v>186</v>
       </c>
@@ -5603,7 +5999,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="18" customHeight="1">
       <c r="A20" s="3" t="s">
         <v>187</v>
       </c>
@@ -5618,15 +6014,15 @@
         <v>166</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" s="3"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22" s="21" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23" s="3" t="s">
         <v>27</v>
       </c>
@@ -5637,7 +6033,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="18" customHeight="1">
       <c r="A24" s="3" t="s">
         <v>188</v>
       </c>
@@ -5656,7 +6052,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="18" customHeight="1">
       <c r="A25" s="3" t="s">
         <v>189</v>
       </c>
@@ -5672,12 +6068,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28" s="3" t="s">
         <v>34</v>
       </c>
@@ -5688,7 +6084,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29" s="3" t="s">
         <v>36</v>
       </c>
@@ -5699,7 +6095,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="18" customHeight="1">
       <c r="A30" s="3" t="s">
         <v>37</v>
       </c>
@@ -5710,7 +6106,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31" s="3" t="s">
         <v>38</v>
       </c>
@@ -5722,7 +6118,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="17.25" customHeight="1">
       <c r="A32" s="3" t="s">
         <v>39</v>
       </c>
@@ -5734,7 +6130,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14">
       <c r="A33" s="3" t="s">
         <v>41</v>
       </c>
@@ -5746,11 +6142,11 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
       <c r="A34" s="3"/>
       <c r="B34" s="6"/>
     </row>
-    <row r="35" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
       <c r="A35" s="21" t="s">
         <v>43</v>
       </c>
@@ -5761,7 +6157,7 @@
       <c r="G35" s="54"/>
       <c r="H35" s="55"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14">
       <c r="A36" s="3"/>
       <c r="F36" s="45" t="s">
         <v>45</v>
@@ -5788,7 +6184,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" ht="18" customHeight="1">
       <c r="A37" s="21" t="s">
         <v>47</v>
       </c>
@@ -5817,7 +6213,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" ht="18.75" customHeight="1" thickBot="1">
       <c r="A38" s="3" t="s">
         <v>191</v>
       </c>
@@ -5853,7 +6249,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" ht="18" customHeight="1">
       <c r="A39" s="3" t="s">
         <v>192</v>
       </c>
@@ -5892,7 +6288,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" ht="18" customHeight="1">
       <c r="A40" s="3" t="s">
         <v>193</v>
       </c>
@@ -5934,7 +6330,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" ht="18.75" customHeight="1" thickBot="1">
       <c r="E41" s="3" t="s">
         <v>58</v>
       </c>
@@ -5963,7 +6359,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" ht="18">
       <c r="A42" s="3" t="s">
         <v>194</v>
       </c>
@@ -5984,7 +6380,7 @@
       <c r="L42" s="56"/>
       <c r="M42" s="56"/>
     </row>
-    <row r="43" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="18">
       <c r="A43" s="3" t="s">
         <v>195</v>
       </c>
@@ -6005,7 +6401,7 @@
       <c r="L43" s="56"/>
       <c r="M43" s="56"/>
     </row>
-    <row r="44" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" ht="18">
       <c r="A44" s="3" t="s">
         <v>196</v>
       </c>
@@ -6026,7 +6422,7 @@
       <c r="L44" s="56"/>
       <c r="M44" s="56"/>
     </row>
-    <row r="45" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" ht="18">
       <c r="A45" s="3" t="s">
         <v>197</v>
       </c>
@@ -6047,7 +6443,7 @@
       <c r="L45" s="56"/>
       <c r="M45" s="56"/>
     </row>
-    <row r="46" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" ht="18">
       <c r="A46" s="3" t="s">
         <v>198</v>
       </c>
@@ -6068,7 +6464,7 @@
       <c r="L46" s="56"/>
       <c r="M46" s="56"/>
     </row>
-    <row r="47" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" ht="18">
       <c r="A47" s="3" t="s">
         <v>199</v>
       </c>
@@ -6089,7 +6485,7 @@
       <c r="L47" s="56"/>
       <c r="M47" s="56"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14">
       <c r="E48" s="3"/>
       <c r="F48" s="56"/>
       <c r="G48" s="56"/>
@@ -6100,7 +6496,7 @@
       <c r="L48" s="56"/>
       <c r="M48" s="56"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13">
       <c r="A49" s="21" t="s">
         <v>65</v>
       </c>
@@ -6114,7 +6510,7 @@
       <c r="L49" s="56"/>
       <c r="M49" s="56"/>
     </row>
-    <row r="50" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" ht="18" customHeight="1">
       <c r="A50" s="3" t="s">
         <v>200</v>
       </c>
@@ -6138,7 +6534,7 @@
       <c r="L50" s="56"/>
       <c r="M50" s="56"/>
     </row>
-    <row r="51" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" ht="18" customHeight="1">
       <c r="A51" s="3" t="s">
         <v>201</v>
       </c>
@@ -6159,7 +6555,7 @@
       <c r="L51" s="56"/>
       <c r="M51" s="56"/>
     </row>
-    <row r="52" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" ht="18" customHeight="1">
       <c r="A52" s="3" t="s">
         <v>202</v>
       </c>
@@ -6180,7 +6576,7 @@
       <c r="L52" s="56"/>
       <c r="M52" s="56"/>
     </row>
-    <row r="53" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" ht="18" customHeight="1">
       <c r="A53" s="3" t="s">
         <v>203</v>
       </c>
@@ -6201,7 +6597,7 @@
       <c r="L53" s="56"/>
       <c r="M53" s="56"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13">
       <c r="A54" s="3"/>
       <c r="B54" s="7"/>
       <c r="E54" s="3"/>
@@ -6214,12 +6610,12 @@
       <c r="L54" s="56"/>
       <c r="M54" s="56"/>
     </row>
-    <row r="55" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" ht="18" customHeight="1">
       <c r="A55" s="21" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13">
       <c r="A56" s="56" t="s">
         <v>27</v>
       </c>
@@ -6236,7 +6632,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" ht="18" customHeight="1">
       <c r="A57" s="56" t="s">
         <v>188</v>
       </c>
@@ -6258,7 +6654,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" ht="18" customHeight="1">
       <c r="A58" s="56" t="s">
         <v>188</v>
       </c>
@@ -6280,7 +6676,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" ht="18" customHeight="1">
       <c r="A59" s="56" t="s">
         <v>188</v>
       </c>
@@ -6302,7 +6698,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" ht="18" customHeight="1">
       <c r="A60" s="56" t="s">
         <v>188</v>
       </c>
@@ -6324,7 +6720,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" ht="18" customHeight="1">
       <c r="A61" s="56" t="s">
         <v>188</v>
       </c>
@@ -6346,7 +6742,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" ht="18" customHeight="1">
       <c r="A62" s="56" t="s">
         <v>188</v>
       </c>
@@ -6368,7 +6764,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" ht="18" customHeight="1">
       <c r="A63" s="56" t="s">
         <v>189</v>
       </c>
@@ -6390,7 +6786,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" ht="18" customHeight="1">
       <c r="A64" s="56" t="s">
         <v>189</v>
       </c>
@@ -6412,7 +6808,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="65" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" ht="18" customHeight="1">
       <c r="A65" s="56" t="s">
         <v>189</v>
       </c>
@@ -6434,7 +6830,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="66" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" ht="18" customHeight="1">
       <c r="A66" s="56" t="s">
         <v>189</v>
       </c>
@@ -6456,7 +6852,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="67" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" ht="18" customHeight="1">
       <c r="A67" s="56" t="s">
         <v>189</v>
       </c>
@@ -6478,7 +6874,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" ht="18" customHeight="1">
       <c r="A68" s="56" t="s">
         <v>189</v>
       </c>
@@ -6500,12 +6896,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="71" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:18" ht="18" customHeight="1">
       <c r="A71" s="52" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:18">
       <c r="A72" s="56" t="s">
         <v>27</v>
       </c>
@@ -6519,7 +6915,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="73" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" ht="18" customHeight="1">
       <c r="A73" s="56" t="s">
         <v>188</v>
       </c>
@@ -6538,7 +6934,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="74" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" ht="18" customHeight="1">
       <c r="A74" s="56" t="s">
         <v>188</v>
       </c>
@@ -6557,7 +6953,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="75" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" ht="18" customHeight="1">
       <c r="A75" s="56" t="s">
         <v>188</v>
       </c>
@@ -6576,7 +6972,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="76" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" ht="18" customHeight="1">
       <c r="A76" s="56" t="s">
         <v>189</v>
       </c>
@@ -6595,7 +6991,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="77" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" ht="18" customHeight="1">
       <c r="A77" s="56" t="s">
         <v>189</v>
       </c>
@@ -6614,7 +7010,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="78" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" ht="18" customHeight="1">
       <c r="A78" s="56" t="s">
         <v>189</v>
       </c>
@@ -6633,7 +7029,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="80" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:18" ht="18" customHeight="1">
       <c r="A80" s="21" t="s">
         <v>80</v>
       </c>
@@ -6647,7 +7043,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:19">
       <c r="A81" s="56" t="s">
         <v>27</v>
       </c>
@@ -6697,7 +7093,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="82" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" ht="18.75" customHeight="1">
       <c r="A82" s="56" t="s">
         <v>188</v>
       </c>
@@ -6759,7 +7155,7 @@
         <v>2.15E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" ht="18.75" customHeight="1">
       <c r="A83" s="56" t="s">
         <v>188</v>
       </c>
@@ -6821,7 +7217,7 @@
         <v>1.98E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" ht="18.75" customHeight="1">
       <c r="A84" s="56" t="s">
         <v>188</v>
       </c>
@@ -6883,7 +7279,7 @@
         <v>1.98E-3</v>
       </c>
     </row>
-    <row r="85" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" ht="18.75" customHeight="1">
       <c r="A85" s="56" t="s">
         <v>189</v>
       </c>
@@ -6945,7 +7341,7 @@
         <v>1.98E-3</v>
       </c>
     </row>
-    <row r="86" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" ht="18.75" customHeight="1">
       <c r="A86" s="56" t="s">
         <v>189</v>
       </c>
@@ -7007,7 +7403,7 @@
         <v>1.98E-3</v>
       </c>
     </row>
-    <row r="87" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" ht="18.75" customHeight="1">
       <c r="A87" s="56" t="s">
         <v>189</v>
       </c>
@@ -7069,12 +7465,12 @@
         <v>1.98E-3</v>
       </c>
     </row>
-    <row r="89" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:19" ht="18" customHeight="1">
       <c r="A89" s="21" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:19">
       <c r="A90" s="56" t="s">
         <v>27</v>
       </c>
@@ -7088,7 +7484,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="91" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" ht="18.75" customHeight="1">
       <c r="A91" s="56" t="s">
         <v>188</v>
       </c>
@@ -7107,7 +7503,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="92" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" ht="18.75" customHeight="1">
       <c r="A92" s="56" t="s">
         <v>188</v>
       </c>
@@ -7126,7 +7522,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="93" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:19" ht="18.75" customHeight="1">
       <c r="A93" s="56" t="s">
         <v>188</v>
       </c>
@@ -7145,7 +7541,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="94" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" ht="18.75" customHeight="1">
       <c r="A94" s="56" t="s">
         <v>189</v>
       </c>
@@ -7164,7 +7560,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="95" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:19" ht="18.75" customHeight="1">
       <c r="A95" s="56" t="s">
         <v>189</v>
       </c>
@@ -7183,7 +7579,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="96" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:19" ht="18.75" customHeight="1">
       <c r="A96" s="56" t="s">
         <v>189</v>
       </c>
@@ -7202,13 +7598,13 @@
         <v>205</v>
       </c>
     </row>
-    <row r="97" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:17" ht="18.75" customHeight="1">
       <c r="A97" s="56"/>
       <c r="B97" s="56"/>
       <c r="C97" s="7"/>
       <c r="D97" s="7"/>
     </row>
-    <row r="98" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:17" ht="18.75" customHeight="1">
       <c r="A98" s="21" t="s">
         <v>224</v>
       </c>
@@ -7216,7 +7612,7 @@
       <c r="C98" s="7"/>
       <c r="D98" s="7"/>
     </row>
-    <row r="99" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:17" ht="18.75" customHeight="1">
       <c r="A99" s="56"/>
       <c r="B99" s="56" t="s">
         <v>28</v>
@@ -7226,7 +7622,7 @@
       </c>
       <c r="D99" s="7"/>
     </row>
-    <row r="100" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:17" ht="18.75" customHeight="1">
       <c r="A100" s="56" t="s">
         <v>30</v>
       </c>
@@ -7240,7 +7636,7 @@
       </c>
       <c r="D100" s="7"/>
     </row>
-    <row r="101" spans="1:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
       <c r="A101" s="56" t="s">
         <v>32</v>
       </c>
@@ -7253,7 +7649,7 @@
         <v>46648</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:17">
       <c r="F102" s="38" t="s">
         <v>28</v>
       </c>
@@ -7291,7 +7687,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="103" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:17" ht="18" customHeight="1">
       <c r="A103" s="21" t="s">
         <v>86</v>
       </c>
@@ -7332,7 +7728,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="104" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:17" ht="18" customHeight="1" thickBot="1">
       <c r="A104" s="56" t="s">
         <v>27</v>
       </c>
@@ -7374,7 +7770,7 @@
       <c r="P104" s="26"/>
       <c r="Q104" s="29"/>
     </row>
-    <row r="105" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:17" ht="18.75" customHeight="1">
       <c r="A105" s="56" t="s">
         <v>188</v>
       </c>
@@ -7441,7 +7837,7 @@
         <v>2.58E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:17" ht="18.75" customHeight="1">
       <c r="A106" s="56" t="s">
         <v>188</v>
       </c>
@@ -7508,7 +7904,7 @@
         <v>2.3760000000000007E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:17" ht="18.75" customHeight="1">
       <c r="A107" s="56" t="s">
         <v>188</v>
       </c>
@@ -7575,7 +7971,7 @@
         <v>2.3760000000000007E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:17" ht="18.75" customHeight="1">
       <c r="A108" s="56" t="s">
         <v>189</v>
       </c>
@@ -7642,7 +8038,7 @@
         <v>2.3760000000000007E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:17" ht="18.75" customHeight="1">
       <c r="A109" s="56" t="s">
         <v>189</v>
       </c>
@@ -7709,7 +8105,7 @@
         <v>2.3760000000000007E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:17" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:17" ht="19.5" customHeight="1" thickBot="1">
       <c r="A110" s="56" t="s">
         <v>189</v>
       </c>
@@ -7776,12 +8172,12 @@
         <v>2.3760000000000007E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:17" ht="18" customHeight="1">
       <c r="A112" s="21" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:5">
       <c r="A113" s="56" t="s">
         <v>27</v>
       </c>
@@ -7792,7 +8188,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" ht="18.75" customHeight="1">
       <c r="A114" s="56" t="s">
         <v>188</v>
       </c>
@@ -7808,7 +8204,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" ht="18.75" customHeight="1">
       <c r="A115" s="56" t="s">
         <v>189</v>
       </c>
@@ -7824,17 +8220,17 @@
         <v>205</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:5">
       <c r="A116" s="56"/>
       <c r="B116" s="56"/>
     </row>
-    <row r="117" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" ht="18" customHeight="1">
       <c r="A117" s="21" t="s">
         <v>207</v>
       </c>
       <c r="B117" s="56"/>
     </row>
-    <row r="118" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" ht="18.75" customHeight="1">
       <c r="A118" s="3" t="s">
         <v>209</v>
       </c>
@@ -7846,16 +8242,16 @@
         <v>205</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:5">
       <c r="A119" s="56"/>
       <c r="B119" s="56"/>
     </row>
-    <row r="120" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" ht="18" customHeight="1">
       <c r="A120" s="21" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" ht="18.75" customHeight="1">
       <c r="A121" s="3" t="s">
         <v>210</v>
       </c>
@@ -7867,12 +8263,12 @@
         <v>205</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" ht="18" customHeight="1">
       <c r="A123" s="52" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" ht="18" customHeight="1">
       <c r="A124" s="3" t="s">
         <v>212</v>
       </c>
@@ -7881,7 +8277,7 @@
         <v>0.42862495861865535</v>
       </c>
     </row>
-    <row r="126" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" ht="19.5" customHeight="1" thickBot="1">
       <c r="A126" s="52" t="s">
         <v>100</v>
       </c>
@@ -7889,7 +8285,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="127" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" ht="18" customHeight="1">
       <c r="A127" s="3" t="s">
         <v>213</v>
       </c>
@@ -7904,7 +8300,7 @@
         <v>7.12</v>
       </c>
     </row>
-    <row r="128" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" ht="18.75" customHeight="1">
       <c r="A128" s="11" t="s">
         <v>214</v>
       </c>
@@ -7923,7 +8319,7 @@
         <v>8.92</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A129" s="11" t="s">
         <v>104</v>
       </c>
@@ -7941,7 +8337,7 @@
         <v>9.2899999999999991</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:5" ht="18" customHeight="1">
       <c r="A130" s="3" t="s">
         <v>106</v>
       </c>
@@ -7953,12 +8349,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:5">
       <c r="A132" s="21" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:5">
       <c r="A133" s="3" t="s">
         <v>109</v>
       </c>
@@ -7970,382 +8366,13 @@
         <v>110</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:5">
       <c r="A134" s="11" t="s">
         <v>216</v>
       </c>
       <c r="B134" s="8">
         <v>0.04</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="13.1640625" style="8" customWidth="1"/>
-    <col min="10" max="10" width="12.1640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.1640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="52" t="s">
-        <v>145</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I2" s="8"/>
-    </row>
-    <row r="3" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B3" s="62">
-        <v>5.48</v>
-      </c>
-      <c r="C3" t="s">
-        <v>107</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B4" s="6">
-        <v>231874.33333333337</v>
-      </c>
-      <c r="C4" t="s">
-        <v>110</v>
-      </c>
-      <c r="I4" s="8"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
-        <v>216</v>
-      </c>
-      <c r="B5" s="61">
-        <f>Slab_Properties!B128</f>
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="11"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="52" t="s">
-        <v>147</v>
-      </c>
-      <c r="H7" s="56" t="s">
-        <v>148</v>
-      </c>
-      <c r="I7" s="56" t="s">
-        <v>149</v>
-      </c>
-      <c r="L7" s="56" t="s">
-        <v>150</v>
-      </c>
-      <c r="M7" s="8"/>
-    </row>
-    <row r="8" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="56" t="s">
-        <v>151</v>
-      </c>
-      <c r="B8" s="56" t="s">
-        <v>126</v>
-      </c>
-      <c r="C8" s="56" t="s">
-        <v>152</v>
-      </c>
-      <c r="D8" s="56" t="s">
-        <v>153</v>
-      </c>
-      <c r="E8" s="56" t="s">
-        <v>154</v>
-      </c>
-      <c r="F8" s="56" t="s">
-        <v>155</v>
-      </c>
-      <c r="G8" s="57" t="s">
-        <v>156</v>
-      </c>
-      <c r="H8" s="56" t="s">
-        <v>157</v>
-      </c>
-      <c r="I8" s="56" t="s">
-        <v>158</v>
-      </c>
-      <c r="J8" s="56" t="s">
-        <v>161</v>
-      </c>
-      <c r="K8" s="56" t="s">
-        <v>160</v>
-      </c>
-      <c r="L8" s="56" t="s">
-        <v>159</v>
-      </c>
-      <c r="M8" s="8"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="56"/>
-      <c r="B9" s="56" t="s">
-        <v>107</v>
-      </c>
-      <c r="C9" s="56" t="s">
-        <v>107</v>
-      </c>
-      <c r="D9" s="56" t="s">
-        <v>107</v>
-      </c>
-      <c r="E9" s="56" t="s">
-        <v>107</v>
-      </c>
-      <c r="F9" s="56" t="s">
-        <v>107</v>
-      </c>
-      <c r="G9" s="57"/>
-      <c r="H9" s="56" t="s">
-        <v>143</v>
-      </c>
-      <c r="I9" s="56" t="s">
-        <v>143</v>
-      </c>
-      <c r="J9" s="56" t="s">
-        <v>143</v>
-      </c>
-      <c r="K9" s="56" t="s">
-        <v>143</v>
-      </c>
-      <c r="L9" s="56" t="s">
-        <v>143</v>
-      </c>
-      <c r="M9" s="56" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="56" t="s">
-        <v>129</v>
-      </c>
-      <c r="B10" s="10">
-        <f>$B$3</f>
-        <v>5.48</v>
-      </c>
-      <c r="C10" s="56">
-        <v>1.25</v>
-      </c>
-      <c r="D10" s="56" t="s">
-        <v>172</v>
-      </c>
-      <c r="E10" s="56" t="s">
-        <v>172</v>
-      </c>
-      <c r="F10" s="56" t="s">
-        <v>172</v>
-      </c>
-      <c r="G10" s="56" t="s">
-        <v>172</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="I10" s="7">
-        <f>250000000/($B$4*$B$5)*($C10^2.43/$B10^1.8)*(1-EXP(-2*PI()*$B$5*$B10/$C10))</f>
-        <v>1448.4954817243618</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="K10" s="7">
-        <f>250000000/($B$4*$B$5)*($C10^2.43/$B10^1.8)*(1-EXP(-2*PI()*$B$5*$B10/$C10))</f>
-        <v>1448.4954817243618</v>
-      </c>
-      <c r="L10" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="M10" s="60">
-        <f>I10</f>
-        <v>1448.4954817243618</v>
-      </c>
-      <c r="N10" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="56" t="s">
-        <v>130</v>
-      </c>
-      <c r="B11" s="10">
-        <f>$B$3</f>
-        <v>5.48</v>
-      </c>
-      <c r="C11" s="56">
-        <v>1.6</v>
-      </c>
-      <c r="D11" s="56">
-        <v>6.8</v>
-      </c>
-      <c r="E11" s="56">
-        <v>6</v>
-      </c>
-      <c r="F11" s="56">
-        <v>8</v>
-      </c>
-      <c r="G11" s="56">
-        <v>0.1</v>
-      </c>
-      <c r="H11" s="7">
-        <f>175000000/($B$4*$B$5*SQRT($B11))*(EXP(-$G11*$B11))</f>
-        <v>4659.5258315145074</v>
-      </c>
-      <c r="I11" s="7">
-        <f t="shared" ref="I11:I13" si="0">250000000/($B$4*$B$5)*($C11^2.43/$B11^1.8)*(1-EXP(-2*PI()*$B$5*$B11/$C11))</f>
-        <v>2281.0838039192163</v>
-      </c>
-      <c r="J11" s="7">
-        <f>175000000/($B$4*$B$5*SQRT($E11))*(EXP(-$G11*$E11))</f>
-        <v>4227.3972905073051</v>
-      </c>
-      <c r="K11" s="7">
-        <f>250000000/($B$4*$B$5)*($C11^2.43/$F11^1.8)*(1-EXP(-2*PI()*$B$5*$F11/$C11))</f>
-        <v>1430.935514651278</v>
-      </c>
-      <c r="L11" s="7" t="str">
-        <f>IF(AND($B11&gt;$E11,$B11&lt;$F11),$J11 + ($B11-$E11) * ($K11-$J11)/($F11-$E11), "N/A")</f>
-        <v>N/A</v>
-      </c>
-      <c r="M11" s="60">
-        <f>IF($B11&gt;=F11,I11, IF($B11&lt;=E11,H11,L11))</f>
-        <v>4659.5258315145074</v>
-      </c>
-      <c r="N11" t="s">
-        <v>143</v>
-      </c>
-      <c r="O11" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="56" t="s">
-        <v>131</v>
-      </c>
-      <c r="B12" s="10">
-        <f>$B$3</f>
-        <v>5.48</v>
-      </c>
-      <c r="C12" s="56">
-        <v>1.85</v>
-      </c>
-      <c r="D12" s="56">
-        <v>8</v>
-      </c>
-      <c r="E12" s="56">
-        <v>7</v>
-      </c>
-      <c r="F12" s="56">
-        <v>9</v>
-      </c>
-      <c r="G12" s="56">
-        <v>0.09</v>
-      </c>
-      <c r="H12" s="7">
-        <f>175000000/($B$4*$B$5*SQRT($B12))*(EXP(-$G12*$B12))</f>
-        <v>4921.9937889204593</v>
-      </c>
-      <c r="I12" s="7">
-        <f t="shared" si="0"/>
-        <v>2952.7150695938485</v>
-      </c>
-      <c r="J12" s="7">
-        <f>175000000/($B$4*$B$5*SQRT($E12))*(EXP(-$G12*$E12))</f>
-        <v>3798.13883321924</v>
-      </c>
-      <c r="K12" s="7">
-        <f>250000000/($B$4*$B$5)*($C12^2.43/$F12^1.8)*(1-EXP(-2*PI()*$B$5*$F12/$C12))</f>
-        <v>1624.6168821294075</v>
-      </c>
-      <c r="L12" s="7" t="str">
-        <f t="shared" ref="L12:L13" si="1">IF(AND($B12&gt;$E12,$B12&lt;$F12),$J12 + ($B12-$E12) * ($K12-$J12)/($F12-$E12), "N/A")</f>
-        <v>N/A</v>
-      </c>
-      <c r="M12" s="60">
-        <f>IF($B12&gt;=F12,I12, IF($B12&lt;=E12,H12,L12))</f>
-        <v>4921.9937889204593</v>
-      </c>
-      <c r="N12" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="56" t="s">
-        <v>132</v>
-      </c>
-      <c r="B13" s="10">
-        <f>$B$3</f>
-        <v>5.48</v>
-      </c>
-      <c r="C13" s="56">
-        <v>2.1</v>
-      </c>
-      <c r="D13" s="56">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="E13" s="56">
-        <v>8</v>
-      </c>
-      <c r="F13" s="56">
-        <v>10</v>
-      </c>
-      <c r="G13" s="56">
-        <v>0.08</v>
-      </c>
-      <c r="H13" s="7">
-        <f>175000000/($B$4*$B$5*SQRT($B13))*(EXP(-$G13*$B13))</f>
-        <v>5199.2463899051454</v>
-      </c>
-      <c r="I13" s="7">
-        <f t="shared" si="0"/>
-        <v>3680.9272708591793</v>
-      </c>
-      <c r="J13" s="7">
-        <f>175000000/($B$4*$B$5*SQRT($E13))*(EXP(-$G13*$E13))</f>
-        <v>3517.4822707898952</v>
-      </c>
-      <c r="K13" s="7">
-        <f>250000000/($B$4*$B$5)*($C13^2.43/$F13^1.8)*(1-EXP(-2*PI()*$B$5*$F13/$C13))</f>
-        <v>1808.7386611958</v>
-      </c>
-      <c r="L13" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>N/A</v>
-      </c>
-      <c r="M13" s="60">
-        <f>IF($B13&gt;=F13,I13, IF($B13&lt;=E13,H13,L13))</f>
-        <v>5199.2463899051454</v>
-      </c>
-      <c r="N13" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="M14" s="52"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8354,35 +8381,403 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:O14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" style="8" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" s="52" t="s">
+        <v>145</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="1:15" ht="18" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" s="62">
+        <v>6.1525863330777328</v>
+      </c>
+      <c r="C3" t="s">
+        <v>107</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="6">
+        <v>231874.33333333337</v>
+      </c>
+      <c r="C4" t="s">
+        <v>110</v>
+      </c>
+      <c r="I4" s="8"/>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="B5" s="61">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="11"/>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="52" t="s">
+        <v>147</v>
+      </c>
+      <c r="H7" s="56" t="s">
+        <v>148</v>
+      </c>
+      <c r="I7" s="56" t="s">
+        <v>149</v>
+      </c>
+      <c r="L7" s="56" t="s">
+        <v>150</v>
+      </c>
+      <c r="M7" s="8"/>
+    </row>
+    <row r="8" spans="1:15" ht="18" customHeight="1">
+      <c r="A8" s="56" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8" s="56" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" s="56" t="s">
+        <v>152</v>
+      </c>
+      <c r="D8" s="56" t="s">
+        <v>153</v>
+      </c>
+      <c r="E8" s="56" t="s">
+        <v>154</v>
+      </c>
+      <c r="F8" s="56" t="s">
+        <v>155</v>
+      </c>
+      <c r="G8" s="57" t="s">
+        <v>156</v>
+      </c>
+      <c r="H8" s="56" t="s">
+        <v>157</v>
+      </c>
+      <c r="I8" s="56" t="s">
+        <v>158</v>
+      </c>
+      <c r="J8" s="56" t="s">
+        <v>161</v>
+      </c>
+      <c r="K8" s="56" t="s">
+        <v>160</v>
+      </c>
+      <c r="L8" s="56" t="s">
+        <v>159</v>
+      </c>
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="56"/>
+      <c r="B9" s="56" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="56" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" s="56" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="56" t="s">
+        <v>107</v>
+      </c>
+      <c r="F9" s="56" t="s">
+        <v>107</v>
+      </c>
+      <c r="G9" s="57"/>
+      <c r="H9" s="56" t="s">
+        <v>143</v>
+      </c>
+      <c r="I9" s="56" t="s">
+        <v>143</v>
+      </c>
+      <c r="J9" s="56" t="s">
+        <v>143</v>
+      </c>
+      <c r="K9" s="56" t="s">
+        <v>143</v>
+      </c>
+      <c r="L9" s="56" t="s">
+        <v>143</v>
+      </c>
+      <c r="M9" s="56" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10" s="10">
+        <f>$B$3</f>
+        <v>6.1525863330777328</v>
+      </c>
+      <c r="C10" s="56">
+        <v>1.25</v>
+      </c>
+      <c r="D10" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="E10" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="F10" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="G10" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="I10" s="7">
+        <f>250000000/($B$4*$B$5)*($C10^2.43/$B10^1.8)*(1-EXP(-2*PI()*$B$5*$B10/$C10))</f>
+        <v>1250.0488089213661</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="K10" s="7">
+        <f>250000000/($B$4*$B$5)*($C10^2.43/$B10^1.8)*(1-EXP(-2*PI()*$B$5*$B10/$C10))</f>
+        <v>1250.0488089213661</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="M10" s="60">
+        <f>I10</f>
+        <v>1250.0488089213661</v>
+      </c>
+      <c r="N10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="56" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" s="10">
+        <f>$B$3</f>
+        <v>6.1525863330777328</v>
+      </c>
+      <c r="C11" s="56">
+        <v>1.6</v>
+      </c>
+      <c r="D11" s="56">
+        <v>6.8</v>
+      </c>
+      <c r="E11" s="56">
+        <v>6</v>
+      </c>
+      <c r="F11" s="56">
+        <v>8</v>
+      </c>
+      <c r="G11" s="56">
+        <v>0.1</v>
+      </c>
+      <c r="H11" s="7">
+        <f>175000000/($B$4*$B$5*SQRT($B11))*(EXP(-$G11*$B11))</f>
+        <v>4111.4318077208081</v>
+      </c>
+      <c r="I11" s="7">
+        <f t="shared" ref="I11:I13" si="0">250000000/($B$4*$B$5)*($C11^2.43/$B11^1.8)*(1-EXP(-2*PI()*$B$5*$B11/$C11))</f>
+        <v>1988.0325851756511</v>
+      </c>
+      <c r="J11" s="7">
+        <f>175000000/($B$4*$B$5*SQRT($E11))*(EXP(-$G11*$E11))</f>
+        <v>4227.3972905073051</v>
+      </c>
+      <c r="K11" s="7">
+        <f>250000000/($B$4*$B$5)*($C11^2.43/$F11^1.8)*(1-EXP(-2*PI()*$B$5*$F11/$C11))</f>
+        <v>1430.935514651278</v>
+      </c>
+      <c r="L11" s="7">
+        <f>IF(AND($B11&gt;$E11,$B11&lt;$F11),$J11 + ($B11-$E11) * ($K11-$J11)/($F11-$E11), "N/A")</f>
+        <v>4014.0463665223469</v>
+      </c>
+      <c r="M11" s="60">
+        <f>IF($B11&gt;=F11,I11, IF($B11&lt;=E11,H11,L11))</f>
+        <v>4014.0463665223469</v>
+      </c>
+      <c r="N11" t="s">
+        <v>143</v>
+      </c>
+      <c r="O11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="56" t="s">
+        <v>131</v>
+      </c>
+      <c r="B12" s="10">
+        <f>$B$3</f>
+        <v>6.1525863330777328</v>
+      </c>
+      <c r="C12" s="56">
+        <v>1.85</v>
+      </c>
+      <c r="D12" s="56">
+        <v>8</v>
+      </c>
+      <c r="E12" s="56">
+        <v>7</v>
+      </c>
+      <c r="F12" s="56">
+        <v>9</v>
+      </c>
+      <c r="G12" s="56">
+        <v>0.09</v>
+      </c>
+      <c r="H12" s="7">
+        <f>175000000/($B$4*$B$5*SQRT($B12))*(EXP(-$G12*$B12))</f>
+        <v>4372.3350504141772</v>
+      </c>
+      <c r="I12" s="7">
+        <f t="shared" si="0"/>
+        <v>2586.6911926190824</v>
+      </c>
+      <c r="J12" s="7">
+        <f>175000000/($B$4*$B$5*SQRT($E12))*(EXP(-$G12*$E12))</f>
+        <v>3798.13883321924</v>
+      </c>
+      <c r="K12" s="7">
+        <f>250000000/($B$4*$B$5)*($C12^2.43/$F12^1.8)*(1-EXP(-2*PI()*$B$5*$F12/$C12))</f>
+        <v>1624.6168821294075</v>
+      </c>
+      <c r="L12" s="7" t="str">
+        <f t="shared" ref="L12:L13" si="1">IF(AND($B12&gt;$E12,$B12&lt;$F12),$J12 + ($B12-$E12) * ($K12-$J12)/($F12-$E12), "N/A")</f>
+        <v>N/A</v>
+      </c>
+      <c r="M12" s="60">
+        <f>IF($B12&gt;=F12,I12, IF($B12&lt;=E12,H12,L12))</f>
+        <v>4372.3350504141772</v>
+      </c>
+      <c r="N12" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="56" t="s">
+        <v>132</v>
+      </c>
+      <c r="B13" s="10">
+        <f>$B$3</f>
+        <v>6.1525863330777328</v>
+      </c>
+      <c r="C13" s="56">
+        <v>2.1</v>
+      </c>
+      <c r="D13" s="56">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="E13" s="56">
+        <v>8</v>
+      </c>
+      <c r="F13" s="56">
+        <v>10</v>
+      </c>
+      <c r="G13" s="56">
+        <v>0.08</v>
+      </c>
+      <c r="H13" s="7">
+        <f>175000000/($B$4*$B$5*SQRT($B13))*(EXP(-$G13*$B13))</f>
+        <v>4649.7946912752313</v>
+      </c>
+      <c r="I13" s="7">
+        <f t="shared" si="0"/>
+        <v>3237.9331287002856</v>
+      </c>
+      <c r="J13" s="7">
+        <f>175000000/($B$4*$B$5*SQRT($E13))*(EXP(-$G13*$E13))</f>
+        <v>3517.4822707898952</v>
+      </c>
+      <c r="K13" s="7">
+        <f>250000000/($B$4*$B$5)*($C13^2.43/$F13^1.8)*(1-EXP(-2*PI()*$B$5*$F13/$C13))</f>
+        <v>1808.7386611958</v>
+      </c>
+      <c r="L13" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>N/A</v>
+      </c>
+      <c r="M13" s="60">
+        <f>IF($B13&gt;=F13,I13, IF($B13&lt;=E13,H13,L13))</f>
+        <v>4649.7946912752313</v>
+      </c>
+      <c r="N13" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="M14" s="52"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AI42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.83203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:35" ht="18" customHeight="1">
       <c r="B1" s="56" t="s">
         <v>112</v>
       </c>
@@ -8486,7 +8881,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:35" ht="18" customHeight="1">
       <c r="A2" t="s">
         <v>133</v>
       </c>
@@ -8591,7 +8986,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:35">
       <c r="A3"/>
       <c r="B3" s="59"/>
       <c r="C3" s="59"/>
@@ -8625,7 +9020,7 @@
       <c r="AH3" s="56"/>
       <c r="AI3" s="56"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:35">
       <c r="A4"/>
       <c r="B4" s="59"/>
       <c r="C4" s="59"/>
@@ -8659,7 +9054,7 @@
       <c r="AH4" s="56"/>
       <c r="AI4" s="56"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:35">
       <c r="A5"/>
       <c r="B5" s="59"/>
       <c r="C5" s="59"/>
@@ -8693,7 +9088,7 @@
       <c r="AH5" s="56"/>
       <c r="AI5" s="56"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:35">
       <c r="A6"/>
       <c r="B6" s="59"/>
       <c r="C6" s="59"/>
@@ -8727,7 +9122,7 @@
       <c r="AH6" s="56"/>
       <c r="AI6" s="56"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:35">
       <c r="A7"/>
       <c r="B7" s="59"/>
       <c r="C7" s="59"/>
@@ -8761,7 +9156,7 @@
       <c r="AH7" s="56"/>
       <c r="AI7" s="56"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:35">
       <c r="A8"/>
       <c r="B8" s="59"/>
       <c r="C8" s="59"/>
@@ -8795,7 +9190,7 @@
       <c r="AH8" s="56"/>
       <c r="AI8" s="56"/>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:35">
       <c r="A9"/>
       <c r="B9" s="59"/>
       <c r="C9" s="59"/>
@@ -8829,7 +9224,7 @@
       <c r="AH9" s="56"/>
       <c r="AI9" s="56"/>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:35">
       <c r="A10"/>
       <c r="B10" s="59"/>
       <c r="C10" s="59"/>
@@ -8863,7 +9258,7 @@
       <c r="AH10" s="56"/>
       <c r="AI10" s="56"/>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:35">
       <c r="A11"/>
       <c r="B11" s="59"/>
       <c r="C11" s="59"/>
@@ -8897,7 +9292,7 @@
       <c r="AH11" s="56"/>
       <c r="AI11" s="56"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:35">
       <c r="A12"/>
       <c r="B12" s="59"/>
       <c r="C12" s="59"/>
@@ -8931,7 +9326,7 @@
       <c r="AH12" s="56"/>
       <c r="AI12" s="56"/>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:35">
       <c r="A13"/>
       <c r="B13" s="59"/>
       <c r="C13" s="59"/>
@@ -8965,7 +9360,7 @@
       <c r="AH13" s="56"/>
       <c r="AI13" s="56"/>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:35">
       <c r="A14"/>
       <c r="B14" s="59"/>
       <c r="C14" s="59"/>
@@ -8999,7 +9394,7 @@
       <c r="AH14" s="56"/>
       <c r="AI14" s="56"/>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:35">
       <c r="A15"/>
       <c r="B15" s="59"/>
       <c r="C15" s="59"/>
@@ -9033,7 +9428,7 @@
       <c r="AH15" s="56"/>
       <c r="AI15" s="56"/>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:35">
       <c r="A16"/>
       <c r="B16" s="59"/>
       <c r="C16" s="59"/>
@@ -9067,7 +9462,7 @@
       <c r="AH16" s="56"/>
       <c r="AI16" s="56"/>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:35">
       <c r="A17"/>
       <c r="B17" s="59"/>
       <c r="C17" s="59"/>
@@ -9101,7 +9496,7 @@
       <c r="AH17" s="56"/>
       <c r="AI17" s="56"/>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:35">
       <c r="A18"/>
       <c r="B18" s="59"/>
       <c r="C18" s="59"/>
@@ -9135,7 +9530,7 @@
       <c r="AH18" s="56"/>
       <c r="AI18" s="56"/>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:35">
       <c r="A19"/>
       <c r="B19" s="59"/>
       <c r="C19" s="59"/>
@@ -9169,7 +9564,7 @@
       <c r="AH19" s="56"/>
       <c r="AI19" s="56"/>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:35">
       <c r="A20"/>
       <c r="B20" s="59"/>
       <c r="C20" s="59"/>
@@ -9203,7 +9598,7 @@
       <c r="AH20" s="56"/>
       <c r="AI20" s="56"/>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:35">
       <c r="A21"/>
       <c r="B21" s="59"/>
       <c r="C21" s="59"/>
@@ -9237,7 +9632,7 @@
       <c r="AH21" s="56"/>
       <c r="AI21" s="56"/>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:35">
       <c r="A22"/>
       <c r="B22" s="59"/>
       <c r="C22" s="59"/>
@@ -9271,7 +9666,7 @@
       <c r="AH22" s="56"/>
       <c r="AI22" s="56"/>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:35">
       <c r="A23"/>
       <c r="B23" s="59"/>
       <c r="C23" s="59"/>
@@ -9305,7 +9700,7 @@
       <c r="AH23" s="56"/>
       <c r="AI23" s="56"/>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:35">
       <c r="A24"/>
       <c r="B24" s="59"/>
       <c r="C24" s="59"/>
@@ -9339,7 +9734,7 @@
       <c r="AH24" s="56"/>
       <c r="AI24" s="56"/>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:35">
       <c r="A25"/>
       <c r="B25" s="59"/>
       <c r="C25" s="59"/>
@@ -9373,7 +9768,7 @@
       <c r="AH25" s="56"/>
       <c r="AI25" s="56"/>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:35">
       <c r="A26"/>
       <c r="B26" s="59"/>
       <c r="C26" s="59"/>
@@ -9407,7 +9802,7 @@
       <c r="AH26" s="56"/>
       <c r="AI26" s="56"/>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:35">
       <c r="A27"/>
       <c r="B27" s="59"/>
       <c r="C27" s="59"/>
@@ -9441,7 +9836,7 @@
       <c r="AH27" s="56"/>
       <c r="AI27" s="56"/>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:35">
       <c r="A28"/>
       <c r="B28" s="59"/>
       <c r="C28" s="59"/>
@@ -9475,7 +9870,7 @@
       <c r="AH28" s="56"/>
       <c r="AI28" s="56"/>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:35">
       <c r="A29"/>
       <c r="B29" s="59"/>
       <c r="C29" s="59"/>
@@ -9509,7 +9904,7 @@
       <c r="AH29" s="56"/>
       <c r="AI29" s="56"/>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:35">
       <c r="A30"/>
       <c r="B30" s="59"/>
       <c r="C30" s="59"/>
@@ -9543,7 +9938,7 @@
       <c r="AH30" s="56"/>
       <c r="AI30" s="56"/>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:35">
       <c r="A31"/>
       <c r="B31" s="59"/>
       <c r="C31" s="59"/>
@@ -9577,7 +9972,7 @@
       <c r="AH31" s="56"/>
       <c r="AI31" s="56"/>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:35">
       <c r="A32"/>
       <c r="B32" s="59"/>
       <c r="C32" s="59"/>
@@ -9611,7 +10006,7 @@
       <c r="AH32" s="56"/>
       <c r="AI32" s="56"/>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:35">
       <c r="A33"/>
       <c r="B33" s="59"/>
       <c r="C33" s="59"/>
@@ -9645,7 +10040,7 @@
       <c r="AH33" s="56"/>
       <c r="AI33" s="56"/>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:35">
       <c r="A34"/>
       <c r="B34" s="59"/>
       <c r="C34" s="59"/>
@@ -9679,7 +10074,7 @@
       <c r="AH34" s="56"/>
       <c r="AI34" s="56"/>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:35">
       <c r="A35"/>
       <c r="B35" s="59"/>
       <c r="C35" s="59"/>
@@ -9713,7 +10108,7 @@
       <c r="AH35" s="56"/>
       <c r="AI35" s="56"/>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:35">
       <c r="A36"/>
       <c r="B36" s="59"/>
       <c r="C36" s="59"/>
@@ -9747,7 +10142,7 @@
       <c r="AH36" s="56"/>
       <c r="AI36" s="56"/>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:35">
       <c r="A37"/>
       <c r="B37" s="59"/>
       <c r="C37" s="59"/>
@@ -9781,7 +10176,7 @@
       <c r="AH37" s="56"/>
       <c r="AI37" s="56"/>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:35">
       <c r="A38"/>
       <c r="B38" s="59"/>
       <c r="C38" s="59"/>
@@ -9815,7 +10210,7 @@
       <c r="AH38" s="56"/>
       <c r="AI38" s="56"/>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:35">
       <c r="A39"/>
       <c r="B39" s="59"/>
       <c r="C39" s="59"/>
@@ -9849,7 +10244,7 @@
       <c r="AH39" s="56"/>
       <c r="AI39" s="56"/>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:35">
       <c r="A40"/>
       <c r="B40" s="59"/>
       <c r="C40" s="59"/>
@@ -9883,7 +10278,7 @@
       <c r="AH40" s="56"/>
       <c r="AI40" s="56"/>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:35">
       <c r="A41"/>
       <c r="B41" s="59"/>
       <c r="C41" s="59"/>
@@ -9917,7 +10312,7 @@
       <c r="AH41" s="56"/>
       <c r="AI41" s="56"/>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:35">
       <c r="A42"/>
       <c r="B42" s="59"/>
       <c r="C42" s="59"/>
@@ -9962,26 +10357,26 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A2:Q128"/>
   <sheetViews>
     <sheetView topLeftCell="A100" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="O126" sqref="O126"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" style="8" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="8" customWidth="1"/>
     <col min="5" max="5" width="12" style="8" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="8" customWidth="1"/>
-    <col min="8" max="9" width="11.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="11.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="8" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="8" customWidth="1"/>
+    <col min="8" max="9" width="11.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="11.42578125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="52" t="s">
         <v>0</v>
       </c>
@@ -9989,7 +10384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="18" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -10006,7 +10401,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="18" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -10020,7 +10415,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="18" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -10032,7 +10427,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="18" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -10043,7 +10438,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="18" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
@@ -10054,7 +10449,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -10062,7 +10457,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="18" customHeight="1">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
@@ -10073,7 +10468,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="18" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
@@ -10084,7 +10479,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="18" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
@@ -10099,7 +10494,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
@@ -10110,7 +10505,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
@@ -10121,7 +10516,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="18" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
@@ -10132,7 +10527,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="18" customHeight="1">
       <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
@@ -10144,7 +10539,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
@@ -10153,7 +10548,7 @@
         <v>5.9315173688353893</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="18" customHeight="1">
       <c r="A17" s="11" t="s">
         <v>24</v>
       </c>
@@ -10162,7 +10557,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="18" customHeight="1">
       <c r="A18" s="3" t="s">
         <v>25</v>
       </c>
@@ -10174,15 +10569,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" s="3"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" s="21" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" s="3" t="s">
         <v>27</v>
       </c>
@@ -10193,7 +10588,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="18" customHeight="1">
       <c r="A22" s="3" t="s">
         <v>30</v>
       </c>
@@ -10212,7 +10607,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="18" customHeight="1">
       <c r="A23" s="3" t="s">
         <v>32</v>
       </c>
@@ -10228,12 +10623,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26" s="3" t="s">
         <v>34</v>
       </c>
@@ -10244,7 +10639,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27" s="3" t="s">
         <v>36</v>
       </c>
@@ -10255,7 +10650,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="18" customHeight="1">
       <c r="A28" s="3" t="s">
         <v>37</v>
       </c>
@@ -10266,7 +10661,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29" s="3" t="s">
         <v>38</v>
       </c>
@@ -10278,7 +10673,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="17.25" customHeight="1">
       <c r="A30" s="3" t="s">
         <v>39</v>
       </c>
@@ -10290,7 +10685,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31" s="3" t="s">
         <v>41</v>
       </c>
@@ -10302,11 +10697,11 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
       <c r="A32" s="3"/>
       <c r="B32" s="6"/>
     </row>
-    <row r="33" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
       <c r="A33" s="21" t="s">
         <v>43</v>
       </c>
@@ -10317,7 +10712,7 @@
       <c r="G33" s="54"/>
       <c r="H33" s="55"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14">
       <c r="A34" s="3"/>
       <c r="F34" s="45" t="s">
         <v>45</v>
@@ -10344,7 +10739,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" ht="18" customHeight="1">
       <c r="A35" s="21" t="s">
         <v>47</v>
       </c>
@@ -10373,7 +10768,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="18.75" customHeight="1" thickBot="1">
       <c r="A36" s="3" t="s">
         <v>48</v>
       </c>
@@ -10409,7 +10804,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" ht="18" customHeight="1">
       <c r="A37" s="3" t="s">
         <v>52</v>
       </c>
@@ -10448,7 +10843,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" ht="18" customHeight="1">
       <c r="A38" s="3" t="s">
         <v>55</v>
       </c>
@@ -10490,7 +10885,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" ht="18.75" customHeight="1" thickBot="1">
       <c r="E39" s="3" t="s">
         <v>58</v>
       </c>
@@ -10519,7 +10914,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14">
       <c r="A40" s="3" t="s">
         <v>59</v>
       </c>
@@ -10540,7 +10935,7 @@
       <c r="L40" s="56"/>
       <c r="M40" s="56"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14">
       <c r="A41" s="3" t="s">
         <v>60</v>
       </c>
@@ -10561,7 +10956,7 @@
       <c r="L41" s="56"/>
       <c r="M41" s="56"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14">
       <c r="A42" s="3" t="s">
         <v>61</v>
       </c>
@@ -10582,7 +10977,7 @@
       <c r="L42" s="56"/>
       <c r="M42" s="56"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14">
       <c r="A43" s="3" t="s">
         <v>62</v>
       </c>
@@ -10603,7 +10998,7 @@
       <c r="L43" s="56"/>
       <c r="M43" s="56"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14">
       <c r="A44" s="3" t="s">
         <v>63</v>
       </c>
@@ -10624,7 +11019,7 @@
       <c r="L44" s="56"/>
       <c r="M44" s="56"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14">
       <c r="A45" s="3" t="s">
         <v>64</v>
       </c>
@@ -10645,7 +11040,7 @@
       <c r="L45" s="56"/>
       <c r="M45" s="56"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14">
       <c r="E46" s="3"/>
       <c r="F46" s="56"/>
       <c r="G46" s="56"/>
@@ -10656,7 +11051,7 @@
       <c r="L46" s="56"/>
       <c r="M46" s="56"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14">
       <c r="A47" s="21" t="s">
         <v>65</v>
       </c>
@@ -10670,7 +11065,7 @@
       <c r="L47" s="56"/>
       <c r="M47" s="56"/>
     </row>
-    <row r="48" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" ht="18" customHeight="1">
       <c r="A48" s="3" t="s">
         <v>66</v>
       </c>
@@ -10691,7 +11086,7 @@
       <c r="L48" s="56"/>
       <c r="M48" s="56"/>
     </row>
-    <row r="49" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" ht="18" customHeight="1">
       <c r="A49" s="3" t="s">
         <v>68</v>
       </c>
@@ -10712,7 +11107,7 @@
       <c r="L49" s="56"/>
       <c r="M49" s="56"/>
     </row>
-    <row r="50" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" ht="18" customHeight="1">
       <c r="A50" s="3" t="s">
         <v>69</v>
       </c>
@@ -10733,7 +11128,7 @@
       <c r="L50" s="56"/>
       <c r="M50" s="56"/>
     </row>
-    <row r="51" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" ht="18" customHeight="1">
       <c r="A51" s="3" t="s">
         <v>70</v>
       </c>
@@ -10754,7 +11149,7 @@
       <c r="L51" s="56"/>
       <c r="M51" s="56"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13">
       <c r="A52" s="3"/>
       <c r="B52" s="7"/>
       <c r="E52" s="3"/>
@@ -10767,12 +11162,12 @@
       <c r="L52" s="56"/>
       <c r="M52" s="56"/>
     </row>
-    <row r="53" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" ht="18" customHeight="1">
       <c r="A53" s="21" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13">
       <c r="A54" s="56" t="s">
         <v>27</v>
       </c>
@@ -10789,7 +11184,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" ht="18" customHeight="1">
       <c r="A55" s="56" t="s">
         <v>30</v>
       </c>
@@ -10811,7 +11206,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" ht="18" customHeight="1">
       <c r="A56" s="56" t="s">
         <v>30</v>
       </c>
@@ -10833,7 +11228,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" ht="18" customHeight="1">
       <c r="A57" s="56" t="s">
         <v>30</v>
       </c>
@@ -10855,7 +11250,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" ht="18" customHeight="1">
       <c r="A58" s="56" t="s">
         <v>30</v>
       </c>
@@ -10877,7 +11272,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" ht="18" customHeight="1">
       <c r="A59" s="56" t="s">
         <v>30</v>
       </c>
@@ -10899,7 +11294,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" ht="18" customHeight="1">
       <c r="A60" s="56" t="s">
         <v>30</v>
       </c>
@@ -10921,7 +11316,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" ht="18" customHeight="1">
       <c r="A61" s="56" t="s">
         <v>32</v>
       </c>
@@ -10943,7 +11338,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" ht="18" customHeight="1">
       <c r="A62" s="56" t="s">
         <v>32</v>
       </c>
@@ -10965,7 +11360,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" ht="18" customHeight="1">
       <c r="A63" s="56" t="s">
         <v>32</v>
       </c>
@@ -10987,7 +11382,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" ht="18" customHeight="1">
       <c r="A64" s="56" t="s">
         <v>32</v>
       </c>
@@ -11009,7 +11404,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" ht="18" customHeight="1">
       <c r="A65" s="56" t="s">
         <v>32</v>
       </c>
@@ -11031,7 +11426,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" ht="18" customHeight="1">
       <c r="A66" s="56" t="s">
         <v>32</v>
       </c>
@@ -11053,12 +11448,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12" ht="18" customHeight="1">
       <c r="A69" s="52" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12">
       <c r="A70" s="56" t="s">
         <v>27</v>
       </c>
@@ -11072,7 +11467,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12" ht="18" customHeight="1">
       <c r="A71" s="56" t="s">
         <v>30</v>
       </c>
@@ -11091,7 +11486,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" ht="18" customHeight="1">
       <c r="A72" s="56" t="s">
         <v>30</v>
       </c>
@@ -11110,7 +11505,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12" ht="18" customHeight="1">
       <c r="A73" s="56" t="s">
         <v>30</v>
       </c>
@@ -11129,7 +11524,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" ht="18" customHeight="1">
       <c r="A74" s="56" t="s">
         <v>32</v>
       </c>
@@ -11148,7 +11543,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" ht="18" customHeight="1">
       <c r="A75" s="56" t="s">
         <v>32</v>
       </c>
@@ -11167,7 +11562,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12" ht="18" customHeight="1">
       <c r="A76" s="56" t="s">
         <v>32</v>
       </c>
@@ -11186,7 +11581,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:12" ht="18" customHeight="1">
       <c r="A78" s="21" t="s">
         <v>80</v>
       </c>
@@ -11194,7 +11589,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12">
       <c r="A79" s="56" t="s">
         <v>27</v>
       </c>
@@ -11223,7 +11618,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" ht="18.75" customHeight="1">
       <c r="A80" s="56" t="s">
         <v>30</v>
       </c>
@@ -11261,7 +11656,7 @@
       <c r="K80" s="9"/>
       <c r="L80" s="9"/>
     </row>
-    <row r="81" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:17" ht="18.75" customHeight="1">
       <c r="A81" s="56" t="s">
         <v>30</v>
       </c>
@@ -11299,7 +11694,7 @@
       <c r="K81" s="9"/>
       <c r="L81" s="9"/>
     </row>
-    <row r="82" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:17" ht="18.75" customHeight="1">
       <c r="A82" s="56" t="s">
         <v>30</v>
       </c>
@@ -11337,7 +11732,7 @@
       <c r="K82" s="9"/>
       <c r="L82" s="9"/>
     </row>
-    <row r="83" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:17" ht="18.75" customHeight="1">
       <c r="A83" s="56" t="s">
         <v>32</v>
       </c>
@@ -11375,7 +11770,7 @@
       <c r="K83" s="9"/>
       <c r="L83" s="9"/>
     </row>
-    <row r="84" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:17" ht="18.75" customHeight="1">
       <c r="A84" s="56" t="s">
         <v>32</v>
       </c>
@@ -11413,7 +11808,7 @@
       <c r="K84" s="9"/>
       <c r="L84" s="9"/>
     </row>
-    <row r="85" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:17" ht="18.75" customHeight="1">
       <c r="A85" s="56" t="s">
         <v>32</v>
       </c>
@@ -11451,12 +11846,12 @@
       <c r="K85" s="9"/>
       <c r="L85" s="9"/>
     </row>
-    <row r="87" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:17" ht="18" customHeight="1">
       <c r="A87" s="21" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:17">
       <c r="A88" s="56" t="s">
         <v>27</v>
       </c>
@@ -11470,7 +11865,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="89" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:17" ht="18.75" customHeight="1">
       <c r="A89" s="56" t="s">
         <v>30</v>
       </c>
@@ -11489,7 +11884,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="90" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:17" ht="18.75" customHeight="1">
       <c r="A90" s="56" t="s">
         <v>30</v>
       </c>
@@ -11508,7 +11903,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="91" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:17" ht="18.75" customHeight="1">
       <c r="A91" s="56" t="s">
         <v>30</v>
       </c>
@@ -11527,7 +11922,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="92" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:17" ht="18.75" customHeight="1">
       <c r="A92" s="56" t="s">
         <v>32</v>
       </c>
@@ -11546,7 +11941,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="93" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:17" ht="18.75" customHeight="1">
       <c r="A93" s="56" t="s">
         <v>32</v>
       </c>
@@ -11565,7 +11960,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="94" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:17" ht="18.75" customHeight="1">
       <c r="A94" s="56" t="s">
         <v>32</v>
       </c>
@@ -11584,8 +11979,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="95" spans="1:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:17" ht="15.75" customHeight="1" thickBot="1"/>
+    <row r="96" spans="1:17">
       <c r="F96" s="38" t="s">
         <v>28</v>
       </c>
@@ -11623,7 +12018,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="97" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:17" ht="18" customHeight="1">
       <c r="A97" s="21" t="s">
         <v>86</v>
       </c>
@@ -11664,7 +12059,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="98" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" ht="18" customHeight="1" thickBot="1">
       <c r="A98" s="56" t="s">
         <v>27</v>
       </c>
@@ -11706,7 +12101,7 @@
       <c r="P98" s="26"/>
       <c r="Q98" s="29"/>
     </row>
-    <row r="99" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:17" ht="18.75" customHeight="1">
       <c r="A99" s="56" t="s">
         <v>30</v>
       </c>
@@ -11773,7 +12168,7 @@
         <v>4.3944649990503321E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:17" ht="18.75" customHeight="1">
       <c r="A100" s="56" t="s">
         <v>30</v>
       </c>
@@ -11840,7 +12235,7 @@
         <v>3.0000000000000002E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:17" ht="18.75" customHeight="1">
       <c r="A101" s="56" t="s">
         <v>30</v>
       </c>
@@ -11907,7 +12302,7 @@
         <v>3.5704726064266931E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:17" ht="18.75" customHeight="1">
       <c r="A102" s="56" t="s">
         <v>32</v>
       </c>
@@ -11974,7 +12369,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="103" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:17" ht="18.75" customHeight="1">
       <c r="A103" s="56" t="s">
         <v>32</v>
       </c>
@@ -12041,7 +12436,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="104" spans="1:17" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:17" ht="19.5" customHeight="1" thickBot="1">
       <c r="A104" s="56" t="s">
         <v>32</v>
       </c>
@@ -12108,12 +12503,12 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="106" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:17" ht="18" customHeight="1">
       <c r="A106" s="21" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:17">
       <c r="A107" s="56" t="s">
         <v>27</v>
       </c>
@@ -12124,7 +12519,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="108" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:17" ht="18.75" customHeight="1">
       <c r="A108" s="56" t="s">
         <v>30</v>
       </c>
@@ -12140,7 +12535,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="109" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:17" ht="18.75" customHeight="1">
       <c r="A109" s="56" t="s">
         <v>32</v>
       </c>
@@ -12156,17 +12551,17 @@
         <v>85</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:17">
       <c r="A110" s="56"/>
       <c r="B110" s="56"/>
     </row>
-    <row r="111" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:17" ht="18" customHeight="1">
       <c r="A111" s="21" t="s">
         <v>94</v>
       </c>
       <c r="B111" s="56"/>
     </row>
-    <row r="112" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:17" ht="18.75" customHeight="1">
       <c r="A112" s="3" t="s">
         <v>95</v>
       </c>
@@ -12178,16 +12573,16 @@
         <v>85</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:5">
       <c r="A113" s="56"/>
       <c r="B113" s="56"/>
     </row>
-    <row r="114" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5" ht="18" customHeight="1">
       <c r="A114" s="21" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:5" ht="18.75" customHeight="1">
       <c r="A115" s="3" t="s">
         <v>97</v>
       </c>
@@ -12199,12 +12594,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:5" ht="18" customHeight="1">
       <c r="A117" s="52" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:5" ht="18" customHeight="1">
       <c r="A118" s="3" t="s">
         <v>99</v>
       </c>
@@ -12213,7 +12608,7 @@
         <v>0.54614289068960964</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" ht="19.5" customHeight="1" thickBot="1">
       <c r="A120" s="52" t="s">
         <v>100</v>
       </c>
@@ -12221,7 +12616,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:5" ht="18" customHeight="1">
       <c r="A121" s="3" t="s">
         <v>102</v>
       </c>
@@ -12236,7 +12631,7 @@
         <v>7.12</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5" ht="18.75" customHeight="1">
       <c r="A122" s="11" t="s">
         <v>103</v>
       </c>
@@ -12255,7 +12650,7 @@
         <v>8.92</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A123" s="11" t="s">
         <v>104</v>
       </c>
@@ -12273,7 +12668,7 @@
         <v>9.2899999999999991</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:5" ht="18" customHeight="1">
       <c r="A124" s="3" t="s">
         <v>106</v>
       </c>
@@ -12285,12 +12680,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:5">
       <c r="A126" s="21" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:5">
       <c r="A127" s="3" t="s">
         <v>109</v>
       </c>
@@ -12302,7 +12697,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:5">
       <c r="A128" s="11" t="s">
         <v>111</v>
       </c>

</xml_diff>

<commit_message>
fixed drop panel to use two_way_slab
</commit_message>
<xml_diff>
--- a/Flat_Plate_Vibration_Template.xlsx
+++ b/Flat_Plate_Vibration_Template.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27809"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mwachter\workspaces\vibraslab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maryannewachter/workspaces/vibraslab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B60B392F-6317-40CD-853E-658899DD6CBC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="33600" windowHeight="18975" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18980" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Slab_Properties" sheetId="1" r:id="rId1"/>
@@ -185,7 +184,7 @@
     <definedName name="y_t">#REF!</definedName>
     <definedName name="y_tdrop">Drop_Slab_Properties!$B$17</definedName>
   </definedNames>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -1916,12 +1915,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2738,29 +2737,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S128"/>
   <sheetViews>
     <sheetView topLeftCell="A118" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="B128" activeCellId="2" sqref="B124 B127 B128"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" style="8" customWidth="1"/>
     <col min="4" max="5" width="12" style="8" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="8" customWidth="1"/>
-    <col min="8" max="9" width="11.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="11.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="8" customWidth="1"/>
+    <col min="8" max="9" width="11.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="11.5" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="I1" s="8" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="52" t="s">
         <v>0</v>
       </c>
@@ -2768,7 +2767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="18" customHeight="1">
+    <row r="3" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>176</v>
       </c>
@@ -2788,7 +2787,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="18" customHeight="1">
+    <row r="4" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>177</v>
       </c>
@@ -2805,7 +2804,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="18" customHeight="1">
+    <row r="5" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>178</v>
       </c>
@@ -2820,7 +2819,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="18" customHeight="1">
+    <row r="6" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>179</v>
       </c>
@@ -2831,7 +2830,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="18" customHeight="1">
+    <row r="7" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>180</v>
       </c>
@@ -2842,7 +2841,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -2850,7 +2849,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="18" customHeight="1">
+    <row r="9" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>181</v>
       </c>
@@ -2861,7 +2860,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="18" customHeight="1">
+    <row r="10" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>182</v>
       </c>
@@ -2872,7 +2871,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="18" customHeight="1">
+    <row r="11" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>183</v>
       </c>
@@ -2887,7 +2886,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="18">
+    <row r="12" spans="1:19" ht="17" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
@@ -2943,7 +2942,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
@@ -2958,7 +2957,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="18" customHeight="1">
+    <row r="14" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>184</v>
       </c>
@@ -2969,7 +2968,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="18" customHeight="1">
+    <row r="15" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>185</v>
       </c>
@@ -2981,7 +2980,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
@@ -2990,7 +2989,7 @@
         <v>5.6374268708751352</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="18" customHeight="1">
+    <row r="17" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>186</v>
       </c>
@@ -3002,7 +3001,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="18" customHeight="1">
+    <row r="18" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>187</v>
       </c>
@@ -3017,15 +3016,15 @@
         <v>166</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="21" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>27</v>
       </c>
@@ -3036,7 +3035,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="18" customHeight="1">
+    <row r="22" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>188</v>
       </c>
@@ -3055,7 +3054,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="18" customHeight="1">
+    <row r="23" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>189</v>
       </c>
@@ -3071,12 +3070,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>34</v>
       </c>
@@ -3087,7 +3086,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>36</v>
       </c>
@@ -3098,7 +3097,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="18" customHeight="1">
+    <row r="28" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>37</v>
       </c>
@@ -3109,7 +3108,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>38</v>
       </c>
@@ -3121,7 +3120,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="17.25" customHeight="1">
+    <row r="30" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>39</v>
       </c>
@@ -3133,7 +3132,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>41</v>
       </c>
@@ -3145,11 +3144,11 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="6"/>
     </row>
-    <row r="33" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
+    <row r="33" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
         <v>43</v>
       </c>
@@ -3160,7 +3159,7 @@
       <c r="G33" s="54"/>
       <c r="H33" s="55"/>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="F34" s="45" t="s">
         <v>45</v>
@@ -3187,7 +3186,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="18" customHeight="1">
+    <row r="35" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="21" t="s">
         <v>47</v>
       </c>
@@ -3216,7 +3215,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="18.75" customHeight="1" thickBot="1">
+    <row r="36" spans="1:14" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>191</v>
       </c>
@@ -3252,7 +3251,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="18" customHeight="1">
+    <row r="37" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>192</v>
       </c>
@@ -3291,7 +3290,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="18" customHeight="1">
+    <row r="38" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>193</v>
       </c>
@@ -3333,7 +3332,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="18.75" customHeight="1" thickBot="1">
+    <row r="39" spans="1:14" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E39" s="3" t="s">
         <v>58</v>
       </c>
@@ -3362,7 +3361,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="18">
+    <row r="40" spans="1:14" ht="17" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>194</v>
       </c>
@@ -3383,7 +3382,7 @@
       <c r="L40" s="56"/>
       <c r="M40" s="56"/>
     </row>
-    <row r="41" spans="1:14" ht="18">
+    <row r="41" spans="1:14" ht="17" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>195</v>
       </c>
@@ -3404,7 +3403,7 @@
       <c r="L41" s="56"/>
       <c r="M41" s="56"/>
     </row>
-    <row r="42" spans="1:14" ht="18">
+    <row r="42" spans="1:14" ht="17" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>196</v>
       </c>
@@ -3425,7 +3424,7 @@
       <c r="L42" s="56"/>
       <c r="M42" s="56"/>
     </row>
-    <row r="43" spans="1:14" ht="18">
+    <row r="43" spans="1:14" ht="17" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>197</v>
       </c>
@@ -3446,7 +3445,7 @@
       <c r="L43" s="56"/>
       <c r="M43" s="56"/>
     </row>
-    <row r="44" spans="1:14" ht="18">
+    <row r="44" spans="1:14" ht="17" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>198</v>
       </c>
@@ -3467,7 +3466,7 @@
       <c r="L44" s="56"/>
       <c r="M44" s="56"/>
     </row>
-    <row r="45" spans="1:14" ht="18">
+    <row r="45" spans="1:14" ht="17" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>199</v>
       </c>
@@ -3488,7 +3487,7 @@
       <c r="L45" s="56"/>
       <c r="M45" s="56"/>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E46" s="3"/>
       <c r="F46" s="56"/>
       <c r="G46" s="56"/>
@@ -3499,7 +3498,7 @@
       <c r="L46" s="56"/>
       <c r="M46" s="56"/>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="21" t="s">
         <v>65</v>
       </c>
@@ -3513,7 +3512,7 @@
       <c r="L47" s="56"/>
       <c r="M47" s="56"/>
     </row>
-    <row r="48" spans="1:14" ht="18" customHeight="1">
+    <row r="48" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>200</v>
       </c>
@@ -3537,7 +3536,7 @@
       <c r="L48" s="56"/>
       <c r="M48" s="56"/>
     </row>
-    <row r="49" spans="1:13" ht="18" customHeight="1">
+    <row r="49" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>201</v>
       </c>
@@ -3558,7 +3557,7 @@
       <c r="L49" s="56"/>
       <c r="M49" s="56"/>
     </row>
-    <row r="50" spans="1:13" ht="18" customHeight="1">
+    <row r="50" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>202</v>
       </c>
@@ -3579,7 +3578,7 @@
       <c r="L50" s="56"/>
       <c r="M50" s="56"/>
     </row>
-    <row r="51" spans="1:13" ht="18" customHeight="1">
+    <row r="51" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>203</v>
       </c>
@@ -3600,7 +3599,7 @@
       <c r="L51" s="56"/>
       <c r="M51" s="56"/>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="3"/>
       <c r="B52" s="7"/>
       <c r="E52" s="3"/>
@@ -3613,12 +3612,12 @@
       <c r="L52" s="56"/>
       <c r="M52" s="56"/>
     </row>
-    <row r="53" spans="1:13" ht="18" customHeight="1">
+    <row r="53" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="21" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="56" t="s">
         <v>27</v>
       </c>
@@ -3635,7 +3634,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="18" customHeight="1">
+    <row r="55" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="56" t="s">
         <v>188</v>
       </c>
@@ -3657,7 +3656,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="18" customHeight="1">
+    <row r="56" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="56" t="s">
         <v>188</v>
       </c>
@@ -3679,7 +3678,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="18" customHeight="1">
+    <row r="57" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="56" t="s">
         <v>188</v>
       </c>
@@ -3701,7 +3700,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="18" customHeight="1">
+    <row r="58" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="56" t="s">
         <v>188</v>
       </c>
@@ -3723,7 +3722,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="18" customHeight="1">
+    <row r="59" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="56" t="s">
         <v>188</v>
       </c>
@@ -3745,7 +3744,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="18" customHeight="1">
+    <row r="60" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="56" t="s">
         <v>188</v>
       </c>
@@ -3767,7 +3766,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="18" customHeight="1">
+    <row r="61" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="56" t="s">
         <v>189</v>
       </c>
@@ -3789,7 +3788,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="18" customHeight="1">
+    <row r="62" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="56" t="s">
         <v>189</v>
       </c>
@@ -3811,7 +3810,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="18" customHeight="1">
+    <row r="63" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="56" t="s">
         <v>189</v>
       </c>
@@ -3833,7 +3832,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="18" customHeight="1">
+    <row r="64" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="56" t="s">
         <v>189</v>
       </c>
@@ -3855,7 +3854,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="18" customHeight="1">
+    <row r="65" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="56" t="s">
         <v>189</v>
       </c>
@@ -3877,7 +3876,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="66" spans="1:19" ht="18" customHeight="1">
+    <row r="66" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="56" t="s">
         <v>189</v>
       </c>
@@ -3899,12 +3898,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="69" spans="1:19" ht="18" customHeight="1">
+    <row r="69" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="52" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="70" spans="1:19">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A70" s="56" t="s">
         <v>27</v>
       </c>
@@ -3918,7 +3917,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="71" spans="1:19" ht="18" customHeight="1">
+    <row r="71" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="56" t="s">
         <v>188</v>
       </c>
@@ -3937,7 +3936,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="72" spans="1:19" ht="18" customHeight="1">
+    <row r="72" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="56" t="s">
         <v>188</v>
       </c>
@@ -3956,7 +3955,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="73" spans="1:19" ht="18" customHeight="1">
+    <row r="73" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="56" t="s">
         <v>188</v>
       </c>
@@ -3975,7 +3974,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="74" spans="1:19" ht="18" customHeight="1">
+    <row r="74" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="56" t="s">
         <v>189</v>
       </c>
@@ -3994,7 +3993,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="75" spans="1:19" ht="18" customHeight="1">
+    <row r="75" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="56" t="s">
         <v>189</v>
       </c>
@@ -4013,7 +4012,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="76" spans="1:19" ht="18" customHeight="1">
+    <row r="76" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="56" t="s">
         <v>189</v>
       </c>
@@ -4032,7 +4031,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="78" spans="1:19" ht="18" customHeight="1">
+    <row r="78" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="21" t="s">
         <v>80</v>
       </c>
@@ -4048,7 +4047,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="79" spans="1:19">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A79" s="56" t="s">
         <v>27</v>
       </c>
@@ -4099,7 +4098,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="80" spans="1:19" ht="18.75" customHeight="1">
+    <row r="80" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="56" t="s">
         <v>188</v>
       </c>
@@ -4162,7 +4161,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:19" ht="18.75" customHeight="1">
+    <row r="81" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="56" t="s">
         <v>188</v>
       </c>
@@ -4225,7 +4224,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:19" ht="18.75" customHeight="1">
+    <row r="82" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="56" t="s">
         <v>188</v>
       </c>
@@ -4288,7 +4287,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:19" ht="18.75" customHeight="1">
+    <row r="83" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="56" t="s">
         <v>189</v>
       </c>
@@ -4351,7 +4350,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:19" ht="18.75" customHeight="1">
+    <row r="84" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="56" t="s">
         <v>189</v>
       </c>
@@ -4414,7 +4413,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="85" spans="1:19" ht="18.75" customHeight="1">
+    <row r="85" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="56" t="s">
         <v>189</v>
       </c>
@@ -4477,12 +4476,12 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="87" spans="1:19" ht="18" customHeight="1">
+    <row r="87" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="21" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="88" spans="1:19">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A88" s="56" t="s">
         <v>27</v>
       </c>
@@ -4496,7 +4495,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="89" spans="1:19" ht="18.75" customHeight="1">
+    <row r="89" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="56" t="s">
         <v>188</v>
       </c>
@@ -4515,7 +4514,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="90" spans="1:19" ht="18.75" customHeight="1">
+    <row r="90" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="56" t="s">
         <v>188</v>
       </c>
@@ -4534,7 +4533,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="91" spans="1:19" ht="18.75" customHeight="1">
+    <row r="91" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="56" t="s">
         <v>188</v>
       </c>
@@ -4553,7 +4552,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="92" spans="1:19" ht="18.75" customHeight="1">
+    <row r="92" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="56" t="s">
         <v>189</v>
       </c>
@@ -4572,7 +4571,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="93" spans="1:19" ht="18.75" customHeight="1">
+    <row r="93" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="56" t="s">
         <v>189</v>
       </c>
@@ -4591,7 +4590,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="94" spans="1:19" ht="18.75" customHeight="1">
+    <row r="94" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="56" t="s">
         <v>189</v>
       </c>
@@ -4610,8 +4609,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="95" spans="1:19" ht="15.75" customHeight="1" thickBot="1"/>
-    <row r="96" spans="1:19">
+    <row r="95" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="96" spans="1:19" x14ac:dyDescent="0.2">
       <c r="F96" s="38" t="s">
         <v>28</v>
       </c>
@@ -4649,7 +4648,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="97" spans="1:17" ht="18" customHeight="1">
+    <row r="97" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="21" t="s">
         <v>86</v>
       </c>
@@ -4690,7 +4689,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="98" spans="1:17" ht="18" customHeight="1" thickBot="1">
+    <row r="98" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A98" s="56" t="s">
         <v>27</v>
       </c>
@@ -4732,7 +4731,7 @@
       <c r="P98" s="26"/>
       <c r="Q98" s="29"/>
     </row>
-    <row r="99" spans="1:17" ht="18.75" customHeight="1">
+    <row r="99" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="56" t="s">
         <v>188</v>
       </c>
@@ -4799,7 +4798,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:17" ht="18.75" customHeight="1">
+    <row r="100" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="56" t="s">
         <v>188</v>
       </c>
@@ -4866,7 +4865,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:17" ht="18.75" customHeight="1">
+    <row r="101" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="56" t="s">
         <v>188</v>
       </c>
@@ -4933,7 +4932,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:17" ht="18.75" customHeight="1">
+    <row r="102" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="56" t="s">
         <v>189</v>
       </c>
@@ -5000,7 +4999,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:17" ht="18.75" customHeight="1">
+    <row r="103" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="56" t="s">
         <v>189</v>
       </c>
@@ -5067,7 +5066,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:17" ht="19.5" customHeight="1" thickBot="1">
+    <row r="104" spans="1:17" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="56" t="s">
         <v>189</v>
       </c>
@@ -5134,12 +5133,12 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:17" ht="18" customHeight="1">
+    <row r="106" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="21" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="107" spans="1:17">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A107" s="56" t="s">
         <v>27</v>
       </c>
@@ -5150,7 +5149,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="108" spans="1:17" ht="18.75" customHeight="1">
+    <row r="108" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="56" t="s">
         <v>188</v>
       </c>
@@ -5166,7 +5165,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="109" spans="1:17" ht="18.75" customHeight="1">
+    <row r="109" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="56" t="s">
         <v>189</v>
       </c>
@@ -5182,17 +5181,17 @@
         <v>205</v>
       </c>
     </row>
-    <row r="110" spans="1:17">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" s="56"/>
       <c r="B110" s="56"/>
     </row>
-    <row r="111" spans="1:17" ht="18" customHeight="1">
+    <row r="111" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="21" t="s">
         <v>207</v>
       </c>
       <c r="B111" s="56"/>
     </row>
-    <row r="112" spans="1:17" ht="18.75" customHeight="1">
+    <row r="112" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>209</v>
       </c>
@@ -5204,16 +5203,16 @@
         <v>205</v>
       </c>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="56"/>
       <c r="B113" s="56"/>
     </row>
-    <row r="114" spans="1:5" ht="18" customHeight="1">
+    <row r="114" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="21" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="18.75" customHeight="1">
+    <row r="115" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
         <v>210</v>
       </c>
@@ -5225,12 +5224,12 @@
         <v>205</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="18" customHeight="1">
+    <row r="117" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="52" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="18" customHeight="1">
+    <row r="118" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
         <v>212</v>
       </c>
@@ -5239,7 +5238,7 @@
         <v>0.42122127857031932</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="19.5" customHeight="1" thickBot="1">
+    <row r="120" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="52" t="s">
         <v>100</v>
       </c>
@@ -5247,7 +5246,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="18" customHeight="1">
+    <row r="121" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>213</v>
       </c>
@@ -5262,7 +5261,7 @@
         <v>7.12</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="18.75" customHeight="1">
+    <row r="122" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="11" t="s">
         <v>214</v>
       </c>
@@ -5281,7 +5280,7 @@
         <v>8.92</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="18" customHeight="1" thickBot="1">
+    <row r="123" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A123" s="11" t="s">
         <v>104</v>
       </c>
@@ -5299,7 +5298,7 @@
         <v>9.2899999999999991</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="18" customHeight="1">
+    <row r="124" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
         <v>106</v>
       </c>
@@ -5311,12 +5310,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="21" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
         <v>109</v>
       </c>
@@ -5328,7 +5327,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="11" t="s">
         <v>216</v>
       </c>
@@ -5343,24 +5342,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABE439E0-7694-4CCC-8DF2-04F46C119F4A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="8" customWidth="1"/>
-    <col min="2" max="9" width="8.85546875" style="8"/>
-    <col min="10" max="10" width="12.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.85546875" style="8"/>
+    <col min="1" max="1" width="13.1640625" style="8" customWidth="1"/>
+    <col min="2" max="9" width="8.83203125" style="8"/>
+    <col min="10" max="10" width="12.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="52" t="s">
         <v>145</v>
       </c>
@@ -5368,7 +5367,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="18" customHeight="1">
+    <row r="3" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>146</v>
       </c>
@@ -5382,7 +5381,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>109</v>
       </c>
@@ -5393,7 +5392,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>216</v>
       </c>
@@ -5401,10 +5400,10 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="11"/>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="52" t="s">
         <v>147</v>
       </c>
@@ -5418,7 +5417,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="18" customHeight="1">
+    <row r="8" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="56" t="s">
         <v>151</v>
       </c>
@@ -5456,7 +5455,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="56"/>
       <c r="B9" s="56" t="s">
         <v>107</v>
@@ -5493,7 +5492,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="56" t="s">
         <v>129</v>
       </c>
@@ -5541,7 +5540,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="56" t="s">
         <v>130</v>
       </c>
@@ -5595,7 +5594,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="56" t="s">
         <v>131</v>
       </c>
@@ -5646,7 +5645,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="56" t="s">
         <v>132</v>
       </c>
@@ -5697,7 +5696,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="M14" s="52"/>
     </row>
   </sheetData>
@@ -5707,31 +5706,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S134"/>
   <sheetViews>
-    <sheetView topLeftCell="A115" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="B134" activeCellId="2" sqref="B130 B133 B134"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" style="8" customWidth="1"/>
-    <col min="2" max="3" width="8.85546875" style="8"/>
+    <col min="2" max="3" width="8.83203125" style="8"/>
     <col min="4" max="5" width="12" style="8" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="8" customWidth="1"/>
-    <col min="8" max="9" width="11.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="11.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="8"/>
+    <col min="6" max="6" width="11.83203125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="8" customWidth="1"/>
+    <col min="8" max="9" width="11.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="11.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="I1" s="8" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="52" t="s">
         <v>0</v>
       </c>
@@ -5739,7 +5738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="18" customHeight="1">
+    <row r="3" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>176</v>
       </c>
@@ -5759,7 +5758,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="18" customHeight="1">
+    <row r="4" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>177</v>
       </c>
@@ -5776,7 +5775,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="18" customHeight="1">
+    <row r="5" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>178</v>
       </c>
@@ -5791,7 +5790,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="18" customHeight="1">
+    <row r="6" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>179</v>
       </c>
@@ -5802,7 +5801,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="18" customHeight="1">
+    <row r="7" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>180</v>
       </c>
@@ -5813,7 +5812,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -5821,7 +5820,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="18" customHeight="1">
+    <row r="9" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>181</v>
       </c>
@@ -5832,7 +5831,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="18" customHeight="1">
+    <row r="10" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>182</v>
       </c>
@@ -5843,7 +5842,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="18" customHeight="1">
+    <row r="11" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>183</v>
       </c>
@@ -5858,7 +5857,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="18">
+    <row r="12" spans="1:19" ht="17" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
@@ -5916,7 +5915,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
@@ -5931,7 +5930,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="18">
+    <row r="14" spans="1:19" ht="17" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>222</v>
       </c>
@@ -5943,7 +5942,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="18" customHeight="1">
+    <row r="15" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>184</v>
       </c>
@@ -5954,7 +5953,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="18" customHeight="1">
+    <row r="16" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>185</v>
       </c>
@@ -5966,7 +5965,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="18" customHeight="1">
+    <row r="17" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>223</v>
       </c>
@@ -5978,7 +5977,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>23</v>
       </c>
@@ -5987,7 +5986,7 @@
         <v>5.6374268708751352</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="18" customHeight="1">
+    <row r="19" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>186</v>
       </c>
@@ -5999,7 +5998,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="18" customHeight="1">
+    <row r="20" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>187</v>
       </c>
@@ -6014,15 +6013,15 @@
         <v>166</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="21" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>27</v>
       </c>
@@ -6033,7 +6032,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="18" customHeight="1">
+    <row r="24" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>188</v>
       </c>
@@ -6052,7 +6051,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="18" customHeight="1">
+    <row r="25" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>189</v>
       </c>
@@ -6068,12 +6067,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>34</v>
       </c>
@@ -6084,7 +6083,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>36</v>
       </c>
@@ -6095,7 +6094,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="18" customHeight="1">
+    <row r="30" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>37</v>
       </c>
@@ -6106,7 +6105,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>38</v>
       </c>
@@ -6118,7 +6117,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="17.25" customHeight="1">
+    <row r="32" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>39</v>
       </c>
@@ -6130,7 +6129,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>41</v>
       </c>
@@ -6142,11 +6141,11 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
+    <row r="34" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="6"/>
     </row>
-    <row r="35" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
+    <row r="35" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="21" t="s">
         <v>43</v>
       </c>
@@ -6157,7 +6156,7 @@
       <c r="G35" s="54"/>
       <c r="H35" s="55"/>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="F36" s="45" t="s">
         <v>45</v>
@@ -6184,7 +6183,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="18" customHeight="1">
+    <row r="37" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="21" t="s">
         <v>47</v>
       </c>
@@ -6213,7 +6212,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="18.75" customHeight="1" thickBot="1">
+    <row r="38" spans="1:14" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>191</v>
       </c>
@@ -6249,7 +6248,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="18" customHeight="1">
+    <row r="39" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>192</v>
       </c>
@@ -6288,7 +6287,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="18" customHeight="1">
+    <row r="40" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>193</v>
       </c>
@@ -6330,7 +6329,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="18.75" customHeight="1" thickBot="1">
+    <row r="41" spans="1:14" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E41" s="3" t="s">
         <v>58</v>
       </c>
@@ -6359,7 +6358,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="18">
+    <row r="42" spans="1:14" ht="17" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>194</v>
       </c>
@@ -6380,7 +6379,7 @@
       <c r="L42" s="56"/>
       <c r="M42" s="56"/>
     </row>
-    <row r="43" spans="1:14" ht="18">
+    <row r="43" spans="1:14" ht="17" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>195</v>
       </c>
@@ -6401,7 +6400,7 @@
       <c r="L43" s="56"/>
       <c r="M43" s="56"/>
     </row>
-    <row r="44" spans="1:14" ht="18">
+    <row r="44" spans="1:14" ht="17" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>196</v>
       </c>
@@ -6422,7 +6421,7 @@
       <c r="L44" s="56"/>
       <c r="M44" s="56"/>
     </row>
-    <row r="45" spans="1:14" ht="18">
+    <row r="45" spans="1:14" ht="17" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>197</v>
       </c>
@@ -6443,7 +6442,7 @@
       <c r="L45" s="56"/>
       <c r="M45" s="56"/>
     </row>
-    <row r="46" spans="1:14" ht="18">
+    <row r="46" spans="1:14" ht="17" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>198</v>
       </c>
@@ -6464,7 +6463,7 @@
       <c r="L46" s="56"/>
       <c r="M46" s="56"/>
     </row>
-    <row r="47" spans="1:14" ht="18">
+    <row r="47" spans="1:14" ht="17" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>199</v>
       </c>
@@ -6485,7 +6484,7 @@
       <c r="L47" s="56"/>
       <c r="M47" s="56"/>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E48" s="3"/>
       <c r="F48" s="56"/>
       <c r="G48" s="56"/>
@@ -6496,7 +6495,7 @@
       <c r="L48" s="56"/>
       <c r="M48" s="56"/>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="21" t="s">
         <v>65</v>
       </c>
@@ -6510,7 +6509,7 @@
       <c r="L49" s="56"/>
       <c r="M49" s="56"/>
     </row>
-    <row r="50" spans="1:13" ht="18" customHeight="1">
+    <row r="50" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>200</v>
       </c>
@@ -6534,7 +6533,7 @@
       <c r="L50" s="56"/>
       <c r="M50" s="56"/>
     </row>
-    <row r="51" spans="1:13" ht="18" customHeight="1">
+    <row r="51" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>201</v>
       </c>
@@ -6555,7 +6554,7 @@
       <c r="L51" s="56"/>
       <c r="M51" s="56"/>
     </row>
-    <row r="52" spans="1:13" ht="18" customHeight="1">
+    <row r="52" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>202</v>
       </c>
@@ -6576,7 +6575,7 @@
       <c r="L52" s="56"/>
       <c r="M52" s="56"/>
     </row>
-    <row r="53" spans="1:13" ht="18" customHeight="1">
+    <row r="53" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>203</v>
       </c>
@@ -6597,7 +6596,7 @@
       <c r="L53" s="56"/>
       <c r="M53" s="56"/>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="3"/>
       <c r="B54" s="7"/>
       <c r="E54" s="3"/>
@@ -6610,12 +6609,12 @@
       <c r="L54" s="56"/>
       <c r="M54" s="56"/>
     </row>
-    <row r="55" spans="1:13" ht="18" customHeight="1">
+    <row r="55" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="21" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" s="56" t="s">
         <v>27</v>
       </c>
@@ -6632,7 +6631,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="18" customHeight="1">
+    <row r="57" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="56" t="s">
         <v>188</v>
       </c>
@@ -6654,7 +6653,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="18" customHeight="1">
+    <row r="58" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="56" t="s">
         <v>188</v>
       </c>
@@ -6676,7 +6675,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="18" customHeight="1">
+    <row r="59" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="56" t="s">
         <v>188</v>
       </c>
@@ -6698,7 +6697,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="18" customHeight="1">
+    <row r="60" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="56" t="s">
         <v>188</v>
       </c>
@@ -6720,7 +6719,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="18" customHeight="1">
+    <row r="61" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="56" t="s">
         <v>188</v>
       </c>
@@ -6742,7 +6741,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="18" customHeight="1">
+    <row r="62" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="56" t="s">
         <v>188</v>
       </c>
@@ -6764,7 +6763,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="18" customHeight="1">
+    <row r="63" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="56" t="s">
         <v>189</v>
       </c>
@@ -6786,7 +6785,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="18" customHeight="1">
+    <row r="64" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="56" t="s">
         <v>189</v>
       </c>
@@ -6808,7 +6807,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="65" spans="1:18" ht="18" customHeight="1">
+    <row r="65" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="56" t="s">
         <v>189</v>
       </c>
@@ -6830,7 +6829,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="66" spans="1:18" ht="18" customHeight="1">
+    <row r="66" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="56" t="s">
         <v>189</v>
       </c>
@@ -6852,7 +6851,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="67" spans="1:18" ht="18" customHeight="1">
+    <row r="67" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="56" t="s">
         <v>189</v>
       </c>
@@ -6874,7 +6873,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="1:18" ht="18" customHeight="1">
+    <row r="68" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="56" t="s">
         <v>189</v>
       </c>
@@ -6896,12 +6895,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="71" spans="1:18" ht="18" customHeight="1">
+    <row r="71" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="52" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="72" spans="1:18">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A72" s="56" t="s">
         <v>27</v>
       </c>
@@ -6915,7 +6914,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="73" spans="1:18" ht="18" customHeight="1">
+    <row r="73" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="56" t="s">
         <v>188</v>
       </c>
@@ -6934,7 +6933,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="74" spans="1:18" ht="18" customHeight="1">
+    <row r="74" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="56" t="s">
         <v>188</v>
       </c>
@@ -6953,7 +6952,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="75" spans="1:18" ht="18" customHeight="1">
+    <row r="75" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="56" t="s">
         <v>188</v>
       </c>
@@ -6972,7 +6971,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="76" spans="1:18" ht="18" customHeight="1">
+    <row r="76" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="56" t="s">
         <v>189</v>
       </c>
@@ -6991,7 +6990,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="77" spans="1:18" ht="18" customHeight="1">
+    <row r="77" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="56" t="s">
         <v>189</v>
       </c>
@@ -7010,7 +7009,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="78" spans="1:18" ht="18" customHeight="1">
+    <row r="78" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="56" t="s">
         <v>189</v>
       </c>
@@ -7029,7 +7028,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="80" spans="1:18" ht="18" customHeight="1">
+    <row r="80" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="21" t="s">
         <v>80</v>
       </c>
@@ -7043,7 +7042,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="81" spans="1:19">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A81" s="56" t="s">
         <v>27</v>
       </c>
@@ -7093,7 +7092,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="82" spans="1:19" ht="18.75" customHeight="1">
+    <row r="82" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="56" t="s">
         <v>188</v>
       </c>
@@ -7155,7 +7154,7 @@
         <v>2.15E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:19" ht="18.75" customHeight="1">
+    <row r="83" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="56" t="s">
         <v>188</v>
       </c>
@@ -7217,7 +7216,7 @@
         <v>1.98E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:19" ht="18.75" customHeight="1">
+    <row r="84" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="56" t="s">
         <v>188</v>
       </c>
@@ -7279,7 +7278,7 @@
         <v>1.98E-3</v>
       </c>
     </row>
-    <row r="85" spans="1:19" ht="18.75" customHeight="1">
+    <row r="85" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="56" t="s">
         <v>189</v>
       </c>
@@ -7341,7 +7340,7 @@
         <v>1.98E-3</v>
       </c>
     </row>
-    <row r="86" spans="1:19" ht="18.75" customHeight="1">
+    <row r="86" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="56" t="s">
         <v>189</v>
       </c>
@@ -7403,7 +7402,7 @@
         <v>1.98E-3</v>
       </c>
     </row>
-    <row r="87" spans="1:19" ht="18.75" customHeight="1">
+    <row r="87" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="56" t="s">
         <v>189</v>
       </c>
@@ -7465,12 +7464,12 @@
         <v>1.98E-3</v>
       </c>
     </row>
-    <row r="89" spans="1:19" ht="18" customHeight="1">
+    <row r="89" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="21" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="90" spans="1:19">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A90" s="56" t="s">
         <v>27</v>
       </c>
@@ -7484,7 +7483,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="91" spans="1:19" ht="18.75" customHeight="1">
+    <row r="91" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="56" t="s">
         <v>188</v>
       </c>
@@ -7503,7 +7502,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="92" spans="1:19" ht="18.75" customHeight="1">
+    <row r="92" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="56" t="s">
         <v>188</v>
       </c>
@@ -7522,7 +7521,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="93" spans="1:19" ht="18.75" customHeight="1">
+    <row r="93" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="56" t="s">
         <v>188</v>
       </c>
@@ -7541,7 +7540,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="94" spans="1:19" ht="18.75" customHeight="1">
+    <row r="94" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="56" t="s">
         <v>189</v>
       </c>
@@ -7560,7 +7559,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="95" spans="1:19" ht="18.75" customHeight="1">
+    <row r="95" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="56" t="s">
         <v>189</v>
       </c>
@@ -7579,7 +7578,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="96" spans="1:19" ht="18.75" customHeight="1">
+    <row r="96" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="56" t="s">
         <v>189</v>
       </c>
@@ -7598,13 +7597,13 @@
         <v>205</v>
       </c>
     </row>
-    <row r="97" spans="1:17" ht="18.75" customHeight="1">
+    <row r="97" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="56"/>
       <c r="B97" s="56"/>
       <c r="C97" s="7"/>
       <c r="D97" s="7"/>
     </row>
-    <row r="98" spans="1:17" ht="18.75" customHeight="1">
+    <row r="98" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="21" t="s">
         <v>224</v>
       </c>
@@ -7612,7 +7611,7 @@
       <c r="C98" s="7"/>
       <c r="D98" s="7"/>
     </row>
-    <row r="99" spans="1:17" ht="18.75" customHeight="1">
+    <row r="99" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="56"/>
       <c r="B99" s="56" t="s">
         <v>28</v>
@@ -7622,7 +7621,7 @@
       </c>
       <c r="D99" s="7"/>
     </row>
-    <row r="100" spans="1:17" ht="18.75" customHeight="1">
+    <row r="100" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="56" t="s">
         <v>30</v>
       </c>
@@ -7636,7 +7635,7 @@
       </c>
       <c r="D100" s="7"/>
     </row>
-    <row r="101" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
+    <row r="101" spans="1:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="56" t="s">
         <v>32</v>
       </c>
@@ -7649,7 +7648,7 @@
         <v>46648</v>
       </c>
     </row>
-    <row r="102" spans="1:17">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.2">
       <c r="F102" s="38" t="s">
         <v>28</v>
       </c>
@@ -7687,7 +7686,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="103" spans="1:17" ht="18" customHeight="1">
+    <row r="103" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="21" t="s">
         <v>86</v>
       </c>
@@ -7728,7 +7727,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="104" spans="1:17" ht="18" customHeight="1" thickBot="1">
+    <row r="104" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="56" t="s">
         <v>27</v>
       </c>
@@ -7770,7 +7769,7 @@
       <c r="P104" s="26"/>
       <c r="Q104" s="29"/>
     </row>
-    <row r="105" spans="1:17" ht="18.75" customHeight="1">
+    <row r="105" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="56" t="s">
         <v>188</v>
       </c>
@@ -7837,7 +7836,7 @@
         <v>2.58E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:17" ht="18.75" customHeight="1">
+    <row r="106" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="56" t="s">
         <v>188</v>
       </c>
@@ -7904,7 +7903,7 @@
         <v>2.3760000000000007E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:17" ht="18.75" customHeight="1">
+    <row r="107" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="56" t="s">
         <v>188</v>
       </c>
@@ -7971,7 +7970,7 @@
         <v>2.3760000000000007E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:17" ht="18.75" customHeight="1">
+    <row r="108" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="56" t="s">
         <v>189</v>
       </c>
@@ -8038,7 +8037,7 @@
         <v>2.3760000000000007E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:17" ht="18.75" customHeight="1">
+    <row r="109" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="56" t="s">
         <v>189</v>
       </c>
@@ -8105,7 +8104,7 @@
         <v>2.3760000000000007E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:17" ht="19.5" customHeight="1" thickBot="1">
+    <row r="110" spans="1:17" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="56" t="s">
         <v>189</v>
       </c>
@@ -8172,12 +8171,12 @@
         <v>2.3760000000000007E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:17" ht="18" customHeight="1">
+    <row r="112" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="21" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="56" t="s">
         <v>27</v>
       </c>
@@ -8188,7 +8187,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="18.75" customHeight="1">
+    <row r="114" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="56" t="s">
         <v>188</v>
       </c>
@@ -8204,7 +8203,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="18.75" customHeight="1">
+    <row r="115" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="56" t="s">
         <v>189</v>
       </c>
@@ -8220,17 +8219,17 @@
         <v>205</v>
       </c>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="56"/>
       <c r="B116" s="56"/>
     </row>
-    <row r="117" spans="1:5" ht="18" customHeight="1">
+    <row r="117" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="21" t="s">
         <v>207</v>
       </c>
       <c r="B117" s="56"/>
     </row>
-    <row r="118" spans="1:5" ht="18.75" customHeight="1">
+    <row r="118" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
         <v>209</v>
       </c>
@@ -8242,16 +8241,16 @@
         <v>205</v>
       </c>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="56"/>
       <c r="B119" s="56"/>
     </row>
-    <row r="120" spans="1:5" ht="18" customHeight="1">
+    <row r="120" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="21" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="18.75" customHeight="1">
+    <row r="121" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>210</v>
       </c>
@@ -8263,12 +8262,12 @@
         <v>205</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="18" customHeight="1">
+    <row r="123" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="52" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="18" customHeight="1">
+    <row r="124" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>212</v>
       </c>
@@ -8277,7 +8276,7 @@
         <v>0.42862495861865535</v>
       </c>
     </row>
-    <row r="126" spans="1:5" ht="19.5" customHeight="1" thickBot="1">
+    <row r="126" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="52" t="s">
         <v>100</v>
       </c>
@@ -8285,7 +8284,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="127" spans="1:5" ht="18" customHeight="1">
+    <row r="127" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
         <v>213</v>
       </c>
@@ -8300,7 +8299,7 @@
         <v>7.12</v>
       </c>
     </row>
-    <row r="128" spans="1:5" ht="18.75" customHeight="1">
+    <row r="128" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="11" t="s">
         <v>214</v>
       </c>
@@ -8319,7 +8318,7 @@
         <v>8.92</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="18" customHeight="1" thickBot="1">
+    <row r="129" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A129" s="11" t="s">
         <v>104</v>
       </c>
@@ -8337,7 +8336,7 @@
         <v>9.2899999999999991</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="18" customHeight="1">
+    <row r="130" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
         <v>106</v>
       </c>
@@ -8349,12 +8348,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="21" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="133" spans="1:5">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
         <v>109</v>
       </c>
@@ -8366,7 +8365,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="134" spans="1:5">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" s="11" t="s">
         <v>216</v>
       </c>
@@ -8381,22 +8380,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="8" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" style="8" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="52" t="s">
         <v>145</v>
       </c>
@@ -8404,10 +8403,10 @@
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="1:15" ht="18" customHeight="1">
+    <row r="3" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>146</v>
       </c>
@@ -8421,7 +8420,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>109</v>
       </c>
@@ -8433,7 +8432,7 @@
       </c>
       <c r="I4" s="8"/>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>216</v>
       </c>
@@ -8441,10 +8440,10 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="11"/>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="52" t="s">
         <v>147</v>
       </c>
@@ -8459,7 +8458,7 @@
       </c>
       <c r="M7" s="8"/>
     </row>
-    <row r="8" spans="1:15" ht="18" customHeight="1">
+    <row r="8" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="56" t="s">
         <v>151</v>
       </c>
@@ -8498,7 +8497,7 @@
       </c>
       <c r="M8" s="8"/>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="56"/>
       <c r="B9" s="56" t="s">
         <v>107</v>
@@ -8535,7 +8534,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="56" t="s">
         <v>129</v>
       </c>
@@ -8583,7 +8582,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="56" t="s">
         <v>130</v>
       </c>
@@ -8637,7 +8636,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="56" t="s">
         <v>131</v>
       </c>
@@ -8688,7 +8687,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="56" t="s">
         <v>132</v>
       </c>
@@ -8739,7 +8738,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="M14" s="52"/>
     </row>
   </sheetData>
@@ -8749,35 +8748,35 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.83203125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="18" customHeight="1">
+    <row r="1" spans="1:35" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="56" t="s">
         <v>112</v>
       </c>
@@ -8881,7 +8880,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="18" customHeight="1">
+    <row r="2" spans="1:35" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>133</v>
       </c>
@@ -8986,7 +8985,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A3"/>
       <c r="B3" s="59"/>
       <c r="C3" s="59"/>
@@ -9020,7 +9019,7 @@
       <c r="AH3" s="56"/>
       <c r="AI3" s="56"/>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A4"/>
       <c r="B4" s="59"/>
       <c r="C4" s="59"/>
@@ -9054,7 +9053,7 @@
       <c r="AH4" s="56"/>
       <c r="AI4" s="56"/>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5"/>
       <c r="B5" s="59"/>
       <c r="C5" s="59"/>
@@ -9088,7 +9087,7 @@
       <c r="AH5" s="56"/>
       <c r="AI5" s="56"/>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A6"/>
       <c r="B6" s="59"/>
       <c r="C6" s="59"/>
@@ -9122,7 +9121,7 @@
       <c r="AH6" s="56"/>
       <c r="AI6" s="56"/>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A7"/>
       <c r="B7" s="59"/>
       <c r="C7" s="59"/>
@@ -9156,7 +9155,7 @@
       <c r="AH7" s="56"/>
       <c r="AI7" s="56"/>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A8"/>
       <c r="B8" s="59"/>
       <c r="C8" s="59"/>
@@ -9190,7 +9189,7 @@
       <c r="AH8" s="56"/>
       <c r="AI8" s="56"/>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A9"/>
       <c r="B9" s="59"/>
       <c r="C9" s="59"/>
@@ -9224,7 +9223,7 @@
       <c r="AH9" s="56"/>
       <c r="AI9" s="56"/>
     </row>
-    <row r="10" spans="1:35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A10"/>
       <c r="B10" s="59"/>
       <c r="C10" s="59"/>
@@ -9258,7 +9257,7 @@
       <c r="AH10" s="56"/>
       <c r="AI10" s="56"/>
     </row>
-    <row r="11" spans="1:35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A11"/>
       <c r="B11" s="59"/>
       <c r="C11" s="59"/>
@@ -9292,7 +9291,7 @@
       <c r="AH11" s="56"/>
       <c r="AI11" s="56"/>
     </row>
-    <row r="12" spans="1:35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A12"/>
       <c r="B12" s="59"/>
       <c r="C12" s="59"/>
@@ -9326,7 +9325,7 @@
       <c r="AH12" s="56"/>
       <c r="AI12" s="56"/>
     </row>
-    <row r="13" spans="1:35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A13"/>
       <c r="B13" s="59"/>
       <c r="C13" s="59"/>
@@ -9360,7 +9359,7 @@
       <c r="AH13" s="56"/>
       <c r="AI13" s="56"/>
     </row>
-    <row r="14" spans="1:35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A14"/>
       <c r="B14" s="59"/>
       <c r="C14" s="59"/>
@@ -9394,7 +9393,7 @@
       <c r="AH14" s="56"/>
       <c r="AI14" s="56"/>
     </row>
-    <row r="15" spans="1:35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A15"/>
       <c r="B15" s="59"/>
       <c r="C15" s="59"/>
@@ -9428,7 +9427,7 @@
       <c r="AH15" s="56"/>
       <c r="AI15" s="56"/>
     </row>
-    <row r="16" spans="1:35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A16"/>
       <c r="B16" s="59"/>
       <c r="C16" s="59"/>
@@ -9462,7 +9461,7 @@
       <c r="AH16" s="56"/>
       <c r="AI16" s="56"/>
     </row>
-    <row r="17" spans="1:35">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A17"/>
       <c r="B17" s="59"/>
       <c r="C17" s="59"/>
@@ -9496,7 +9495,7 @@
       <c r="AH17" s="56"/>
       <c r="AI17" s="56"/>
     </row>
-    <row r="18" spans="1:35">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A18"/>
       <c r="B18" s="59"/>
       <c r="C18" s="59"/>
@@ -9530,7 +9529,7 @@
       <c r="AH18" s="56"/>
       <c r="AI18" s="56"/>
     </row>
-    <row r="19" spans="1:35">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A19"/>
       <c r="B19" s="59"/>
       <c r="C19" s="59"/>
@@ -9564,7 +9563,7 @@
       <c r="AH19" s="56"/>
       <c r="AI19" s="56"/>
     </row>
-    <row r="20" spans="1:35">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A20"/>
       <c r="B20" s="59"/>
       <c r="C20" s="59"/>
@@ -9598,7 +9597,7 @@
       <c r="AH20" s="56"/>
       <c r="AI20" s="56"/>
     </row>
-    <row r="21" spans="1:35">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A21"/>
       <c r="B21" s="59"/>
       <c r="C21" s="59"/>
@@ -9632,7 +9631,7 @@
       <c r="AH21" s="56"/>
       <c r="AI21" s="56"/>
     </row>
-    <row r="22" spans="1:35">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A22"/>
       <c r="B22" s="59"/>
       <c r="C22" s="59"/>
@@ -9666,7 +9665,7 @@
       <c r="AH22" s="56"/>
       <c r="AI22" s="56"/>
     </row>
-    <row r="23" spans="1:35">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A23"/>
       <c r="B23" s="59"/>
       <c r="C23" s="59"/>
@@ -9700,7 +9699,7 @@
       <c r="AH23" s="56"/>
       <c r="AI23" s="56"/>
     </row>
-    <row r="24" spans="1:35">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A24"/>
       <c r="B24" s="59"/>
       <c r="C24" s="59"/>
@@ -9734,7 +9733,7 @@
       <c r="AH24" s="56"/>
       <c r="AI24" s="56"/>
     </row>
-    <row r="25" spans="1:35">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A25"/>
       <c r="B25" s="59"/>
       <c r="C25" s="59"/>
@@ -9768,7 +9767,7 @@
       <c r="AH25" s="56"/>
       <c r="AI25" s="56"/>
     </row>
-    <row r="26" spans="1:35">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A26"/>
       <c r="B26" s="59"/>
       <c r="C26" s="59"/>
@@ -9802,7 +9801,7 @@
       <c r="AH26" s="56"/>
       <c r="AI26" s="56"/>
     </row>
-    <row r="27" spans="1:35">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A27"/>
       <c r="B27" s="59"/>
       <c r="C27" s="59"/>
@@ -9836,7 +9835,7 @@
       <c r="AH27" s="56"/>
       <c r="AI27" s="56"/>
     </row>
-    <row r="28" spans="1:35">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A28"/>
       <c r="B28" s="59"/>
       <c r="C28" s="59"/>
@@ -9870,7 +9869,7 @@
       <c r="AH28" s="56"/>
       <c r="AI28" s="56"/>
     </row>
-    <row r="29" spans="1:35">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A29"/>
       <c r="B29" s="59"/>
       <c r="C29" s="59"/>
@@ -9904,7 +9903,7 @@
       <c r="AH29" s="56"/>
       <c r="AI29" s="56"/>
     </row>
-    <row r="30" spans="1:35">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A30"/>
       <c r="B30" s="59"/>
       <c r="C30" s="59"/>
@@ -9938,7 +9937,7 @@
       <c r="AH30" s="56"/>
       <c r="AI30" s="56"/>
     </row>
-    <row r="31" spans="1:35">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A31"/>
       <c r="B31" s="59"/>
       <c r="C31" s="59"/>
@@ -9972,7 +9971,7 @@
       <c r="AH31" s="56"/>
       <c r="AI31" s="56"/>
     </row>
-    <row r="32" spans="1:35">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A32"/>
       <c r="B32" s="59"/>
       <c r="C32" s="59"/>
@@ -10006,7 +10005,7 @@
       <c r="AH32" s="56"/>
       <c r="AI32" s="56"/>
     </row>
-    <row r="33" spans="1:35">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A33"/>
       <c r="B33" s="59"/>
       <c r="C33" s="59"/>
@@ -10040,7 +10039,7 @@
       <c r="AH33" s="56"/>
       <c r="AI33" s="56"/>
     </row>
-    <row r="34" spans="1:35">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A34"/>
       <c r="B34" s="59"/>
       <c r="C34" s="59"/>
@@ -10074,7 +10073,7 @@
       <c r="AH34" s="56"/>
       <c r="AI34" s="56"/>
     </row>
-    <row r="35" spans="1:35">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A35"/>
       <c r="B35" s="59"/>
       <c r="C35" s="59"/>
@@ -10108,7 +10107,7 @@
       <c r="AH35" s="56"/>
       <c r="AI35" s="56"/>
     </row>
-    <row r="36" spans="1:35">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A36"/>
       <c r="B36" s="59"/>
       <c r="C36" s="59"/>
@@ -10142,7 +10141,7 @@
       <c r="AH36" s="56"/>
       <c r="AI36" s="56"/>
     </row>
-    <row r="37" spans="1:35">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A37"/>
       <c r="B37" s="59"/>
       <c r="C37" s="59"/>
@@ -10176,7 +10175,7 @@
       <c r="AH37" s="56"/>
       <c r="AI37" s="56"/>
     </row>
-    <row r="38" spans="1:35">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A38"/>
       <c r="B38" s="59"/>
       <c r="C38" s="59"/>
@@ -10210,7 +10209,7 @@
       <c r="AH38" s="56"/>
       <c r="AI38" s="56"/>
     </row>
-    <row r="39" spans="1:35">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A39"/>
       <c r="B39" s="59"/>
       <c r="C39" s="59"/>
@@ -10244,7 +10243,7 @@
       <c r="AH39" s="56"/>
       <c r="AI39" s="56"/>
     </row>
-    <row r="40" spans="1:35">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A40"/>
       <c r="B40" s="59"/>
       <c r="C40" s="59"/>
@@ -10278,7 +10277,7 @@
       <c r="AH40" s="56"/>
       <c r="AI40" s="56"/>
     </row>
-    <row r="41" spans="1:35">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A41"/>
       <c r="B41" s="59"/>
       <c r="C41" s="59"/>
@@ -10312,7 +10311,7 @@
       <c r="AH41" s="56"/>
       <c r="AI41" s="56"/>
     </row>
-    <row r="42" spans="1:35">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A42"/>
       <c r="B42" s="59"/>
       <c r="C42" s="59"/>
@@ -10358,25 +10357,25 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q128"/>
   <sheetViews>
     <sheetView topLeftCell="A100" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="O126" sqref="O126"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" style="8" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="8" customWidth="1"/>
     <col min="5" max="5" width="12" style="8" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="8" customWidth="1"/>
-    <col min="8" max="9" width="11.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="11.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="8" customWidth="1"/>
+    <col min="8" max="9" width="11.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="11.5" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="52" t="s">
         <v>0</v>
       </c>
@@ -10384,7 +10383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18" customHeight="1">
+    <row r="3" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -10401,7 +10400,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18" customHeight="1">
+    <row r="4" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -10415,7 +10414,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18" customHeight="1">
+    <row r="5" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -10427,7 +10426,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1">
+    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -10438,7 +10437,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1">
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
@@ -10449,7 +10448,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -10457,7 +10456,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
@@ -10468,7 +10467,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="18" customHeight="1">
+    <row r="10" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
@@ -10479,7 +10478,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="18" customHeight="1">
+    <row r="11" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
@@ -10494,7 +10493,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
@@ -10505,7 +10504,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
@@ -10516,7 +10515,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="18" customHeight="1">
+    <row r="14" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
@@ -10527,7 +10526,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="18" customHeight="1">
+    <row r="15" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
@@ -10539,7 +10538,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
@@ -10548,7 +10547,7 @@
         <v>5.9315173688353893</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="18" customHeight="1">
+    <row r="17" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>24</v>
       </c>
@@ -10557,7 +10556,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="18" customHeight="1">
+    <row r="18" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>25</v>
       </c>
@@ -10569,15 +10568,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="21" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>27</v>
       </c>
@@ -10588,7 +10587,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="18" customHeight="1">
+    <row r="22" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>30</v>
       </c>
@@ -10607,7 +10606,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="18" customHeight="1">
+    <row r="23" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>32</v>
       </c>
@@ -10623,12 +10622,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>34</v>
       </c>
@@ -10639,7 +10638,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>36</v>
       </c>
@@ -10650,7 +10649,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="18" customHeight="1">
+    <row r="28" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>37</v>
       </c>
@@ -10661,7 +10660,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>38</v>
       </c>
@@ -10673,7 +10672,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="17.25" customHeight="1">
+    <row r="30" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>39</v>
       </c>
@@ -10685,7 +10684,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>41</v>
       </c>
@@ -10697,11 +10696,11 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="6"/>
     </row>
-    <row r="33" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
+    <row r="33" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
         <v>43</v>
       </c>
@@ -10712,7 +10711,7 @@
       <c r="G33" s="54"/>
       <c r="H33" s="55"/>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="F34" s="45" t="s">
         <v>45</v>
@@ -10739,7 +10738,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="18" customHeight="1">
+    <row r="35" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="21" t="s">
         <v>47</v>
       </c>
@@ -10768,7 +10767,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="18.75" customHeight="1" thickBot="1">
+    <row r="36" spans="1:14" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>48</v>
       </c>
@@ -10804,7 +10803,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="18" customHeight="1">
+    <row r="37" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>52</v>
       </c>
@@ -10843,7 +10842,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="18" customHeight="1">
+    <row r="38" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>55</v>
       </c>
@@ -10885,7 +10884,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="18.75" customHeight="1" thickBot="1">
+    <row r="39" spans="1:14" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E39" s="3" t="s">
         <v>58</v>
       </c>
@@ -10914,7 +10913,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>59</v>
       </c>
@@ -10935,7 +10934,7 @@
       <c r="L40" s="56"/>
       <c r="M40" s="56"/>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>60</v>
       </c>
@@ -10956,7 +10955,7 @@
       <c r="L41" s="56"/>
       <c r="M41" s="56"/>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>61</v>
       </c>
@@ -10977,7 +10976,7 @@
       <c r="L42" s="56"/>
       <c r="M42" s="56"/>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>62</v>
       </c>
@@ -10998,7 +10997,7 @@
       <c r="L43" s="56"/>
       <c r="M43" s="56"/>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>63</v>
       </c>
@@ -11019,7 +11018,7 @@
       <c r="L44" s="56"/>
       <c r="M44" s="56"/>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>64</v>
       </c>
@@ -11040,7 +11039,7 @@
       <c r="L45" s="56"/>
       <c r="M45" s="56"/>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E46" s="3"/>
       <c r="F46" s="56"/>
       <c r="G46" s="56"/>
@@ -11051,7 +11050,7 @@
       <c r="L46" s="56"/>
       <c r="M46" s="56"/>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="21" t="s">
         <v>65</v>
       </c>
@@ -11065,7 +11064,7 @@
       <c r="L47" s="56"/>
       <c r="M47" s="56"/>
     </row>
-    <row r="48" spans="1:14" ht="18" customHeight="1">
+    <row r="48" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>66</v>
       </c>
@@ -11086,7 +11085,7 @@
       <c r="L48" s="56"/>
       <c r="M48" s="56"/>
     </row>
-    <row r="49" spans="1:13" ht="18" customHeight="1">
+    <row r="49" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>68</v>
       </c>
@@ -11107,7 +11106,7 @@
       <c r="L49" s="56"/>
       <c r="M49" s="56"/>
     </row>
-    <row r="50" spans="1:13" ht="18" customHeight="1">
+    <row r="50" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>69</v>
       </c>
@@ -11128,7 +11127,7 @@
       <c r="L50" s="56"/>
       <c r="M50" s="56"/>
     </row>
-    <row r="51" spans="1:13" ht="18" customHeight="1">
+    <row r="51" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>70</v>
       </c>
@@ -11149,7 +11148,7 @@
       <c r="L51" s="56"/>
       <c r="M51" s="56"/>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="3"/>
       <c r="B52" s="7"/>
       <c r="E52" s="3"/>
@@ -11162,12 +11161,12 @@
       <c r="L52" s="56"/>
       <c r="M52" s="56"/>
     </row>
-    <row r="53" spans="1:13" ht="18" customHeight="1">
+    <row r="53" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="21" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="56" t="s">
         <v>27</v>
       </c>
@@ -11184,7 +11183,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="18" customHeight="1">
+    <row r="55" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="56" t="s">
         <v>30</v>
       </c>
@@ -11206,7 +11205,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="18" customHeight="1">
+    <row r="56" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="56" t="s">
         <v>30</v>
       </c>
@@ -11228,7 +11227,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="18" customHeight="1">
+    <row r="57" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="56" t="s">
         <v>30</v>
       </c>
@@ -11250,7 +11249,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="18" customHeight="1">
+    <row r="58" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="56" t="s">
         <v>30</v>
       </c>
@@ -11272,7 +11271,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="18" customHeight="1">
+    <row r="59" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="56" t="s">
         <v>30</v>
       </c>
@@ -11294,7 +11293,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="18" customHeight="1">
+    <row r="60" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="56" t="s">
         <v>30</v>
       </c>
@@ -11316,7 +11315,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="18" customHeight="1">
+    <row r="61" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="56" t="s">
         <v>32</v>
       </c>
@@ -11338,7 +11337,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="18" customHeight="1">
+    <row r="62" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="56" t="s">
         <v>32</v>
       </c>
@@ -11360,7 +11359,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="18" customHeight="1">
+    <row r="63" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="56" t="s">
         <v>32</v>
       </c>
@@ -11382,7 +11381,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="18" customHeight="1">
+    <row r="64" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="56" t="s">
         <v>32</v>
       </c>
@@ -11404,7 +11403,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="18" customHeight="1">
+    <row r="65" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="56" t="s">
         <v>32</v>
       </c>
@@ -11426,7 +11425,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="18" customHeight="1">
+    <row r="66" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="56" t="s">
         <v>32</v>
       </c>
@@ -11448,12 +11447,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="18" customHeight="1">
+    <row r="69" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="52" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="70" spans="1:12">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" s="56" t="s">
         <v>27</v>
       </c>
@@ -11467,7 +11466,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="18" customHeight="1">
+    <row r="71" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="56" t="s">
         <v>30</v>
       </c>
@@ -11486,7 +11485,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="18" customHeight="1">
+    <row r="72" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="56" t="s">
         <v>30</v>
       </c>
@@ -11505,7 +11504,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="18" customHeight="1">
+    <row r="73" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="56" t="s">
         <v>30</v>
       </c>
@@ -11524,7 +11523,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="18" customHeight="1">
+    <row r="74" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="56" t="s">
         <v>32</v>
       </c>
@@ -11543,7 +11542,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="18" customHeight="1">
+    <row r="75" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="56" t="s">
         <v>32</v>
       </c>
@@ -11562,7 +11561,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="18" customHeight="1">
+    <row r="76" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="56" t="s">
         <v>32</v>
       </c>
@@ -11581,7 +11580,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="18" customHeight="1">
+    <row r="78" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="21" t="s">
         <v>80</v>
       </c>
@@ -11589,7 +11588,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="79" spans="1:12">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" s="56" t="s">
         <v>27</v>
       </c>
@@ -11618,7 +11617,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="18.75" customHeight="1">
+    <row r="80" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="56" t="s">
         <v>30</v>
       </c>
@@ -11656,7 +11655,7 @@
       <c r="K80" s="9"/>
       <c r="L80" s="9"/>
     </row>
-    <row r="81" spans="1:17" ht="18.75" customHeight="1">
+    <row r="81" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="56" t="s">
         <v>30</v>
       </c>
@@ -11694,7 +11693,7 @@
       <c r="K81" s="9"/>
       <c r="L81" s="9"/>
     </row>
-    <row r="82" spans="1:17" ht="18.75" customHeight="1">
+    <row r="82" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="56" t="s">
         <v>30</v>
       </c>
@@ -11732,7 +11731,7 @@
       <c r="K82" s="9"/>
       <c r="L82" s="9"/>
     </row>
-    <row r="83" spans="1:17" ht="18.75" customHeight="1">
+    <row r="83" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="56" t="s">
         <v>32</v>
       </c>
@@ -11770,7 +11769,7 @@
       <c r="K83" s="9"/>
       <c r="L83" s="9"/>
     </row>
-    <row r="84" spans="1:17" ht="18.75" customHeight="1">
+    <row r="84" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="56" t="s">
         <v>32</v>
       </c>
@@ -11808,7 +11807,7 @@
       <c r="K84" s="9"/>
       <c r="L84" s="9"/>
     </row>
-    <row r="85" spans="1:17" ht="18.75" customHeight="1">
+    <row r="85" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="56" t="s">
         <v>32</v>
       </c>
@@ -11846,12 +11845,12 @@
       <c r="K85" s="9"/>
       <c r="L85" s="9"/>
     </row>
-    <row r="87" spans="1:17" ht="18" customHeight="1">
+    <row r="87" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="21" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="88" spans="1:17">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A88" s="56" t="s">
         <v>27</v>
       </c>
@@ -11865,7 +11864,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="89" spans="1:17" ht="18.75" customHeight="1">
+    <row r="89" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="56" t="s">
         <v>30</v>
       </c>
@@ -11884,7 +11883,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="90" spans="1:17" ht="18.75" customHeight="1">
+    <row r="90" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="56" t="s">
         <v>30</v>
       </c>
@@ -11903,7 +11902,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="91" spans="1:17" ht="18.75" customHeight="1">
+    <row r="91" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="56" t="s">
         <v>30</v>
       </c>
@@ -11922,7 +11921,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="92" spans="1:17" ht="18.75" customHeight="1">
+    <row r="92" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="56" t="s">
         <v>32</v>
       </c>
@@ -11941,7 +11940,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="93" spans="1:17" ht="18.75" customHeight="1">
+    <row r="93" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="56" t="s">
         <v>32</v>
       </c>
@@ -11960,7 +11959,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="94" spans="1:17" ht="18.75" customHeight="1">
+    <row r="94" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="56" t="s">
         <v>32</v>
       </c>
@@ -11979,8 +11978,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="95" spans="1:17" ht="15.75" customHeight="1" thickBot="1"/>
-    <row r="96" spans="1:17">
+    <row r="95" spans="1:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.2">
       <c r="F96" s="38" t="s">
         <v>28</v>
       </c>
@@ -12018,7 +12017,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="97" spans="1:17" ht="18" customHeight="1">
+    <row r="97" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="21" t="s">
         <v>86</v>
       </c>
@@ -12059,7 +12058,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="98" spans="1:17" ht="18" customHeight="1" thickBot="1">
+    <row r="98" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A98" s="56" t="s">
         <v>27</v>
       </c>
@@ -12101,7 +12100,7 @@
       <c r="P98" s="26"/>
       <c r="Q98" s="29"/>
     </row>
-    <row r="99" spans="1:17" ht="18.75" customHeight="1">
+    <row r="99" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="56" t="s">
         <v>30</v>
       </c>
@@ -12168,7 +12167,7 @@
         <v>4.3944649990503321E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:17" ht="18.75" customHeight="1">
+    <row r="100" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="56" t="s">
         <v>30</v>
       </c>
@@ -12235,7 +12234,7 @@
         <v>3.0000000000000002E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:17" ht="18.75" customHeight="1">
+    <row r="101" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="56" t="s">
         <v>30</v>
       </c>
@@ -12302,7 +12301,7 @@
         <v>3.5704726064266931E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:17" ht="18.75" customHeight="1">
+    <row r="102" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="56" t="s">
         <v>32</v>
       </c>
@@ -12369,7 +12368,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="103" spans="1:17" ht="18.75" customHeight="1">
+    <row r="103" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="56" t="s">
         <v>32</v>
       </c>
@@ -12436,7 +12435,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="104" spans="1:17" ht="19.5" customHeight="1" thickBot="1">
+    <row r="104" spans="1:17" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="56" t="s">
         <v>32</v>
       </c>
@@ -12503,12 +12502,12 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="106" spans="1:17" ht="18" customHeight="1">
+    <row r="106" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="21" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="107" spans="1:17">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A107" s="56" t="s">
         <v>27</v>
       </c>
@@ -12519,7 +12518,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="108" spans="1:17" ht="18.75" customHeight="1">
+    <row r="108" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="56" t="s">
         <v>30</v>
       </c>
@@ -12535,7 +12534,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="109" spans="1:17" ht="18.75" customHeight="1">
+    <row r="109" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="56" t="s">
         <v>32</v>
       </c>
@@ -12551,17 +12550,17 @@
         <v>85</v>
       </c>
     </row>
-    <row r="110" spans="1:17">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" s="56"/>
       <c r="B110" s="56"/>
     </row>
-    <row r="111" spans="1:17" ht="18" customHeight="1">
+    <row r="111" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="21" t="s">
         <v>94</v>
       </c>
       <c r="B111" s="56"/>
     </row>
-    <row r="112" spans="1:17" ht="18.75" customHeight="1">
+    <row r="112" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>95</v>
       </c>
@@ -12573,16 +12572,16 @@
         <v>85</v>
       </c>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="56"/>
       <c r="B113" s="56"/>
     </row>
-    <row r="114" spans="1:5" ht="18" customHeight="1">
+    <row r="114" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="21" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="18.75" customHeight="1">
+    <row r="115" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>97</v>
       </c>
@@ -12594,12 +12593,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="18" customHeight="1">
+    <row r="117" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="52" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="18" customHeight="1">
+    <row r="118" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
         <v>99</v>
       </c>
@@ -12608,7 +12607,7 @@
         <v>0.54614289068960964</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="19.5" customHeight="1" thickBot="1">
+    <row r="120" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A120" s="52" t="s">
         <v>100</v>
       </c>
@@ -12616,7 +12615,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="18" customHeight="1">
+    <row r="121" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
         <v>102</v>
       </c>
@@ -12631,7 +12630,7 @@
         <v>7.12</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="18.75" customHeight="1">
+    <row r="122" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="11" t="s">
         <v>103</v>
       </c>
@@ -12650,7 +12649,7 @@
         <v>8.92</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="18" customHeight="1" thickBot="1">
+    <row r="123" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A123" s="11" t="s">
         <v>104</v>
       </c>
@@ -12668,7 +12667,7 @@
         <v>9.2899999999999991</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="18" customHeight="1">
+    <row r="124" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
         <v>106</v>
       </c>
@@ -12680,12 +12679,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="21" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
         <v>109</v>
       </c>
@@ -12697,7 +12696,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="11" t="s">
         <v>111</v>
       </c>

</xml_diff>